<commit_message>
change schedule to use sub
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13900" yWindow="0" windowWidth="11700" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>date</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Wk</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
   </si>
   <si>
     <t>eval</t>
-  </si>
-  <si>
-    <t>Introduction to class logistics</t>
   </si>
   <si>
     <t>How to submit homework 
@@ -74,34 +68,16 @@
     <t>Logistics, Programs, Accounts, Metacognition, Intro to Data Camp and R</t>
   </si>
   <si>
-    <t>Read the [Syllabus]()
-* Install Suite of Programs [Instruction Slides]()
-* Make a Data Camp account (use link in email)</t>
-  </si>
-  <si>
     <t>Data Camp - Intro to R (entire module) 
 * [Metacognition pre-assessment]()</t>
   </si>
   <si>
-    <t>* HW 1</t>
-  </si>
-  <si>
-    <t>* Download the [HW 1 Template]()
-* Install the `rmarkdown` package</t>
-  </si>
-  <si>
     <t>How data is stored</t>
   </si>
   <si>
-    <t>Calculating summary statistics</t>
-  </si>
-  <si>
     <t>data basics, struture</t>
   </si>
   <si>
-    <t>summary stats</t>
-  </si>
-  <si>
     <t>Choose a data set to explore</t>
   </si>
   <si>
@@ -151,9 +127,6 @@
   </si>
   <si>
     <t>experimental design</t>
-  </si>
-  <si>
-    <t>univariate graphics (need 1 week?)</t>
   </si>
   <si>
     <t>Exam 2</t>
@@ -219,6 +192,65 @@
   </si>
   <si>
     <t xml:space="preserve">lit review, using passion driven stats. How to teach this? </t>
+  </si>
+  <si>
+    <t>univariate numerical</t>
+  </si>
+  <si>
+    <t>univariate categorical</t>
+  </si>
+  <si>
+    <t>Hw1: team formation</t>
+  </si>
+  <si>
+    <t>Intro to data sets</t>
+  </si>
+  <si>
+    <t>Introduction to class logistics
+Team Formation</t>
+  </si>
+  <si>
+    <t>HW 1</t>
+  </si>
+  <si>
+    <t>RAT on class logistics</t>
+  </si>
+  <si>
+    <t>RAT on data vocabulary (Ch 1.1)</t>
+  </si>
+  <si>
+    <t>CN 1.2</t>
+  </si>
+  <si>
+    <t>CN 1.1</t>
+  </si>
+  <si>
+    <t>Create a MATH315 folder on your computer
+* Follow the [Instruction Slides]() to install needed onto your own computer
+* Download the HW 1 [RMD Template]() and [PDF] file into this folder
+* Install the `rmarkdown` package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read [Learning: Your First Job](../Articles/Learning - Your First Job (Leamnson 2002).pdf)&lt;/a&gt;
+* Read [Self Regulated Learning](../Articles/Self Regulated Learning Questions (Neilson).pdf)&lt;/a&gt;
+* Read the UMN page on [Zombies]() and teamwork. Complete the strengths identifier. </t>
+  </si>
+  <si>
+    <t>Data Camp: Introduction to Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the [Syllabus](syllabus_315.pdf)
+* Purchase the Course Notes (CN) packet
+* Download or purchase Open Intro (OI) Textbook
+* Bookmark the class website 
+* Join the class Data Camp group &amp; start the Intro to R lesson (USE EMAILED LINK)
+* Read [Adventures in R (Nature article)](../Articles/Adventures in R (Tippmann 2015).pdf) 
+* Read [Metacognition and academic achievement](../Articles/MAI and academic achievement in college students (Young, Fry, 2008).pdf)
+* Take the [Metacognition Awareness Inventory](../Articles/Metacognition Awareness Inventory.pdf)
+</t>
+  </si>
+  <si>
+    <t>Week</t>
   </si>
 </sst>
 </file>
@@ -534,10 +566,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -949,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -960,16 +992,16 @@
     <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="5" customWidth="1"/>
     <col min="5" max="5" width="26" style="13" customWidth="1"/>
-    <col min="6" max="6" width="35.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="52.5" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="39.5" style="13" customWidth="1"/>
     <col min="9" max="9" width="31.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1">
+    <row r="1" spans="1:10" ht="19" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -978,26 +1010,26 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="75">
+    <row r="2" spans="1:10" ht="210">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1005,67 +1037,75 @@
         <v>41506</v>
       </c>
       <c r="C2" s="4" t="str">
-        <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
+        <f t="shared" ref="C2:C40" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="30">
+    <row r="3" spans="1:10" ht="90">
       <c r="B3" s="3">
         <f>B2+2</f>
         <v>41508</v>
       </c>
       <c r="C3" s="4" t="str">
-        <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="19"/>
+        <v>61</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="90">
       <c r="A4" s="6"/>
       <c r="B4" s="7">
         <f>B3+2</f>
         <v>41510</v>
       </c>
       <c r="C4" s="8" t="str">
-        <f>TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="10"/>
     </row>
@@ -1075,57 +1115,66 @@
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <f>B2+7</f>
+        <f t="shared" ref="B5:B41" si="1">B2+7</f>
         <v>41513</v>
       </c>
       <c r="C5" s="4" t="str">
-        <f>TEXT(WEEKDAY(B5,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="30">
       <c r="B6" s="3">
-        <f>B3+7</f>
+        <f t="shared" si="1"/>
         <v>41515</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f>TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="19" t="s">
-        <v>24</v>
+        <v>56</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="30">
+    <row r="7" spans="1:10">
       <c r="A7" s="6"/>
       <c r="B7" s="7">
-        <f>B4+7</f>
+        <f t="shared" si="1"/>
         <v>41517</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>TEXT(WEEKDAY(B7,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="22" t="s">
-        <v>42</v>
+      <c r="E7" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="24"/>
-      <c r="G7" s="32" t="s">
-        <v>25</v>
+      <c r="G7" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="H7" s="21"/>
       <c r="I7" s="11"/>
@@ -1136,30 +1185,30 @@
         <v>3</v>
       </c>
       <c r="B8" s="3">
-        <f>B5+7</f>
+        <f t="shared" si="1"/>
         <v>41520</v>
       </c>
       <c r="C8" s="4" t="str">
-        <f>TEXT(WEEKDAY(B8,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="3">
-        <f>B6+7</f>
+        <f t="shared" si="1"/>
         <v>41522</v>
       </c>
       <c r="C9" s="4" t="str">
-        <f>TEXT(WEEKDAY(B9,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="17"/>
@@ -1167,19 +1216,19 @@
     <row r="10" spans="1:10">
       <c r="A10" s="6"/>
       <c r="B10" s="7">
-        <f>B7+7</f>
+        <f t="shared" si="1"/>
         <v>41524</v>
       </c>
       <c r="C10" s="8" t="str">
-        <f>TEXT(WEEKDAY(B10,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F10" s="24"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="21"/>
       <c r="I10" s="11"/>
     </row>
@@ -1189,15 +1238,15 @@
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <f>B8+7</f>
+        <f t="shared" si="1"/>
         <v>41527</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f>TEXT(WEEKDAY(B11,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E11" s="19"/>
       <c r="H11" s="19"/>
@@ -1205,15 +1254,15 @@
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="3">
-        <f>B9+7</f>
+        <f t="shared" si="1"/>
         <v>41529</v>
       </c>
       <c r="C12" s="4" t="str">
-        <f>TEXT(WEEKDAY(B12,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E12" s="19"/>
       <c r="H12" s="19"/>
@@ -1222,19 +1271,19 @@
     <row r="13" spans="1:10">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
-        <f>B10+7</f>
+        <f t="shared" si="1"/>
         <v>41531</v>
       </c>
       <c r="C13" s="8" t="str">
-        <f>TEXT(WEEKDAY(B13,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="11"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="21"/>
       <c r="I13" s="11"/>
     </row>
@@ -1244,30 +1293,30 @@
         <v>5</v>
       </c>
       <c r="B14" s="3">
-        <f>B11+7</f>
+        <f t="shared" si="1"/>
         <v>41534</v>
       </c>
       <c r="C14" s="4" t="str">
-        <f>TEXT(WEEKDAY(B14,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="3">
-        <f>B12+7</f>
+        <f t="shared" si="1"/>
         <v>41536</v>
       </c>
       <c r="C15" s="4" t="str">
-        <f>TEXT(WEEKDAY(B15,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="17"/>
@@ -1275,19 +1324,19 @@
     <row r="16" spans="1:10">
       <c r="A16" s="6"/>
       <c r="B16" s="7">
-        <f>B13+7</f>
+        <f t="shared" si="1"/>
         <v>41538</v>
       </c>
       <c r="C16" s="8" t="str">
-        <f>TEXT(WEEKDAY(B16,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F16" s="24"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="21"/>
       <c r="I16" s="11"/>
     </row>
@@ -1297,30 +1346,30 @@
         <v>6</v>
       </c>
       <c r="B17" s="3">
-        <f>B14+7</f>
+        <f t="shared" si="1"/>
         <v>41541</v>
       </c>
       <c r="C17" s="4" t="str">
-        <f>TEXT(WEEKDAY(B17,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="B18" s="3">
-        <f>B15+7</f>
+        <f t="shared" si="1"/>
         <v>41543</v>
       </c>
       <c r="C18" s="4" t="str">
-        <f>TEXT(WEEKDAY(B18,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="17"/>
@@ -1328,19 +1377,19 @@
     <row r="19" spans="1:9">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
-        <f>B16+7</f>
+        <f t="shared" si="1"/>
         <v>41545</v>
       </c>
       <c r="C19" s="8" t="str">
-        <f>TEXT(WEEKDAY(B19,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F19" s="24"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="21"/>
       <c r="I19" s="11"/>
     </row>
@@ -1350,30 +1399,30 @@
         <v>7</v>
       </c>
       <c r="B20" s="3">
-        <f>B17+7</f>
+        <f t="shared" si="1"/>
         <v>41548</v>
       </c>
       <c r="C20" s="4" t="str">
-        <f>TEXT(WEEKDAY(B20,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9">
       <c r="B21" s="3">
-        <f>B18+7</f>
+        <f t="shared" si="1"/>
         <v>41550</v>
       </c>
       <c r="C21" s="4" t="str">
-        <f>TEXT(WEEKDAY(B21,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="17"/>
@@ -1381,19 +1430,19 @@
     <row r="22" spans="1:9">
       <c r="A22" s="6"/>
       <c r="B22" s="7">
-        <f>B19+7</f>
+        <f t="shared" si="1"/>
         <v>41552</v>
       </c>
       <c r="C22" s="8" t="str">
-        <f>TEXT(WEEKDAY(B22,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="20" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F22" s="24"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="21"/>
       <c r="I22" s="11"/>
     </row>
@@ -1403,36 +1452,36 @@
         <v>8</v>
       </c>
       <c r="B23" s="3">
-        <f>B20+7</f>
+        <f t="shared" si="1"/>
         <v>41555</v>
       </c>
       <c r="C23" s="4" t="str">
-        <f>TEXT(WEEKDAY(B23,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="17"/>
     </row>
     <row r="24" spans="1:9" ht="45">
       <c r="B24" s="3">
-        <f>B21+7</f>
+        <f t="shared" si="1"/>
         <v>41557</v>
       </c>
       <c r="C24" s="4" t="str">
-        <f>TEXT(WEEKDAY(B24,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="17"/>
@@ -1440,21 +1489,21 @@
     <row r="25" spans="1:9" ht="45">
       <c r="A25" s="6"/>
       <c r="B25" s="7">
-        <f>B22+7</f>
+        <f t="shared" si="1"/>
         <v>41559</v>
       </c>
       <c r="C25" s="8" t="str">
-        <f>TEXT(WEEKDAY(B25,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F25" s="24"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="21"/>
       <c r="I25" s="11"/>
     </row>
@@ -1464,31 +1513,31 @@
         <v>9</v>
       </c>
       <c r="B26" s="3">
-        <f>B23+7</f>
+        <f t="shared" si="1"/>
         <v>41562</v>
       </c>
       <c r="C26" s="4" t="str">
-        <f>TEXT(WEEKDAY(B26,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="33"/>
+        <v>36</v>
+      </c>
+      <c r="E26" s="32"/>
       <c r="H26" s="19"/>
       <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" s="3">
-        <f>B24+7</f>
+        <f t="shared" si="1"/>
         <v>41564</v>
       </c>
       <c r="C27" s="4" t="str">
-        <f>TEXT(WEEKDAY(B27,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E27" s="19"/>
       <c r="H27" s="19"/>
@@ -1497,17 +1546,17 @@
     <row r="28" spans="1:9">
       <c r="A28" s="6"/>
       <c r="B28" s="7">
-        <f>B25+7</f>
+        <f t="shared" si="1"/>
         <v>41566</v>
       </c>
       <c r="C28" s="8" t="str">
-        <f>TEXT(WEEKDAY(B28,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="20"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="11"/>
+      <c r="G28" s="9"/>
       <c r="H28" s="21"/>
       <c r="I28" s="11"/>
     </row>
@@ -1517,11 +1566,11 @@
         <v>10</v>
       </c>
       <c r="B29" s="3">
-        <f>B26+7</f>
+        <f t="shared" si="1"/>
         <v>41569</v>
       </c>
       <c r="C29" s="4" t="str">
-        <f>TEXT(WEEKDAY(B29,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="E29" s="19"/>
@@ -1530,11 +1579,11 @@
     </row>
     <row r="30" spans="1:9">
       <c r="B30" s="3">
-        <f>B27+7</f>
+        <f t="shared" si="1"/>
         <v>41571</v>
       </c>
       <c r="C30" s="4" t="str">
-        <f>TEXT(WEEKDAY(B30,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="E30" s="19"/>
@@ -1544,17 +1593,17 @@
     <row r="31" spans="1:9">
       <c r="A31" s="6"/>
       <c r="B31" s="7">
-        <f>B28+7</f>
+        <f t="shared" si="1"/>
         <v>41573</v>
       </c>
       <c r="C31" s="8" t="str">
-        <f>TEXT(WEEKDAY(B31,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="20"/>
       <c r="F31" s="24"/>
-      <c r="G31" s="11"/>
+      <c r="G31" s="9"/>
       <c r="H31" s="21"/>
       <c r="I31" s="11"/>
     </row>
@@ -1564,33 +1613,33 @@
         <v>11</v>
       </c>
       <c r="B32" s="3">
-        <f>B29+7</f>
+        <f t="shared" si="1"/>
         <v>41576</v>
       </c>
       <c r="C32" s="4" t="str">
-        <f>TEXT(WEEKDAY(B32,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" ht="30">
       <c r="B33" s="3">
-        <f>B30+7</f>
+        <f t="shared" si="1"/>
         <v>41578</v>
       </c>
       <c r="C33" s="4" t="str">
-        <f>TEXT(WEEKDAY(B33,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E33" s="19"/>
       <c r="H33" s="19"/>
@@ -1599,19 +1648,19 @@
     <row r="34" spans="1:9" ht="30">
       <c r="A34" s="6"/>
       <c r="B34" s="7">
-        <f>B31+7</f>
+        <f t="shared" si="1"/>
         <v>41580</v>
       </c>
       <c r="C34" s="8" t="str">
-        <f>TEXT(WEEKDAY(B34,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="24"/>
-      <c r="G34" s="11"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="21"/>
       <c r="I34" s="11"/>
     </row>
@@ -1621,33 +1670,33 @@
         <v>12</v>
       </c>
       <c r="B35" s="3">
-        <f>B32+7</f>
+        <f t="shared" si="1"/>
         <v>41583</v>
       </c>
       <c r="C35" s="4" t="str">
-        <f>TEXT(WEEKDAY(B35,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9">
       <c r="B36" s="3">
-        <f>B33+7</f>
+        <f t="shared" si="1"/>
         <v>41585</v>
       </c>
       <c r="C36" s="4" t="str">
-        <f>TEXT(WEEKDAY(B36,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E36" s="19"/>
       <c r="H36" s="19"/>
@@ -1656,19 +1705,19 @@
     <row r="37" spans="1:9" ht="30">
       <c r="A37" s="6"/>
       <c r="B37" s="7">
-        <f>B34+7</f>
+        <f t="shared" si="1"/>
         <v>41587</v>
       </c>
       <c r="C37" s="8" t="str">
-        <f>TEXT(WEEKDAY(B37,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="11"/>
+      <c r="G37" s="9"/>
       <c r="H37" s="21"/>
       <c r="I37" s="11"/>
     </row>
@@ -1678,26 +1727,26 @@
         <v>13</v>
       </c>
       <c r="B38" s="3">
-        <f>B35+7</f>
+        <f t="shared" si="1"/>
         <v>41590</v>
       </c>
       <c r="C38" s="4" t="str">
-        <f>TEXT(WEEKDAY(B38,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H38" s="19"/>
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9">
       <c r="B39" s="3">
-        <f>B36+7</f>
+        <f t="shared" si="1"/>
         <v>41592</v>
       </c>
       <c r="C39" s="4" t="str">
-        <f>TEXT(WEEKDAY(B39,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
       <c r="E39" s="19"/>
@@ -1707,33 +1756,33 @@
     <row r="40" spans="1:9">
       <c r="A40" s="6"/>
       <c r="B40" s="7">
-        <f>B37+7</f>
+        <f t="shared" si="1"/>
         <v>41594</v>
       </c>
       <c r="C40" s="8" t="str">
-        <f>TEXT(WEEKDAY(B40,1)+1, "ddd")</f>
+        <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="20"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="11"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="21"/>
       <c r="I40" s="11"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="25"/>
       <c r="B41" s="26">
-        <f>B38+7</f>
+        <f t="shared" si="1"/>
         <v>41597</v>
       </c>
       <c r="C41" s="27"/>
       <c r="D41" s="28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="29"/>
       <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
+      <c r="G41" s="28"/>
       <c r="H41" s="29"/>
       <c r="I41" s="31"/>
     </row>
@@ -1746,11 +1795,11 @@
         <v>41604</v>
       </c>
       <c r="C42" s="4" t="str">
-        <f>TEXT(WEEKDAY(B42,1)+1, "ddd")</f>
+        <f t="shared" ref="C42:C47" si="2">TEXT(WEEKDAY(B42,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="17"/>
@@ -1761,7 +1810,7 @@
         <v>41606</v>
       </c>
       <c r="C43" s="4" t="str">
-        <f>TEXT(WEEKDAY(B43,1)+1, "ddd")</f>
+        <f t="shared" si="2"/>
         <v>Wed</v>
       </c>
       <c r="E43" s="19"/>
@@ -1775,13 +1824,13 @@
         <v>41608</v>
       </c>
       <c r="C44" s="8" t="str">
-        <f>TEXT(WEEKDAY(B44,1)+1, "ddd")</f>
+        <f t="shared" si="2"/>
         <v>Fri</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="20"/>
       <c r="F44" s="24"/>
-      <c r="G44" s="11"/>
+      <c r="G44" s="9"/>
       <c r="H44" s="21"/>
       <c r="I44" s="11"/>
     </row>
@@ -1795,14 +1844,14 @@
         <v>41611</v>
       </c>
       <c r="C45" s="4" t="str">
-        <f>TEXT(WEEKDAY(B45,1)+1, "ddd")</f>
+        <f t="shared" si="2"/>
         <v>Mon</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="17"/>
@@ -1813,11 +1862,11 @@
         <v>41613</v>
       </c>
       <c r="C46" s="4" t="str">
-        <f>TEXT(WEEKDAY(B46,1)+1, "ddd")</f>
+        <f t="shared" si="2"/>
         <v>Wed</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E46" s="19"/>
       <c r="H46" s="19"/>
@@ -1830,24 +1879,24 @@
         <v>41615</v>
       </c>
       <c r="C47" s="8" t="str">
-        <f>TEXT(WEEKDAY(B47,1)+1, "ddd")</f>
+        <f t="shared" si="2"/>
         <v>Fri</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="20"/>
       <c r="F47" s="24"/>
-      <c r="G47" s="11"/>
+      <c r="G47" s="9"/>
       <c r="H47" s="21"/>
       <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:9" ht="45">
       <c r="A48" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E48" s="19"/>
       <c r="F48" s="12"/>

</xml_diff>

<commit_message>
redo schedule, weekly overview. add hw1
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>date</t>
   </si>
@@ -45,219 +50,137 @@
     <t>topic</t>
   </si>
   <si>
-    <t>prep</t>
-  </si>
-  <si>
     <t>eval</t>
   </si>
   <si>
-    <t>How to submit homework 
-* Intro to R Markdown</t>
-  </si>
-  <si>
-    <t>R Markdown</t>
-  </si>
-  <si>
-    <t>Data types and codebooks</t>
-  </si>
-  <si>
-    <t>Characterizing Data
+    <t>data basics, struture</t>
+  </si>
+  <si>
+    <t>Exam 1</t>
+  </si>
+  <si>
+    <t>Distributions (Normal, T)</t>
+  </si>
+  <si>
+    <t>LLN, CLT</t>
+  </si>
+  <si>
+    <t>Introduction to Inference</t>
+  </si>
+  <si>
+    <t>R for 1 sample inference - mean, prop</t>
+  </si>
+  <si>
+    <t>confidence intervals</t>
+  </si>
+  <si>
+    <t>hypothesis testing</t>
+  </si>
+  <si>
+    <t>Assessing normality</t>
+  </si>
+  <si>
+    <t>bivariate graphics - cat vs cat</t>
+  </si>
+  <si>
+    <t>cont vs cat</t>
+  </si>
+  <si>
+    <t>cont vs cont</t>
+  </si>
+  <si>
+    <t>explanatory vs response</t>
+  </si>
+  <si>
+    <t>experimental design</t>
+  </si>
+  <si>
+    <t>Exam 2</t>
+  </si>
+  <si>
+    <t>Two sample inference - paired</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Multiple Regression</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>Decision Errors, choosing analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lit review, using passion driven stats. How to teach this? </t>
+  </si>
+  <si>
+    <t>univariate numerical</t>
+  </si>
+  <si>
+    <t>univariate categorical</t>
+  </si>
+  <si>
+    <t>Hw1: team formation</t>
+  </si>
+  <si>
+    <t>Intro to data sets</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>How to turn in Homework 
 * Data Dictionaries</t>
   </si>
   <si>
-    <t>Logistics, Programs, Accounts, Metacognition, Intro to Data Camp and R</t>
-  </si>
-  <si>
-    <t>How data is stored</t>
-  </si>
-  <si>
-    <t>data basics, struture</t>
-  </si>
-  <si>
-    <t>Choose a data set to explore</t>
-  </si>
-  <si>
-    <t>Exam 1</t>
-  </si>
-  <si>
-    <t>Work on EDA</t>
-  </si>
-  <si>
-    <t>Exam Prep</t>
-  </si>
-  <si>
-    <t>Distributions (Normal, T)</t>
-  </si>
-  <si>
-    <t>LLN, CLT</t>
-  </si>
-  <si>
-    <t>Introduction to Inference</t>
-  </si>
-  <si>
-    <t>R for 1 sample inference - mean, prop</t>
-  </si>
-  <si>
-    <t>confidence intervals</t>
-  </si>
-  <si>
-    <t>hypothesis testing</t>
-  </si>
-  <si>
-    <t>Assessing normality</t>
-  </si>
-  <si>
-    <t>bivariate graphics - cat vs cat</t>
-  </si>
-  <si>
-    <t>cont vs cat</t>
-  </si>
-  <si>
-    <t>cont vs cont</t>
-  </si>
-  <si>
-    <t>Population and samples</t>
-  </si>
-  <si>
-    <t>explanatory vs response</t>
-  </si>
-  <si>
-    <t>experimental design</t>
-  </si>
-  <si>
-    <t>Exam 2</t>
-  </si>
-  <si>
-    <t>Exam review</t>
-  </si>
-  <si>
-    <t>Two sample inference - paired</t>
-  </si>
-  <si>
-    <t>Testing a difference between paired means</t>
-  </si>
-  <si>
-    <t>Testing a difference between independent means</t>
-  </si>
-  <si>
-    <t>Testing a difference between independent proportions</t>
-  </si>
-  <si>
-    <t>Introduction to ANOVA</t>
-  </si>
-  <si>
-    <t>One-way ANOVA</t>
-  </si>
-  <si>
-    <t>Two-way ANOVA with mean plots</t>
-  </si>
-  <si>
-    <t>Open Project work time</t>
-  </si>
-  <si>
-    <t>Entire week</t>
-  </si>
-  <si>
-    <t>Final Exam
-* e-Poster presentation and evaluation</t>
-  </si>
-  <si>
-    <t>Linear Regression</t>
-  </si>
-  <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>Multiple Regression</t>
-  </si>
-  <si>
-    <t>EDA</t>
-  </si>
-  <si>
-    <t>Statistical inference using R</t>
-  </si>
-  <si>
-    <t>Decision Errors, choosing analysis</t>
-  </si>
-  <si>
-    <t>Types of statistical errors 
-* Choosing appropriate analysis procedures</t>
-  </si>
-  <si>
-    <t>Refining your research question, writing science and statistics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lit review, using passion driven stats. How to teach this? </t>
-  </si>
-  <si>
-    <t>univariate numerical</t>
-  </si>
-  <si>
-    <t>univariate categorical</t>
-  </si>
-  <si>
-    <t>Hw1: team formation</t>
-  </si>
-  <si>
-    <t>Intro to data sets</t>
-  </si>
-  <si>
-    <t>HW 1</t>
-  </si>
-  <si>
-    <t>RAT on data vocabulary (Ch 1.1)</t>
-  </si>
-  <si>
-    <t>CN 1.2</t>
-  </si>
-  <si>
-    <t>Create a MATH315 folder on your computer
-* Follow the [Instruction Slides]() to install needed onto your own computer
-* Download the HW 1 [RMD Template]() and [PDF] file into this folder
-* Install the `rmarkdown` package</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>RAT on class logistics
-* [Metacognition pre-assessment]()</t>
-  </si>
-  <si>
-    <t>CN 1.1
-* Read [Learning: Your First Job](../Articles/Learning - Your First Job (Leamnson 2002).pdf)
-* Read [Self Regulated Learning](../Articles/Self Regulated Learning Questions (Neilson).pdf)</t>
-  </si>
-  <si>
-    <t>* Read the UMN page on [Zombies]() and teamwork. Complete the strengths identifier. 
-* Read [Metacognition and academic achievement](../Articles/MAI and academic achievement in college students (Young, Fry, 2008).pdf)
-* Take the [Metacognition Awareness Inventory](../Articles/Metacognition Awareness Inventory.pdf)</t>
-  </si>
-  <si>
-    <t>Introduction to class logistics * 
-Team Formation</t>
-  </si>
-  <si>
-    <t>Data Camp - Introduction to Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read the [Syllabus](syllabus_315.pdf)
-* Purchase the Course Notes (CN) packet
-* Download or purchase Open Intro (OI) Textbook
-* Bookmark the class website 
-* Join the class Data Camp group (USE EMAILED LINK)
-* Read [Adventures in R (Nature article)](../Articles/Adventures in R (Tippmann 2015).pdf) 
+    <t>No Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Collection
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Data Camp - Intro to R (first chapter only) 
-</t>
+    <t>Intro to data camp and R (outside of class)</t>
+  </si>
+  <si>
+    <t>in: Logistics, Programs, Accounts, Metacognition, Teams, PDS
+out: Data Camp and R, PDS intro video</t>
+  </si>
+  <si>
+    <t>codebooks</t>
+  </si>
+  <si>
+    <t>[Week 1 Overview](week/1.html)</t>
+  </si>
+  <si>
+    <t>Intro to R Data Camp Lesson
+* Corresponding BBLearn quiz
+* PS 1.1-1.6 (part of HW 1)
+* PS 1.5 (BBL)
+* HW 1</t>
+  </si>
+  <si>
+    <t>Introduction to the class structure and logistics</t>
+  </si>
+  <si>
+    <t>How data is stored * Data Types</t>
+  </si>
+  <si>
+    <t>[Week 2 Overview](week/2.html)</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -472,7 +395,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -504,9 +427,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -522,9 +442,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -564,13 +481,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,57 +897,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="5" customWidth="1"/>
-    <col min="5" max="5" width="26" style="13" customWidth="1"/>
+    <col min="5" max="5" width="26" style="12" customWidth="1"/>
     <col min="6" max="6" width="52.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="39.5" style="13" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="27.125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="39.5" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" thickBot="1">
-      <c r="A1" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="120">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1042,21 +955,20 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>14</v>
+        <v>44</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="90">
+        <v>43</v>
+      </c>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <f>B2+2</f>
         <v>41508</v>
@@ -1066,23 +978,17 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="105">
+        <v>38</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="H3" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7">
         <f>B3+2</f>
@@ -1093,24 +999,19 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" ht="75">
+        <v>36</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>A2+1</f>
         <v>2</v>
@@ -1124,21 +1025,17 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>16</v>
+        <v>45</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" ht="30">
+        <v>46</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <f t="shared" si="1"/>
         <v>41515</v>
@@ -1147,19 +1044,13 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="E6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7">
         <f t="shared" si="1"/>
@@ -1170,17 +1061,14 @@
         <v>Fri</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="E7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>A5+1</f>
         <v>3</v>
@@ -1193,13 +1081,15 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="D8" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" si="1"/>
         <v>41522</v>
@@ -1208,13 +1098,12 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="E9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7">
         <f t="shared" si="1"/>
@@ -1225,15 +1114,14 @@
         <v>Fri</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="24"/>
+      <c r="E10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="22"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>A8+1</f>
         <v>4</v>
@@ -1246,14 +1134,10 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="E11" s="17"/>
+      <c r="H11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="1"/>
         <v>41529</v>
@@ -1262,14 +1146,10 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="E12" s="17"/>
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
         <f t="shared" si="1"/>
@@ -1280,15 +1160,14 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f>A11+1</f>
         <v>5</v>
@@ -1301,13 +1180,10 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="E14" s="17"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="1"/>
         <v>41536</v>
@@ -1316,13 +1192,12 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="E15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7">
         <f t="shared" si="1"/>
@@ -1333,15 +1208,14 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="24"/>
+      <c r="E16" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="22"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="H16" s="19"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f>A14+1</f>
         <v>6</v>
@@ -1354,13 +1228,12 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="E17" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="1"/>
         <v>41543</v>
@@ -1369,13 +1242,12 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="E18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
         <f t="shared" si="1"/>
@@ -1386,15 +1258,14 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="24"/>
+      <c r="E19" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="22"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f>A17+1</f>
         <v>7</v>
@@ -1407,13 +1278,12 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="E20" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="1"/>
         <v>41550</v>
@@ -1422,13 +1292,12 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="E21" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7">
         <f t="shared" si="1"/>
@@ -1439,15 +1308,14 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="24"/>
+      <c r="E22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="22"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" ht="30">
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f>A20+1</f>
         <v>8</v>
@@ -1460,16 +1328,12 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-    </row>
-    <row r="24" spans="1:9" ht="45">
+      <c r="E23" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="1"/>
         <v>41557</v>
@@ -1478,16 +1342,12 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="17"/>
-    </row>
-    <row r="25" spans="1:9" ht="45">
+      <c r="E24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7">
         <f t="shared" si="1"/>
@@ -1497,18 +1357,15 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="24"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="22"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f>A23+1</f>
         <v>9</v>
@@ -1521,14 +1378,10 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="32"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="E26" s="29"/>
+      <c r="H26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="1"/>
         <v>41564</v>
@@ -1538,13 +1391,12 @@
         <v>Wed</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9">
+        <v>23</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="H27" s="17"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="7">
         <f t="shared" si="1"/>
@@ -1555,13 +1407,12 @@
         <v>Fri</v>
       </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="24"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f>A26+1</f>
         <v>10</v>
@@ -1574,11 +1425,10 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="17"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="E29" s="17"/>
+      <c r="H29" s="17"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="1"/>
         <v>41571</v>
@@ -1587,11 +1437,10 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="17"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="E30" s="17"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="7">
         <f t="shared" si="1"/>
@@ -1602,13 +1451,12 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="9"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="24"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="22"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" ht="30">
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>A29+1</f>
         <v>11</v>
@@ -1621,16 +1469,12 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="17"/>
-    </row>
-    <row r="33" spans="1:9" ht="30">
+      <c r="E32" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <f t="shared" si="1"/>
         <v>41578</v>
@@ -1639,14 +1483,10 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="17"/>
-    </row>
-    <row r="34" spans="1:9" ht="30">
+      <c r="E33" s="17"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="7">
         <f t="shared" si="1"/>
@@ -1656,16 +1496,13 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="24"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="H34" s="19"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f>A32+1</f>
         <v>12</v>
@@ -1678,16 +1515,12 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="17"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="E35" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <f t="shared" si="1"/>
         <v>41585</v>
@@ -1696,14 +1529,10 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="17"/>
-    </row>
-    <row r="37" spans="1:9" ht="30">
+      <c r="E36" s="17"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="7">
         <f t="shared" si="1"/>
@@ -1713,16 +1542,13 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="24"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="H37" s="19"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f>A35+1</f>
         <v>13</v>
@@ -1735,13 +1561,12 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E38" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="17"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="E38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="17"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
         <f t="shared" si="1"/>
         <v>41592</v>
@@ -1750,11 +1575,10 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="17"/>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="E39" s="17"/>
+      <c r="H39" s="17"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="7">
         <f t="shared" si="1"/>
@@ -1765,29 +1589,27 @@
         <v>Fri</v>
       </c>
       <c r="D40" s="9"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="24"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="22"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="11"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="25"/>
-      <c r="B41" s="26">
+      <c r="H40" s="19"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24">
         <f t="shared" si="1"/>
         <v>41597</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="28" t="s">
+      <c r="C41" s="25"/>
+      <c r="D41" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="31"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="27"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>14</v>
       </c>
@@ -1799,13 +1621,12 @@
         <f t="shared" ref="C42:C47" si="2">TEXT(WEEKDAY(B42,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="E42" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H42" s="19"/>
-      <c r="I42" s="17"/>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="E42" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H42" s="17"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <f>B42+2</f>
         <v>41606</v>
@@ -1814,11 +1635,10 @@
         <f t="shared" si="2"/>
         <v>Wed</v>
       </c>
-      <c r="E43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="17"/>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="E43" s="17"/>
+      <c r="H43" s="17"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="7">
         <f>B43+2</f>
@@ -1829,13 +1649,12 @@
         <v>Fri</v>
       </c>
       <c r="D44" s="9"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="24"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="22"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="11"/>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="H44" s="19"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f>A42+1</f>
         <v>15</v>
@@ -1848,16 +1667,12 @@
         <f t="shared" si="2"/>
         <v>Mon</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="19"/>
-      <c r="I45" s="17"/>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="E45" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <f>B43+7</f>
         <v>41613</v>
@@ -1866,14 +1681,10 @@
         <f t="shared" si="2"/>
         <v>Wed</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="17"/>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="E46" s="17"/>
+      <c r="H46" s="17"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="7">
         <f>B44+7</f>
@@ -1884,28 +1695,27 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="9"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="24"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="22"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="11"/>
-    </row>
-    <row r="48" spans="1:9" ht="45">
+      <c r="H47" s="19"/>
+    </row>
+    <row r="48" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="12"/>
-      <c r="H48" s="19"/>
+        <v>47</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="F48" s="11"/>
+      <c r="H48" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
move week overviews, rebuild.
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -155,9 +155,6 @@
     <t>codebooks</t>
   </si>
   <si>
-    <t>[Week 1 Overview](week/1.html)</t>
-  </si>
-  <si>
     <t>Intro to R Data Camp Lesson
 * Corresponding BBLearn quiz
 * PS 1.1-1.6 (part of HW 1)
@@ -171,10 +168,13 @@
     <t>How data is stored * Data Types</t>
   </si>
   <si>
-    <t>[Week 2 Overview](week/2.html)</t>
-  </si>
-  <si>
     <t>Final Exam</t>
+  </si>
+  <si>
+    <t>[Week 1 Overview](wk1.html)</t>
+  </si>
+  <si>
+    <t>[Week 2 Overview](wk2.html)</t>
   </si>
 </sst>
 </file>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -955,16 +955,16 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="H2" s="17"/>
     </row>
@@ -1025,13 +1025,13 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" s="17"/>
     </row>
@@ -1707,7 +1707,7 @@
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="11"/>

</xml_diff>

<commit_message>
update syllabus and day 1 activities.
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -378,12 +378,6 @@
     <t>* Personal Codebook / Research question assignment (Due 9/3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Acquire course materials
-* Sign up for data camp
-* Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Get your computer ready for analysis
 * Download the Add Health codebook </t>
   </si>
@@ -461,6 +455,12 @@
   <si>
     <t>RAT on CN 2.4 (bivariate)
 * Answer questions about CN 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acquire course materials
+* Sign up for data camp, Google Group. 
+* Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
+</t>
   </si>
 </sst>
 </file>
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1225,10 +1225,10 @@
         <v>46</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>21</v>
@@ -1259,13 +1259,13 @@
         <v>31</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -1290,13 +1290,13 @@
         <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
         <v>41</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
         <v>61</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1490,13 +1490,13 @@
       <c r="F10" s="15"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>58</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -1520,13 +1520,13 @@
         <v>69</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>65</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>63</v>
@@ -1558,7 +1558,7 @@
         <v>71</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1609,10 +1609,10 @@
         <v>66</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
alter week 1, rename all assignments more clearly
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="156">
   <si>
     <t>date</t>
   </si>
@@ -45,21 +45,9 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Exam 1</t>
-  </si>
-  <si>
     <t>R for 1 sample inference - mean, prop</t>
   </si>
   <si>
-    <t>confidence intervals</t>
-  </si>
-  <si>
-    <t>hypothesis testing</t>
-  </si>
-  <si>
-    <t>Decision Errors, choosing analysis</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -69,9 +57,6 @@
     <t>Introduction to the class structure and logistics</t>
   </si>
   <si>
-    <t>Final Exam</t>
-  </si>
-  <si>
     <t>Describing univariate numerical data</t>
   </si>
   <si>
@@ -82,9 +67,6 @@
   </si>
   <si>
     <t>Describing bivariate relationships</t>
-  </si>
-  <si>
-    <t>PDS video 4 - post personal codebook, talks about lit review</t>
   </si>
   <si>
     <t xml:space="preserve">Logistics, Programs, Accounts, Metacognition, Teams, Data Camp. 
@@ -97,29 +79,6 @@
     <t>after</t>
   </si>
   <si>
-    <t>RAT on Ch 1
-* Share answers to questions and examples in Ch 1</t>
-  </si>
-  <si>
-    <t>* PDS Intro section
-* Add Health codebook
-* Software overview</t>
-  </si>
-  <si>
-    <t>Write down questions about class logistics and structure
-* Learn about the Add Health data
-* Form analysis pairs
-* Learn how to use Rstudio and how to turn in Homework</t>
-  </si>
-  <si>
-    <t>Data analysis life cycle
-* Add Health data
-* How to turn in homework using R Markdown</t>
-  </si>
-  <si>
-    <t>Class logistic FAQ, Data analysis life cycle, Introduce Add Health, R Studio</t>
-  </si>
-  <si>
     <t>Data architecture</t>
   </si>
   <si>
@@ -127,15 +86,6 @@
   </si>
   <si>
     <t>[Week 2 overview](wk02.html)</t>
-  </si>
-  <si>
-    <t>[Week 1 overview](wk01.html)
-* metacognition paper, inventory
-* Learning - Your first job
-* Nature: Adventures in R</t>
-  </si>
-  <si>
-    <t>* Read CN 1 and OI 1.3-1.5</t>
   </si>
   <si>
     <t>Watch PDS Video 2 (24 min) (Due 8/25)
@@ -151,36 +101,10 @@
     <t>univariate numerical (2.2)</t>
   </si>
   <si>
-    <t>Discuss class logistics
-* Form support groups
-* What does it take to get an A? a C-?</t>
-  </si>
-  <si>
-    <t>Data Collection and experimental design
-* Continuing to learn how to use R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ch 1
-pop vs samp. X vs y. data collection bias. Confounding. </t>
-  </si>
-  <si>
-    <t>Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
-* Complete both corresponding BBL quizzes (Due 9/3)
-* PS 1.5 (Due 9/3)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Share your research topic and questions
 * Search primary sources, take notes of articles to further look into. </t>
   </si>
   <si>
-    <t xml:space="preserve">RAT on Class logistics &amp; Data Types
-* Medical records assignment
-</t>
-  </si>
-  <si>
-    <t>PS 2.2 (Due 8/30)</t>
-  </si>
-  <si>
     <t>Data types (2.1). How data is stored, mini codebooks</t>
   </si>
   <si>
@@ -190,41 +114,15 @@
     <t>comments</t>
   </si>
   <si>
-    <t>* PDS Video 4 (8 min)
-* Read: How to read a journal article</t>
-  </si>
-  <si>
-    <t>open work</t>
-  </si>
-  <si>
-    <t>ANOVA - 1 sample</t>
-  </si>
-  <si>
-    <t>ANOVA- 2 sample</t>
-  </si>
-  <si>
     <t>Chi-square</t>
   </si>
   <si>
-    <t>Logistic regression</t>
-  </si>
-  <si>
     <t>data viz lab</t>
   </si>
   <si>
     <t>Creating data visualizations in R</t>
   </si>
   <si>
-    <t xml:space="preserve">* Data viz tutorial website
-</t>
-  </si>
-  <si>
-    <t>Research plan outline</t>
-  </si>
-  <si>
-    <t>Research plan</t>
-  </si>
-  <si>
     <t>Answer questions in CN 2.3</t>
   </si>
   <si>
@@ -232,34 +130,12 @@
   </si>
   <si>
     <t>[Week 3 overview](wk03.html)</t>
-  </si>
-  <si>
-    <t>RAT on CN 2.2, 2.3
-* Answer questions in CN 2.2</t>
   </si>
   <si>
     <t>Data management
 * Raw vs cleaned data</t>
   </si>
   <si>
-    <t>Data management assignment (DM file)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 8 (30min - 1hr)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 7 (30min - 1hr)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 9 (30min - 1hr)</t>
-  </si>
-  <si>
-    <t>Bivariate graphing assignment</t>
-  </si>
-  <si>
-    <t>Exam on collecting and describing data (Ch 1 &amp; 2)</t>
-  </si>
-  <si>
     <t>dplyr
 video focuses on recoding, skip patterns and missing data</t>
   </si>
@@ -273,23 +149,6 @@
     <t>Data visualization lab - bivariate portion</t>
   </si>
   <si>
-    <t>Discuss structure of exam
-* Finish all remaining assignments</t>
-  </si>
-  <si>
-    <t>Exam logistics
-* Open work time</t>
-  </si>
-  <si>
-    <t>Open work time</t>
-  </si>
-  <si>
-    <t>multiple regression, indicator variables</t>
-  </si>
-  <si>
-    <t>Review research plan</t>
-  </si>
-  <si>
     <t>Distributions Ch  3</t>
   </si>
   <si>
@@ -300,56 +159,22 @@
 * Assessing Normality</t>
   </si>
   <si>
-    <t>data camp intro to inference</t>
-  </si>
-  <si>
     <t>LLN CLT</t>
   </si>
   <si>
     <t>Confidence intervals</t>
   </si>
   <si>
-    <t>Hypothesis testing</t>
-  </si>
-  <si>
     <t>confidence intervals (4.5, 4.6)</t>
   </si>
   <si>
     <t>Using R for hypothesis testing</t>
   </si>
   <si>
-    <t>R chapter 11 is anova</t>
-  </si>
-  <si>
-    <t>R chapter 12 is chi square</t>
-  </si>
-  <si>
-    <t>How to choose appropriate analyses</t>
-  </si>
-  <si>
-    <t>Comparing means between groups</t>
-  </si>
-  <si>
-    <t>Two sample inference - independent</t>
-  </si>
-  <si>
-    <t>Linear regression and correlation</t>
-  </si>
-  <si>
     <t>presentations</t>
   </si>
   <si>
-    <t>Exam review 
-Next steps</t>
-  </si>
-  <si>
     <t>project work time</t>
-  </si>
-  <si>
-    <t>Watch PDS video 11</t>
-  </si>
-  <si>
-    <t>Watch PDS video 12</t>
   </si>
   <si>
     <t>Hypothesis testing (4.8)</t>
@@ -360,10 +185,6 @@
 * Import data into R</t>
   </si>
   <si>
-    <t>* Learn how to read and create a codebook
-* Import the Add Health data into R</t>
-  </si>
-  <si>
     <t>readxl</t>
   </si>
   <si>
@@ -371,39 +192,27 @@
 </t>
   </si>
   <si>
-    <t>Watch the R Markdown [Tutorial](http://rmarkdown.rstudio.com/lesson-1.html) by R Studio
-* Install necessary packages for the course</t>
-  </si>
-  <si>
-    <t>* Personal Codebook / Research question assignment (Due 9/3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get your computer ready for analysis
-* Download the Add Health codebook </t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
     <t>before</t>
   </si>
   <si>
-    <t>PS 2.8, 2.10</t>
-  </si>
-  <si>
-    <t>R Markdown test file (Due 8/23)
-* HW 1 (Due 8/27)</t>
-  </si>
-  <si>
-    <t>Watch PDS video 1 (6 min) (Due 8/23)
-* Read Nature paper (Due 8/25)
-* DC: Intro to R - Basic Building Blocks (Due 8/27)
-* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
-* Metacognition Inventory  (Due 8/27)
-* Read Learning - Your first job paper (Due 8/27)</t>
-  </si>
-  <si>
     <t>PS 2.4, 2.5 (Due 9/10)</t>
+  </si>
+  <si>
+    <t>* RAT on data management
+* Lab on `dplyr`
+* Create a DM file for Add Health
+* Save an analysis data set to work with</t>
+  </si>
+  <si>
+    <t>RAT on CN 2.4 (bivariate)
+* Answer questions about CN 2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Data viz tutorial website](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
+</t>
   </si>
   <si>
     <r>
@@ -417,12 +226,164 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* Data prep lecture notes</t>
+      <t>* [[Data prep]](https://norcalbiostat.github.io/MATH615/docs/lec02_data_prep.html) lecture notes
+* [[dplyr lab]](https://norcalbiostat.github.io/MATH130/materials/day78-data-manipulation.html)</t>
     </r>
   </si>
   <si>
-    <t>Univariate graphing assignment
-* Peer review assignment</t>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Indicator variables and contrasts</t>
+  </si>
+  <si>
+    <t>Watch OI [[Video]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=NVbPE1_Cbx8) on HT and DE (8 min)</t>
+  </si>
+  <si>
+    <t>Watch OI video on the [[Normal Distribution]](https://www.youtube.com/watch?list=PLkIselvEzpM6V9h55s0l9Kzivih9BUWeW&amp;v=S_p5D-YXLS4) (20 min) and [[Assessing Normality]](https://www.youtube.com/watch?v=smJBsZ4YQZw&amp;index=2&amp;list=PLkIselvEzpM6V9h55s0l9Kzivih9BUWeW) (10 min)</t>
+  </si>
+  <si>
+    <t>Watch PDS video 11 (30 min)</t>
+  </si>
+  <si>
+    <t>Watch PDS video 12 (28 min)</t>
+  </si>
+  <si>
+    <t>Watch PDS video 14 (21 min)</t>
+  </si>
+  <si>
+    <t>Watch PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
+  </si>
+  <si>
+    <t>Watch OI [[Video]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=FUaXoKdCre4) (6 min)</t>
+  </si>
+  <si>
+    <t>PDS Video 4 (8 min)
+* Read: How to read a journal article</t>
+  </si>
+  <si>
+    <t>Read and create a codebook
+* Import the Add Health data into R</t>
+  </si>
+  <si>
+    <t>[Week 5 overview](wk05.html)</t>
+  </si>
+  <si>
+    <t>[Week 6 overview](wk06.html)</t>
+  </si>
+  <si>
+    <t>[Week 7 overview](wk07.html)</t>
+  </si>
+  <si>
+    <t>[Week 8 overview](wk08.html)</t>
+  </si>
+  <si>
+    <t>[Week 9 overview](wk09.html)</t>
+  </si>
+  <si>
+    <t>[Week 10 overview](wk10.html)</t>
+  </si>
+  <si>
+    <t>[Week 11 overview](wk11.html)</t>
+  </si>
+  <si>
+    <t>[Week 13 overview](wk13.html)</t>
+  </si>
+  <si>
+    <t>Presentations</t>
+  </si>
+  <si>
+    <t>Watch OI Video on [[conditions for ANOVA]](https://www.coursera.org/learn/inferential-statistics-intro/lecture/hSgp3/conditions-for-anova) (3 min)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 10 (30 min)
+* Watch OI Video on the [[CLT]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=lsCc_pS3O28) (5 min)</t>
+  </si>
+  <si>
+    <t>Regression Assigment (Due 11/17)</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment (Due 9/24)</t>
+  </si>
+  <si>
+    <t>PS 2.8, 2.10 (Due 9/24)</t>
+  </si>
+  <si>
+    <t>Data management assignment (DM file) (Due 9/17)</t>
+  </si>
+  <si>
+    <t>[Week 1 overview](wk01.html)
+* metacognition paper, inventory
+* Learning - Your first job
+* Nature: Path to better science in less time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+* Install necessary packages for the course</t>
+  </si>
+  <si>
+    <t>Class logistic FAQ,  R Studio</t>
+  </si>
+  <si>
+    <t>Medical Records Assignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R Markdown test file (Due 8/23)
+</t>
+  </si>
+  <si>
+    <t>HW 1 (Due 8/27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get your computer ready for analysis 
+* Watch the R Markdown [Tutorial](http://rmarkdown.rstudio.com/lesson-1.html) by R Studio
+</t>
+  </si>
+  <si>
+    <t>Data analysis life cycle
+* Add Health data</t>
+  </si>
+  <si>
+    <t>Reproducible research using open source tools.</t>
+  </si>
+  <si>
+    <t>PDS Intro section
+* Add Health codebook</t>
+  </si>
+  <si>
+    <t>Software overview</t>
+  </si>
+  <si>
+    <t>RAT on Class logistics
+* Learn about the Add Health data
+* Form analysis pairs</t>
+  </si>
+  <si>
+    <t>Write down questions about class logistics and structure
+* Form support groups
+* Learn how to use Rstudio and how to turn in Homework</t>
+  </si>
+  <si>
+    <t>Drop in question time. 
+10am class go see an eclipse!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Watch the introduction video 
+* Acquire course materials
+* Sign up for data camp, Google Group. 
+* Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
+</t>
+  </si>
+  <si>
+    <t>* Read Nature paper (Due 8/23)
+* DC: Intro to R - Basic Building Blocks (Due 8/27)
+* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
+* Metacognition Inventory  (Due 8/27)
+* Read Learning - Your first job paper (Due 8/27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch PDS video 1 (6 min) (Due 8/23)
+* Download the Add Health codebook </t>
   </si>
   <si>
     <r>
@@ -432,41 +393,247 @@
     <r>
       <rPr>
         <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* Answer DM steps for ad health  (9/10)</t>
+      <t>* DM Prep questions (9/10)</t>
     </r>
   </si>
   <si>
-    <t>Watch PDS Video 6 (30min - 1hr)</t>
-  </si>
-  <si>
-    <t>Citation assignment (Due 9/10)
-* Data Camp: Intro to ggplot (Due 9/5)</t>
-  </si>
-  <si>
-    <t>* RAT on data management
-* Lab on `dplyr`
-* Create a DM file for Add Health
-* Save an analysis data set to work with</t>
-  </si>
-  <si>
-    <t>RAT on CN 2.4 (bivariate)
-* Answer questions about CN 2.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acquire course materials
-* Sign up for data camp, Google Group. 
-* Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
+    <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
 </t>
+  </si>
+  <si>
+    <t>Personal Codebook / Research question assignment (Due 9/5)</t>
+  </si>
+  <si>
+    <t>Research plan outline (Due 9/22)</t>
+  </si>
+  <si>
+    <t>RAT on CN 2.2, APA citation styles
+* Answer questions in CN 2.2</t>
+  </si>
+  <si>
+    <t>Writing about Empirical Research</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data Camp: Intro to ggplot (Due 9/5)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Citation assignment (Due 9/10)</t>
+    </r>
+  </si>
+  <si>
+    <t>Kristel week 5</t>
+  </si>
+  <si>
+    <t>Start the research plan outline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read PDS Chapter 5 </t>
+  </si>
+  <si>
+    <t>The T distribution
+* Hypothesis testing</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 17 (1 hr)
+* Read PDS Chapter 17</t>
+  </si>
+  <si>
+    <t>[Week 12 overview](wk12.html)
+* CN Chapter 8</t>
+  </si>
+  <si>
+    <t>Watch Video on [Preparing your final project](https://www.youtube.com/watch?v=NjPWVbXdRuo&amp;list=PLDEF0B9CBD27AD37E&amp;index=49) (13 min)
+* Read PDS Chapter 18</t>
+  </si>
+  <si>
+    <t>Poster Prep III (Due11/17)</t>
+  </si>
+  <si>
+    <t>Analysis &amp; Poster work</t>
+  </si>
+  <si>
+    <t>Build your poster</t>
+  </si>
+  <si>
+    <t>Poster Prep II (Due 11/3)</t>
+  </si>
+  <si>
+    <t>Multiple Regression
+* Confounding</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Finish remaining assignments</t>
+  </si>
+  <si>
+    <t>I won't be here</t>
+  </si>
+  <si>
+    <t>Finish all remaining graphics assignments</t>
+  </si>
+  <si>
+    <t>Research Plan Introduction</t>
+  </si>
+  <si>
+    <t>Start Research plan</t>
+  </si>
+  <si>
+    <t>Research Plan (Due 10/6)
+* Poster Prep I (Due 10/15)</t>
+  </si>
+  <si>
+    <t>Moderation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderation Assignment Due (10/29)
+</t>
+  </si>
+  <si>
+    <t>Chi Square Assignment Due (10/27)</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation Assignment (Due 11/5)
+</t>
+  </si>
+  <si>
+    <t>Error Analysis Due 10/27</t>
+  </si>
+  <si>
+    <t>Error Analysis Due 10/6</t>
+  </si>
+  <si>
+    <t>Types of Bias (Ch 1)</t>
+  </si>
+  <si>
+    <t>Final version of poster (Due 12/3)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 8 (30min)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 7 (30min)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 6 (30min)</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 9 (30min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam 1 </t>
+  </si>
+  <si>
+    <t>Exam 2</t>
+  </si>
+  <si>
+    <t>Exam on Ch 3-5</t>
+  </si>
+  <si>
+    <t>Exam on Ch 2</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t>Exam on Weeks 9-12</t>
+  </si>
+  <si>
+    <t>PS 3.1, 3.2 (Due 10/1)</t>
+  </si>
+  <si>
+    <t>PS 7.1, 7.3 (Due 11/5)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ANOVA Assignment (Due 10/22)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+* PS 6.6  (Due 10/22)</t>
+    </r>
+  </si>
+  <si>
+    <t>Data Camp: Foundations for Inference: Sampling Distributions (Due 10/12)
+* PS 4.1, 4.2 (Due 10/12)</t>
+  </si>
+  <si>
+    <t>Data Camp: Foundations for Inference: Confidence Intervals (Due 10/12)
+PS 4.4 (Due 10/12)</t>
+  </si>
+  <si>
+    <t>PS 4.7, 4.8 (10/12)</t>
+  </si>
+  <si>
+    <t>PDS video 4 - post personal codebook, talks about lit review
+use kristel ch4 notes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medical Records Assignment (Due 8/30)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+* PS 2.2 (Due 9/3) 
+* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
+* Complete both corresponding BBL quizzes (Due 9/3)
+</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -552,7 +719,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,7 +746,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,7 +866,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -773,10 +946,52 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -848,8 +1063,8 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1185,11 +1400,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1205,9 +1421,9 @@
     <col min="10" max="10" width="64.125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -1222,26 +1438,26 @@
         <v>2</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="126" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="41">
         <v>41506</v>
       </c>
       <c r="C2" s="3" t="str">
@@ -1249,27 +1465,27 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="41">
         <f>B2+2</f>
         <v>41508</v>
       </c>
@@ -1278,30 +1494,30 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="28">
+      <c r="B4" s="42">
         <f>B3+2</f>
         <v>41510</v>
       </c>
@@ -1310,29 +1526,29 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>44</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="H4" s="8" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="41">
         <f t="shared" ref="B5:B41" si="1">B2+7</f>
         <v>41513</v>
       </c>
@@ -1341,27 +1557,27 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="27">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="41">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
@@ -1370,27 +1586,27 @@
         <v>Wed</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="J6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="30" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="28">
+      <c r="B7" s="42">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
@@ -1399,33 +1615,34 @@
         <v>Fri</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="41">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
@@ -1434,7 +1651,7 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
@@ -1443,8 +1660,8 @@
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="27">
+    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="41">
         <f t="shared" si="1"/>
         <v>41522</v>
       </c>
@@ -1453,27 +1670,25 @@
         <v>Wed</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>45</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F9" s="14"/>
       <c r="G9" s="4" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="28">
+      <c r="B10" s="42">
         <f t="shared" si="1"/>
         <v>41524</v>
       </c>
@@ -1482,24 +1697,26 @@
         <v>Fri</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="15"/>
+        <v>11</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>A8+1</f>
         <v>4</v>
@@ -1513,26 +1730,26 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f>B9+7</f>
         <v>41529</v>
@@ -1542,26 +1759,26 @@
         <v>Wed</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6">
         <f>B10+7</f>
@@ -1572,20 +1789,24 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>A11+1</f>
         <v>5</v>
@@ -1599,23 +1820,26 @@
         <v>Mon</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E14" s="14">
         <v>2.4</v>
       </c>
       <c r="F14" s="14"/>
+      <c r="G14" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="H14" s="4" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <f t="shared" si="1"/>
         <v>41536</v>
@@ -1624,24 +1848,25 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D15" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6">
         <f t="shared" si="1"/>
@@ -1651,19 +1876,19 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="8"/>
+      <c r="D16" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1678,13 +1903,19 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
+      <c r="D17" s="33" t="s">
+        <v>125</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
+      <c r="G17" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="I17" s="4" t="s">
-        <v>68</v>
+        <v>126</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1696,16 +1927,19 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>77</v>
+      <c r="D18" s="34" t="s">
+        <v>142</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
-      <c r="J18" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="I18" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J18" s="40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6">
         <f t="shared" si="1"/>
@@ -1716,18 +1950,22 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f>A17+1</f>
         <v>7</v>
@@ -1741,16 +1979,23 @@
         <v>Mon</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <f t="shared" si="1"/>
         <v>41550</v>
@@ -1760,16 +2005,20 @@
         <v>Wed</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="H21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6">
         <f t="shared" si="1"/>
@@ -1780,18 +2029,20 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>9</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F22" s="15"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="J22" s="8" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1807,14 +2058,18 @@
         <v>Mon</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G23" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <f t="shared" si="1"/>
         <v>41557</v>
@@ -1823,15 +2078,10 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="E24" s="14"/>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6">
         <f t="shared" si="1"/>
@@ -1841,19 +2091,21 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>91</v>
-      </c>
+      <c r="D25" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>A23+1</f>
         <v>9</v>
@@ -1866,17 +2118,22 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>87</v>
+      <c r="D26" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <f t="shared" si="1"/>
         <v>41564</v>
@@ -1885,10 +2142,11 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E27" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="E27" s="14"/>
       <c r="F27" s="14"/>
+      <c r="H27" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
@@ -1900,19 +2158,19 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>88</v>
-      </c>
+      <c r="D28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="J28" s="31" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -1927,10 +2185,20 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>92</v>
-      </c>
+      <c r="D29" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="14"/>
       <c r="F29" s="14"/>
+      <c r="G29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
@@ -1941,8 +2209,14 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
+      <c r="D30" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
+      <c r="J30" s="40" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
@@ -1954,7 +2228,9 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="8"/>
@@ -1962,7 +2238,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>A29+1</f>
         <v>11</v>
@@ -1975,10 +2251,20 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="D32" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="H32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" s="30" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
@@ -2002,15 +2288,19 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f>A32+1</f>
         <v>12</v>
@@ -2023,12 +2313,22 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>52</v>
-      </c>
+      <c r="D35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="14"/>
       <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G35" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J35" s="30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <f t="shared" si="1"/>
         <v>41585</v>
@@ -2036,6 +2336,9 @@
       <c r="C36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -2050,7 +2353,9 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="8"/>
@@ -2071,8 +2376,14 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
+      <c r="D38" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
+      <c r="G38" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
@@ -2083,9 +2394,7 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="E39" s="14" t="s">
-        <v>95</v>
-      </c>
+      <c r="E39" s="14"/>
       <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2098,13 +2407,15 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D40" s="8"/>
+      <c r="D40" s="29"/>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
+      <c r="J40" s="31" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
@@ -2123,7 +2434,7 @@
       <c r="I41" s="21"/>
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>14</v>
       </c>
@@ -2135,8 +2446,14 @@
         <f t="shared" ref="C42:C47" si="2">TEXT(WEEKDAY(B42,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
+      <c r="D42" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
+      <c r="H42" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
@@ -2148,7 +2465,7 @@
         <v>Wed</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="F43" s="14"/>
     </row>
@@ -2168,7 +2485,9 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="J44" s="8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
@@ -2183,8 +2502,11 @@
         <f t="shared" si="2"/>
         <v>Mon</v>
       </c>
+      <c r="D45" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E45" s="14" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="F45" s="14"/>
     </row>
@@ -2197,10 +2519,13 @@
         <f t="shared" si="2"/>
         <v>Wed</v>
       </c>
+      <c r="D46" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
     </row>
-    <row r="47" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="6">
         <f>B44+7</f>
@@ -2210,10 +2535,10 @@
         <f t="shared" si="2"/>
         <v>Fri</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="15" t="s">
-        <v>94</v>
-      </c>
+      <c r="D47" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -2226,11 +2551,14 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="4" t="s">
-        <v>14</v>
+      <c r="D48" s="27" t="s">
+        <v>146</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
+      <c r="I48" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add holiday to schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="159">
   <si>
     <t>date</t>
   </si>
@@ -480,9 +480,6 @@
   </si>
   <si>
     <t>Finish remaining assignments</t>
-  </si>
-  <si>
-    <t>I won't be here</t>
   </si>
   <si>
     <t>Finish all remaining graphics assignments</t>
@@ -628,6 +625,20 @@
 * Complete both corresponding BBL quizzes (Due 9/3)
 </t>
     </r>
+  </si>
+  <si>
+    <t>could take an entire class period</t>
+  </si>
+  <si>
+    <t>No Class - Holiday</t>
+  </si>
+  <si>
+    <t>data viz lab
+Edward cover 10am class</t>
+  </si>
+  <si>
+    <t>I won't be here
+Edward cover 10am class</t>
   </si>
 </sst>
 </file>
@@ -1404,8 +1415,8 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1573,7 +1584,7 @@
         <v>88</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1621,7 +1632,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>51</v>
@@ -1707,7 +1718,7 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>31</v>
@@ -1740,7 +1751,7 @@
         <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>55</v>
@@ -1769,7 +1780,7 @@
         <v>57</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>37</v>
@@ -1830,7 +1841,7 @@
         <v>70</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>56</v>
@@ -1853,7 +1864,7 @@
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="G15" s="35" t="s">
         <v>57</v>
@@ -1881,12 +1892,12 @@
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J16" s="38"/>
     </row>
@@ -1904,7 +1915,7 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1912,10 +1923,10 @@
         <v>71</v>
       </c>
       <c r="I17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1928,15 +1939,15 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1962,7 +1973,7 @@
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -1992,7 +2003,7 @@
         <v>80</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2015,7 +2026,7 @@
         <v>67</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2041,7 +2052,7 @@
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2092,17 +2103,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2130,7 +2141,7 @@
         <v>63</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2169,7 +2180,7 @@
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2186,7 +2197,7 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -2197,7 +2208,7 @@
         <v>65</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2210,12 +2221,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2252,7 +2263,7 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -2263,7 +2274,7 @@
         <v>66</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2340,7 +2351,9 @@
       <c r="D36" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="14"/>
+      <c r="E36" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2354,7 +2367,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -2377,7 +2390,7 @@
         <v>Mon</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -2393,6 +2406,9 @@
       <c r="C39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2486,7 +2502,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2536,7 +2552,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2552,12 +2568,12 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add med records fix schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="167">
   <si>
     <t>date</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Regression Assigment (Due 11/17)</t>
   </si>
   <si>
-    <t>Bivariate graphing assignment (Due 9/24)</t>
-  </si>
-  <si>
     <t>PS 2.8, 2.10 (Due 9/24)</t>
   </si>
   <si>
@@ -323,9 +320,6 @@
   </si>
   <si>
     <t>Class logistic FAQ,  R Studio</t>
-  </si>
-  <si>
-    <t>Medical Records Assignment</t>
   </si>
   <si>
     <t xml:space="preserve">R Markdown test file (Due 8/23)
@@ -446,16 +440,10 @@
 * Read PDS Chapter 18</t>
   </si>
   <si>
-    <t>Poster Prep III (Due11/17)</t>
-  </si>
-  <si>
     <t>Analysis &amp; Poster work</t>
   </si>
   <si>
     <t>Build your poster</t>
-  </si>
-  <si>
-    <t>Poster Prep II (Due 11/3)</t>
   </si>
   <si>
     <t>Multiple Regression
@@ -477,30 +465,15 @@
     <t>Start Research plan</t>
   </si>
   <si>
-    <t>Research Plan (Due 10/6)
-* Poster Prep I (Due 10/15)</t>
-  </si>
-  <si>
     <t>Moderation</t>
   </si>
   <si>
-    <t xml:space="preserve">Moderation Assignment Due (10/29)
-</t>
-  </si>
-  <si>
-    <t>Chi Square Assignment Due (10/27)</t>
-  </si>
-  <si>
     <t>Correlation</t>
   </si>
   <si>
     <t>Linear Regression</t>
   </si>
   <si>
-    <t xml:space="preserve">Correlation Assignment (Due 11/5)
-</t>
-  </si>
-  <si>
     <t>Error Analysis Due 10/27</t>
   </si>
   <si>
@@ -544,9 +517,6 @@
   </si>
   <si>
     <t>PS 3.1, 3.2 (Due 10/1)</t>
-  </si>
-  <si>
-    <t>PS 7.1, 7.3 (Due 11/5)</t>
   </si>
   <si>
     <r>
@@ -572,45 +542,8 @@
     </r>
   </si>
   <si>
-    <t>Data Camp: Foundations for Inference: Sampling Distributions (Due 10/12)
-* PS 4.1, 4.2 (Due 10/12)</t>
-  </si>
-  <si>
-    <t>Data Camp: Foundations for Inference: Confidence Intervals (Due 10/12)
-PS 4.4 (Due 10/12)</t>
-  </si>
-  <si>
-    <t>PS 4.7, 4.8 (10/12)</t>
-  </si>
-  <si>
     <t>PDS video 4 - post personal codebook, talks about lit review
 use kristel ch4 notes</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Medical Records Assignment (Due 8/30)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-* PS 2.2 (Due 9/3) 
-* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
-* Complete both corresponding BBL quizzes (Due 9/3)
-</t>
-    </r>
   </si>
   <si>
     <t>could take an entire class period</t>
@@ -639,6 +572,84 @@
 * Sign up for data camp, Google Group. 
 * Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS 2.2 (Due 9/3) 
+* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
+* Complete both corresponding BBL quizzes (Due 9/3)
+</t>
+  </si>
+  <si>
+    <t>RAT on data types 
+* Medical Records Assignment</t>
+  </si>
+  <si>
+    <t>RAT: CN 4.1-4.4</t>
+  </si>
+  <si>
+    <t>PS 4.7, 4.8 (10/8)</t>
+  </si>
+  <si>
+    <t>Data Camp: Foundations for Inference: Sampling Distributions (Due 10/3)
+* PS 4.1, 4.2 (Due 10/3)</t>
+  </si>
+  <si>
+    <t>Data Camp: Foundations for Inference: Confidence Intervals (Due 10/5)
+PS 4.4 (Due 10/5)</t>
+  </si>
+  <si>
+    <t>Chi-Squared Assignment (Due 10/27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation Assignment (Due 10/29)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderation Assignment Due (11/5)
+</t>
+  </si>
+  <si>
+    <t>RAT: Multiple Regression</t>
+  </si>
+  <si>
+    <t>RAT: Moderation</t>
+  </si>
+  <si>
+    <t>RAT: Correlation</t>
+  </si>
+  <si>
+    <t>RAT: ANOVA</t>
+  </si>
+  <si>
+    <t>Build your own exam questions (Due 12/6)</t>
+  </si>
+  <si>
+    <t>Post assessment in R 
+* Post Metacognition Assessment</t>
+  </si>
+  <si>
+    <t>RAT: Logistic Regression</t>
+  </si>
+  <si>
+    <t>PS 7.1, 7.3 (Due 10/29)
+* DC Correlation and Regression</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment (Due 9/24)
+* Peer Review of this assignment (Due 10/1)</t>
+  </si>
+  <si>
+    <t>Research Plan (Due 10/6)
+* Poster Prep I (Due 10/15)
+* Peer Review Poster Prep 1 (Due 10/20)</t>
+  </si>
+  <si>
+    <t>Poster Prep III (Due 11/17)
+* Peer Review PPIII (Due 11/29)</t>
+  </si>
+  <si>
+    <t>Poster Prep II (Due 11/3)
+* Peer Review PPII (Due 11/9)</t>
   </si>
 </sst>
 </file>
@@ -877,7 +888,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1004,6 +1015,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1414,9 +1428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1439,7 @@
     <col min="2" max="2" width="10.875" style="1"/>
     <col min="3" max="3" width="4.375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="4" customWidth="1"/>
-    <col min="5" max="6" width="26" style="10" customWidth="1"/>
+    <col min="5" max="6" width="26" style="10" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="34.125" style="4" customWidth="1"/>
     <col min="8" max="8" width="35.25" style="4" customWidth="1"/>
     <col min="9" max="9" width="31.25" style="4" customWidth="1"/>
@@ -1483,16 +1497,16 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1505,25 +1519,25 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1537,24 +1551,24 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="J4" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -1581,10 +1595,10 @@
         <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1606,13 +1620,13 @@
         <v>50</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>69</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1632,7 +1646,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>51</v>
@@ -1644,7 +1658,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K7" s="32"/>
     </row>
@@ -1691,7 +1705,7 @@
         <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>54</v>
@@ -1718,13 +1732,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
@@ -1751,13 +1765,13 @@
         <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>55</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1780,13 +1794,13 @@
         <v>57</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1800,21 +1814,21 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>107</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1841,13 +1855,13 @@
         <v>70</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>56</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1864,7 +1878,7 @@
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G15" s="35" t="s">
         <v>57</v>
@@ -1874,7 +1888,7 @@
         <v>38</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1888,20 +1902,20 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J16" s="38"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>A14+1</f>
         <v>6</v>
@@ -1915,7 +1929,7 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1923,10 +1937,10 @@
         <v>71</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1939,15 +1953,15 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1973,7 +1987,7 @@
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2002,8 +2016,11 @@
       <c r="H20" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="I20" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="J20" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2026,7 +2043,7 @@
         <v>67</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2040,7 +2057,7 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>48</v>
@@ -2052,7 +2069,7 @@
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2103,17 +2120,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2130,7 +2147,7 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -2140,8 +2157,11 @@
       <c r="H26" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="I26" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="J26" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2180,7 +2200,7 @@
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2197,7 +2217,7 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -2207,11 +2227,14 @@
       <c r="H29" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="I29" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="J29" s="30" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <f t="shared" si="1"/>
         <v>41571</v>
@@ -2221,12 +2244,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="40" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2240,7 +2263,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2263,7 +2286,7 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -2273,8 +2296,11 @@
       <c r="H32" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="I32" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="J32" s="30" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2289,7 +2315,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="6">
         <f t="shared" si="1"/>
@@ -2300,7 +2326,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2308,7 +2334,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2325,15 +2351,18 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>81</v>
@@ -2352,7 +2381,7 @@
         <v>60</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="F36" s="14"/>
     </row>
@@ -2367,7 +2396,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -2397,6 +2426,9 @@
       <c r="G38" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="I38" s="4" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
@@ -2408,12 +2440,12 @@
         <v>Wed</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="6">
         <f t="shared" si="1"/>
@@ -2430,7 +2462,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="31" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2463,12 +2495,12 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="H42" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2502,7 +2534,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2540,6 +2572,9 @@
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
+      <c r="J46" s="4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
@@ -2552,7 +2587,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2568,16 +2603,19 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix links, add you tube link to intro video
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -309,12 +309,6 @@
     <t>Data management assignment (DM file) (Due 9/17)</t>
   </si>
   <si>
-    <t>[Week 1 overview](wk01.html)
-* metacognition paper, inventory
-* Learning - Your first job
-* Nature: Path to better science in less time</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 * Install necessary packages for the course</t>
   </si>
@@ -650,6 +644,10 @@
   <si>
     <t>Poster Prep II (Due 11/3)
 * Peer Review PPII (Due 11/9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 1 overview](wk01.html)
+</t>
   </si>
 </sst>
 </file>
@@ -1429,8 +1427,8 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1497,16 +1495,16 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1519,25 +1517,25 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1551,21 +1549,21 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1595,10 +1593,10 @@
         <v>20</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1620,13 +1618,13 @@
         <v>50</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>69</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1646,7 +1644,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>51</v>
@@ -1658,7 +1656,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K7" s="32"/>
     </row>
@@ -1705,7 +1703,7 @@
         <v>33</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>54</v>
@@ -1732,13 +1730,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
@@ -1765,7 +1763,7 @@
         <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>55</v>
@@ -1794,13 +1792,13 @@
         <v>57</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1814,21 +1812,21 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1855,7 +1853,7 @@
         <v>70</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>56</v>
@@ -1878,7 +1876,7 @@
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G15" s="35" t="s">
         <v>57</v>
@@ -1888,7 +1886,7 @@
         <v>38</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1902,16 +1900,16 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J16" s="38"/>
     </row>
@@ -1929,7 +1927,7 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1937,10 +1935,10 @@
         <v>71</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1953,15 +1951,15 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1987,7 +1985,7 @@
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2017,10 +2015,10 @@
         <v>80</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2043,7 +2041,7 @@
         <v>67</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2057,7 +2055,7 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>48</v>
@@ -2069,7 +2067,7 @@
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2120,17 +2118,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2147,7 +2145,7 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -2158,10 +2156,10 @@
         <v>63</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2200,7 +2198,7 @@
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2217,7 +2215,7 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -2228,10 +2226,10 @@
         <v>65</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2244,12 +2242,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2263,7 +2261,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2286,7 +2284,7 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -2297,10 +2295,10 @@
         <v>66</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2326,7 +2324,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2334,7 +2332,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2351,18 +2349,18 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>81</v>
@@ -2381,7 +2379,7 @@
         <v>60</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F36" s="14"/>
     </row>
@@ -2396,7 +2394,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -2427,7 +2425,7 @@
         <v>77</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2440,7 +2438,7 @@
         <v>Wed</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2462,7 +2460,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2495,12 +2493,12 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="H42" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2534,7 +2532,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2573,7 +2571,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="J46" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2587,7 +2585,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2603,15 +2601,15 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add OH to FAQ
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1426,9 +1426,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1437,7 @@
     <col min="2" max="2" width="10.875" style="1"/>
     <col min="3" max="3" width="4.375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="4" customWidth="1"/>
-    <col min="5" max="6" width="26" style="10" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="26" style="10" customWidth="1"/>
     <col min="7" max="7" width="34.125" style="4" customWidth="1"/>
     <col min="8" max="8" width="35.25" style="4" customWidth="1"/>
     <col min="9" max="9" width="31.25" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
fix wk1F and wk2M, rebuild. add lit review notes
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
   <si>
     <t>date</t>
   </si>
@@ -86,10 +86,6 @@
   </si>
   <si>
     <t>[Week 2 overview](wk02.html)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 2 (24 min) (Due 8/25)
-* Read Course Notes (CN) Section 2.1 and Open Intro Textbook (OI) Section 1.2</t>
   </si>
   <si>
     <t>Conducting a literature review to refine and support research questions</t>
@@ -185,20 +181,10 @@
 * Import data into R</t>
   </si>
   <si>
-    <t>readxl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to read a journal article
-</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
     <t>before</t>
-  </si>
-  <si>
-    <t>PS 2.4, 2.5 (Due 9/10)</t>
   </si>
   <si>
     <t>* RAT on data management
@@ -211,26 +197,6 @@
 * Answer questions about CN 2.4</t>
   </si>
   <si>
-    <t xml:space="preserve">[Data viz tutorial website](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[Week 4 overview](wk04.html)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* [[Data prep]](https://norcalbiostat.github.io/MATH615/docs/lec02_data_prep.html) lecture notes
-* [[dplyr lab]](https://norcalbiostat.github.io/MATH130/materials/day78-data-manipulation.html)</t>
-    </r>
-  </si>
-  <si>
     <t>Logistic Regression</t>
   </si>
   <si>
@@ -256,14 +222,6 @@
   </si>
   <si>
     <t>Watch OI [[Video]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=FUaXoKdCre4) (6 min)</t>
-  </si>
-  <si>
-    <t>PDS Video 4 (8 min)
-* Read: How to read a journal article</t>
-  </si>
-  <si>
-    <t>Read and create a codebook
-* Import the Add Health data into R</t>
   </si>
   <si>
     <t>[Week 5 overview](wk05.html)</t>
@@ -307,10 +265,6 @@
   </si>
   <si>
     <t>Data management assignment (DM file) (Due 9/17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-* Install necessary packages for the course</t>
   </si>
   <si>
     <t>Class logistic FAQ,  R Studio</t>
@@ -335,13 +289,6 @@
     <t>Reproducible research using open source tools.</t>
   </si>
   <si>
-    <t>PDS Intro section
-* Add Health codebook</t>
-  </si>
-  <si>
-    <t>Software overview</t>
-  </si>
-  <si>
     <t>RAT on Class logistics
 * Learn about the Add Health data
 * Form analysis pairs</t>
@@ -354,10 +301,6 @@
   <si>
     <t>Drop in question time. 
 10am class go see an eclipse!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch PDS video 1 (6 min) (Due 8/23)
-* Download the Add Health codebook </t>
   </si>
   <si>
     <r>
@@ -393,26 +336,7 @@
     <t>Writing about Empirical Research</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Data Camp: Intro to ggplot (Due 9/5)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* Citation assignment (Due 9/10)</t>
-    </r>
-  </si>
-  <si>
     <t>Kristel week 5</t>
-  </si>
-  <si>
-    <t>Start the research plan outline</t>
   </si>
   <si>
     <t xml:space="preserve">Read PDS Chapter 5 </t>
@@ -424,10 +348,6 @@
   <si>
     <t>Watch PDS Video 17 (1 hr)
 * Read PDS Chapter 17</t>
-  </si>
-  <si>
-    <t>[Week 12 overview](wk12.html)
-* CN Chapter 8</t>
   </si>
   <si>
     <t>Watch Video on [Preparing your final project](https://www.youtube.com/watch?v=NjPWVbXdRuo&amp;list=PLDEF0B9CBD27AD37E&amp;index=49) (13 min)
@@ -649,11 +569,50 @@
     <t xml:space="preserve">[Week 1 overview](wk01.html)
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">Download the AddHealth data into your projects folder. 
+* Read the research questions/personal codebook assignment instructions. </t>
+  </si>
+  <si>
+    <t>Import the Add Health data into R
+* Read and create a codebook for AddHealth</t>
+  </si>
+  <si>
+    <t>Citation assignment (Due 9/10)</t>
+  </si>
+  <si>
+    <t>PS 2.4, 2.5 (Due 9/10)
+* Data Camp: Intro to ggplot (Due 9/10)</t>
+  </si>
+  <si>
+    <t>Start the research plan outline
+* Open work time on DM and graphing</t>
+  </si>
+  <si>
+    <t>[Week 4 overview](wk04.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 12 overview](wk12.html)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch PDS video 1 (6 min) 
+* Download the Add Health codebook </t>
+  </si>
+  <si>
+    <t>Watch PDS Video 2 (24 min) 
+* Read Course Notes (CN) Section 2.1 and Open Intro Textbook (OI) Section 1.2</t>
+  </si>
+  <si>
+    <t>PDS Video 4 (8 min)
+* Read: How to read a journal article
+* Read lecture notes on literature reviews</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -739,7 +698,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -773,6 +732,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -886,7 +857,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1016,6 +987,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1086,8 +1066,8 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1423,12 +1403,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1461,13 +1441,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>15</v>
@@ -1480,7 +1460,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="44">
         <v>41506</v>
       </c>
       <c r="C2" s="3" t="str">
@@ -1495,20 +1475,20 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="41">
+      <c r="B3" s="44">
         <f>B2+2</f>
         <v>41508</v>
       </c>
@@ -1517,30 +1497,27 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="42">
+      <c r="B4" s="45">
         <f>B3+2</f>
         <v>41510</v>
       </c>
@@ -1549,21 +1526,19 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="8" t="s">
-        <v>91</v>
-      </c>
+      <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1571,7 +1546,7 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="46">
         <f t="shared" ref="B5:B41" si="1">B2+7</f>
         <v>41513</v>
       </c>
@@ -1583,24 +1558,24 @@
         <v>17</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="B6" s="46">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
@@ -1609,27 +1584,25 @@
         <v>Wed</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="F6" s="14"/>
       <c r="H6" s="4" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>99</v>
+        <v>153</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="42">
+      <c r="B7" s="45">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
@@ -1638,25 +1611,23 @@
         <v>Fri</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>51</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>103</v>
+        <v>23</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>154</v>
       </c>
       <c r="K7" s="32"/>
     </row>
@@ -1665,7 +1636,7 @@
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="46">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
@@ -1696,17 +1667,17 @@
         <v>10</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1726,20 +1697,20 @@
         <v>11</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>A8+1</f>
         <v>4</v>
@@ -1753,26 +1724,26 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f>B9+7</f>
         <v>41529</v>
@@ -1782,26 +1753,23 @@
         <v>Wed</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6">
         <f>B10+7</f>
@@ -1812,21 +1780,21 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1850,19 +1818,19 @@
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <f t="shared" si="1"/>
         <v>41536</v>
@@ -1872,21 +1840,19 @@
         <v>Wed</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>57</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1900,16 +1866,16 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="J16" s="38"/>
     </row>
@@ -1927,18 +1893,18 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1951,15 +1917,15 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1973,19 +1939,19 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2002,23 +1968,23 @@
         <v>Mon</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="I20" s="4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2031,17 +1997,17 @@
         <v>Wed</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="F21" s="14"/>
       <c r="H21" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2055,19 +2021,19 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2084,14 +2050,14 @@
         <v>Mon</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="J23" s="30"/>
     </row>
@@ -2118,17 +2084,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2145,21 +2111,21 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2174,7 +2140,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="H27" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2188,17 +2154,17 @@
         <v>Fri</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2215,21 +2181,21 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2242,12 +2208,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="40" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2261,7 +2227,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2284,21 +2250,21 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2324,7 +2290,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2332,7 +2298,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2349,21 +2315,21 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2376,10 +2342,10 @@
         <v>Wed</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="F36" s="14"/>
     </row>
@@ -2394,7 +2360,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -2417,15 +2383,15 @@
         <v>Mon</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2438,7 +2404,7 @@
         <v>Wed</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2460,7 +2426,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="31" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2493,12 +2459,12 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="H42" s="4" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2511,7 +2477,7 @@
         <v>Wed</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F43" s="14"/>
     </row>
@@ -2532,7 +2498,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2549,10 +2515,10 @@
         <v>Mon</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F45" s="14"/>
     </row>
@@ -2566,12 +2532,12 @@
         <v>Wed</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="J46" s="4" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2585,7 +2551,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2601,15 +2567,15 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more faq, wk3 updates.
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="163">
   <si>
     <t>date</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Creating data visualizations in R</t>
-  </si>
-  <si>
-    <t>Answer questions in CN 2.3</t>
   </si>
   <si>
     <t>install tidyverse, desr packages</t>
@@ -303,22 +300,6 @@
 10am class go see an eclipse!</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">PS 2.7 (Due 9/10)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* DM Prep questions (9/10)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
 </t>
   </si>
@@ -329,10 +310,6 @@
     <t>Research plan outline (Due 9/22)</t>
   </si>
   <si>
-    <t>RAT on CN 2.2, APA citation styles
-* Answer questions in CN 2.2</t>
-  </si>
-  <si>
     <t>Writing about Empirical Research</t>
   </si>
   <si>
@@ -404,9 +381,6 @@
   </si>
   <si>
     <t>Watch PDS Video 7 (30min)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 6 (30min)</t>
   </si>
   <si>
     <t>Watch PDS Video 9 (30min)</t>
@@ -607,6 +581,24 @@
     <t>PDS Video 4 (8 min)
 * Read: How to read a journal article
 * Read lecture notes on literature reviews</t>
+  </si>
+  <si>
+    <t>Read CN Section 2.2</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 6 (30min)
+* Read CN Section 2.3</t>
+  </si>
+  <si>
+    <t>RAT on CN 2.2, APA citation styles
+* Discussion examples in CN 2.2</t>
+  </si>
+  <si>
+    <t>Discuss examples in CN 2.3</t>
+  </si>
+  <si>
+    <t>PS 2.7 (Due 9/10)
+* DM Prep questions (9/10)</t>
   </si>
 </sst>
 </file>
@@ -857,7 +849,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -978,12 +970,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1407,8 +1393,8 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1444,10 +1430,10 @@
         <v>26</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>15</v>
@@ -1460,7 +1446,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="42">
         <v>41506</v>
       </c>
       <c r="C2" s="3" t="str">
@@ -1475,20 +1461,20 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="44">
+      <c r="B3" s="42">
         <f>B2+2</f>
         <v>41508</v>
       </c>
@@ -1497,27 +1483,27 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="45">
+      <c r="B4" s="43">
         <f>B3+2</f>
         <v>41510</v>
       </c>
@@ -1526,19 +1512,19 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="43" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1546,7 +1532,7 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="44">
         <f t="shared" ref="B5:B41" si="1">B2+7</f>
         <v>41513</v>
       </c>
@@ -1565,17 +1551,17 @@
         <v>19</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
+      <c r="B6" s="44">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
@@ -1584,25 +1570,25 @@
         <v>Wed</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="14"/>
       <c r="H6" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="45">
+      <c r="B7" s="43">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
@@ -1617,17 +1603,17 @@
         <v>21</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="43" t="s">
-        <v>154</v>
+      <c r="J7" s="41" t="s">
+        <v>150</v>
       </c>
       <c r="K7" s="32"/>
     </row>
@@ -1636,7 +1622,7 @@
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="44">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
@@ -1655,7 +1641,7 @@
       <c r="J8" s="25"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="41">
+      <c r="B9" s="44">
         <f t="shared" si="1"/>
         <v>41522</v>
       </c>
@@ -1671,18 +1657,21 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="42">
+      <c r="B10" s="43">
         <f t="shared" si="1"/>
         <v>41524</v>
       </c>
@@ -1701,13 +1690,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>85</v>
+        <v>161</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1724,23 +1713,23 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1760,13 +1749,13 @@
         <v>28</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1780,21 +1769,21 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1818,16 +1807,16 @@
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1840,19 +1829,19 @@
         <v>Wed</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1866,16 +1855,16 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J16" s="38"/>
     </row>
@@ -1893,18 +1882,18 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1917,15 +1906,15 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1939,19 +1928,19 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -1968,23 +1957,23 @@
         <v>Mon</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -1997,17 +1986,17 @@
         <v>Wed</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="F21" s="14"/>
       <c r="H21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2021,19 +2010,19 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2050,14 +2039,14 @@
         <v>Mon</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J23" s="30"/>
     </row>
@@ -2084,17 +2073,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2111,21 +2100,21 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2140,7 +2129,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="H27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2160,11 +2149,11 @@
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2181,21 +2170,21 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2208,12 +2197,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="40" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2227,7 +2216,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2250,21 +2239,21 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2290,7 +2279,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2298,7 +2287,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2315,21 +2304,21 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2342,10 +2331,10 @@
         <v>Wed</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F36" s="14"/>
     </row>
@@ -2360,7 +2349,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
@@ -2383,15 +2372,15 @@
         <v>Mon</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2404,7 +2393,7 @@
         <v>Wed</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2426,7 +2415,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2459,12 +2448,12 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="H42" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2477,7 +2466,7 @@
         <v>Wed</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F43" s="14"/>
     </row>
@@ -2498,7 +2487,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2515,10 +2504,10 @@
         <v>Mon</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F45" s="14"/>
     </row>
@@ -2532,12 +2521,12 @@
         <v>Wed</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="J46" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2551,7 +2540,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2567,15 +2556,15 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add week 4, rebuild
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -122,14 +122,6 @@
     <t>[Week 3 overview](wk03.html)</t>
   </si>
   <si>
-    <t>Data management
-* Raw vs cleaned data</t>
-  </si>
-  <si>
-    <t>dplyr
-video focuses on recoding, skip patterns and missing data</t>
-  </si>
-  <si>
     <t>Creating bivariate graphics in R</t>
   </si>
   <si>
@@ -181,12 +173,6 @@
     <t>before</t>
   </si>
   <si>
-    <t>* RAT on data management
-* Lab on `dplyr`
-* Create a DM file for Add Health
-* Save an analysis data set to work with</t>
-  </si>
-  <si>
     <t>RAT on CN 2.4 (bivariate)
 * Answer questions about CN 2.4</t>
   </si>
@@ -372,12 +358,6 @@
   </si>
   <si>
     <t>Final version of poster (Due 12/3)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 8 (30min)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 7 (30min)</t>
   </si>
   <si>
     <t>Watch PDS Video 9 (30min)</t>
@@ -584,10 +564,6 @@
 * Read CN Section 2.3</t>
   </si>
   <si>
-    <t>RAT on CN 2.2, APA citation styles
-* Discussion examples in CN 2.2</t>
-  </si>
-  <si>
     <t>Discuss examples in CN 2.3</t>
   </si>
   <si>
@@ -596,6 +572,30 @@
   </si>
   <si>
     <t>No Class (Holiday)</t>
+  </si>
+  <si>
+    <t>RAT on data management
+* data management with the depression data</t>
+  </si>
+  <si>
+    <t>data management
+video focuses on recoding, skip patterns and missing data</t>
+  </si>
+  <si>
+    <t>RAT on CN 2.2
+* Discussion examples in CN 2.2</t>
+  </si>
+  <si>
+    <t>Data management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch PDS Video 7 (30min)
+* Install the `ggplot2`  packages
+* Download the `dm_depress.Rmd` into your `math315/code` folder </t>
+  </si>
+  <si>
+    <t>Watch PDS Video 8 (30min)
+* Start a new RMD file - replicate all univariate plots in tutorial</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -990,6 +990,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1402,8 +1408,8 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1439,10 +1445,10 @@
         <v>25</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>14</v>
@@ -1470,16 +1476,16 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1492,22 +1498,22 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1521,19 +1527,19 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1560,13 +1566,13 @@
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1579,20 +1585,20 @@
         <v>Wed</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="14"/>
       <c r="H6" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1612,17 +1618,17 @@
         <v>20</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="41" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="K7" s="32"/>
     </row>
@@ -1640,7 +1646,7 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
@@ -1668,13 +1674,13 @@
       </c>
       <c r="F9" s="14"/>
       <c r="H9" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>158</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
@@ -1698,21 +1704,21 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>A8+1</f>
         <v>4</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="44">
         <f t="shared" si="1"/>
         <v>41527</v>
       </c>
@@ -1721,27 +1727,27 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+        <v>156</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="44">
         <f>B9+7</f>
         <v>41529</v>
       </c>
@@ -1757,18 +1763,18 @@
         <v>27</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>83</v>
+        <v>32</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="6">
+      <c r="B13" s="43">
         <f>B10+7</f>
         <v>41531</v>
       </c>
@@ -1777,21 +1783,21 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>85</v>
+        <v>145</v>
+      </c>
+      <c r="J13" s="50" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1815,16 +1821,16 @@
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1837,19 +1843,19 @@
         <v>Wed</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="36" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1863,16 +1869,16 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J16" s="38"/>
     </row>
@@ -1890,18 +1896,18 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1914,15 +1920,15 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1936,19 +1942,19 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -1965,23 +1971,23 @@
         <v>Mon</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -1994,17 +2000,17 @@
         <v>Wed</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F21" s="14"/>
       <c r="H21" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2018,19 +2024,19 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2047,14 +2053,14 @@
         <v>Mon</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J23" s="30"/>
     </row>
@@ -2081,17 +2087,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2108,21 +2114,21 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2137,7 +2143,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="H27" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2157,11 +2163,11 @@
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2178,21 +2184,21 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2205,12 +2211,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2224,7 +2230,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2247,21 +2253,21 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2287,7 +2293,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2295,7 +2301,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2312,21 +2318,21 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2339,10 +2345,10 @@
         <v>Wed</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F36" s="14"/>
     </row>
@@ -2357,7 +2363,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="47" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E37" s="48"/>
       <c r="F37" s="48"/>
@@ -2380,15 +2386,15 @@
         <v>Mon</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2401,7 +2407,7 @@
         <v>Wed</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2423,7 +2429,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="31" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2456,12 +2462,12 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="H42" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2474,7 +2480,7 @@
         <v>Wed</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F43" s="14"/>
     </row>
@@ -2495,7 +2501,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2512,10 +2518,10 @@
         <v>Mon</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F45" s="14"/>
     </row>
@@ -2529,12 +2535,12 @@
         <v>Wed</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="J46" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2548,7 +2554,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2564,15 +2570,15 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clarify research plan outline. revise schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="161">
   <si>
     <t>date</t>
   </si>
@@ -283,17 +283,7 @@
 10am class go see an eclipse!</t>
   </si>
   <si>
-    <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
-</t>
-  </si>
-  <si>
     <t>Personal Codebook / Research question assignment (Due 9/5)</t>
-  </si>
-  <si>
-    <t>Research plan outline (Due 9/22)</t>
-  </si>
-  <si>
-    <t>Writing about Empirical Research</t>
   </si>
   <si>
     <t>Kristel week 5</t>
@@ -331,9 +321,6 @@
   </si>
   <si>
     <t>Research Plan Introduction</t>
-  </si>
-  <si>
-    <t>Start Research plan</t>
   </si>
   <si>
     <t>Moderation</t>
@@ -486,15 +473,6 @@
 * DC Correlation and Regression</t>
   </si>
   <si>
-    <t>Bivariate graphing assignment (Due 9/24)
-* Peer Review of this assignment (Due 10/1)</t>
-  </si>
-  <si>
-    <t>Research Plan (Due 10/6)
-* Poster Prep I (Due 10/15)
-* Peer Review Poster Prep 1 (Due 10/20)</t>
-  </si>
-  <si>
     <t>Poster Prep III (Due 11/17)
 * Peer Review PPIII (Due 11/29)</t>
   </si>
@@ -520,10 +498,6 @@
   <si>
     <t>PS 2.4, 2.5 (Due 9/10)
 * Data Camp: Intro to ggplot (Due 9/10)</t>
-  </si>
-  <si>
-    <t>Start the research plan outline
-* Open work time on DM and graphing</t>
   </si>
   <si>
     <t>[Week 4 overview](wk04.html)</t>
@@ -595,6 +569,52 @@
   </si>
   <si>
     <t>Edward (10am), Kathy (12)</t>
+  </si>
+  <si>
+    <t>Research Plan Outline (Due 10/1)
+* Poster Prep I (Due 10/15)
+* Peer Review Poster Prep 1 (Due 10/20)</t>
+  </si>
+  <si>
+    <t>Open work time</t>
+  </si>
+  <si>
+    <t>Open work time on DM and graphing</t>
+  </si>
+  <si>
+    <t>Introduce Research plan outline
+* Prep for Exam 1</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment (Due 9/26)
+* Peer Review Biv. Graph (Due 10/1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Peer Review of this assignment (Due 9/24)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -686,7 +706,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,6 +746,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,9 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -987,6 +1010,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="69">
@@ -1399,7 +1425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1477,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="48">
+      <c r="B2" s="47">
         <v>41506</v>
       </c>
       <c r="C2" s="3" t="str">
@@ -1466,20 +1492,20 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>79</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="48">
+      <c r="B3" s="47">
         <f>B2+2</f>
         <v>41508</v>
       </c>
@@ -1508,7 +1534,7 @@
     </row>
     <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="49">
+      <c r="B4" s="48">
         <f>B3+2</f>
         <v>41510</v>
       </c>
@@ -1523,12 +1549,12 @@
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="40" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1537,7 +1563,7 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="47">
         <f t="shared" ref="B5:B41" si="1">B2+7</f>
         <v>41513</v>
       </c>
@@ -1556,17 +1582,17 @@
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="B6" s="48">
+      <c r="B6" s="47">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
@@ -1582,18 +1608,18 @@
       </c>
       <c r="F6" s="14"/>
       <c r="H6" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J6" s="40" t="s">
-        <v>81</v>
+        <v>133</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="49">
+      <c r="B7" s="48">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
@@ -1608,17 +1634,17 @@
         <v>20</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="41" t="s">
-        <v>140</v>
+      <c r="J7" s="40" t="s">
+        <v>134</v>
       </c>
       <c r="K7" s="32"/>
     </row>
@@ -1627,7 +1653,7 @@
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="47">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
@@ -1636,7 +1662,7 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
@@ -1648,7 +1674,7 @@
       <c r="J8" s="25"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="48">
+      <c r="B9" s="47">
         <f t="shared" si="1"/>
         <v>41522</v>
       </c>
@@ -1664,18 +1690,18 @@
       </c>
       <c r="F9" s="14"/>
       <c r="H9" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="J9" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="49">
+      <c r="B10" s="48">
         <f t="shared" si="1"/>
         <v>41524</v>
       </c>
@@ -1694,13 +1720,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>151</v>
+        <v>143</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1708,7 +1734,7 @@
         <f>A8+1</f>
         <v>4</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="47">
         <f t="shared" si="1"/>
         <v>41527</v>
       </c>
@@ -1717,27 +1743,27 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="J11" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="45" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="48">
+      <c r="B12" s="47">
         <f>B9+7</f>
         <v>41529</v>
       </c>
@@ -1753,18 +1779,18 @@
         <v>27</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="46" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="J12" s="45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="49">
+      <c r="B13" s="48">
         <f>B10+7</f>
         <v>41531</v>
       </c>
@@ -1773,29 +1799,25 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>159</v>
-      </c>
+      <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J13" s="47" t="s">
-        <v>82</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="J13" s="46"/>
     </row>
     <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>A11+1</f>
         <v>5</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="47">
         <f>B11+7</f>
         <v>41534</v>
       </c>
@@ -1814,7 +1836,7 @@
         <v>57</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>47</v>
@@ -1824,7 +1846,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="48">
+      <c r="B15" s="47">
         <f t="shared" si="1"/>
         <v>41536</v>
       </c>
@@ -1832,25 +1854,25 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35" t="s">
+      <c r="E15" s="35"/>
+      <c r="F15" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="37" t="s">
-        <v>133</v>
+      <c r="J15" s="36" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="49">
+      <c r="B16" s="48">
         <f t="shared" si="1"/>
         <v>41538</v>
       </c>
@@ -1858,19 +1880,19 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D16" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="J16" s="38"/>
+      <c r="D16" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1886,18 +1908,21 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="H17" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="I17" s="4" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1909,16 +1934,16 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D18" s="34" t="s">
-        <v>104</v>
+      <c r="D18" s="49" t="s">
+        <v>100</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="J18" s="40" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1944,7 +1969,7 @@
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -1974,10 +1999,10 @@
         <v>67</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2000,7 +2025,7 @@
         <v>56</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2014,7 +2039,7 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>43</v>
@@ -2026,7 +2051,7 @@
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2077,17 +2102,17 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2104,7 +2129,7 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -2115,10 +2140,10 @@
         <v>52</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2157,7 +2182,7 @@
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2174,7 +2199,7 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -2185,10 +2210,10 @@
         <v>54</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2201,12 +2226,12 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
-      <c r="J30" s="40" t="s">
-        <v>132</v>
+      <c r="J30" s="39" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2220,7 +2245,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2243,7 +2268,7 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -2254,10 +2279,10 @@
         <v>55</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2283,7 +2308,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2291,7 +2316,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2308,18 +2333,18 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>68</v>
@@ -2338,29 +2363,29 @@
         <v>49</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="42">
+      <c r="B37" s="41">
         <f t="shared" si="1"/>
         <v>41587</v>
       </c>
-      <c r="C37" s="43" t="str">
+      <c r="C37" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D37" s="44" t="s">
-        <v>152</v>
-      </c>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
+      <c r="D37" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -2384,7 +2409,7 @@
         <v>64</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2397,7 +2422,7 @@
         <v>Wed</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2419,7 +2444,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="31" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2452,12 +2477,12 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="H42" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2491,7 +2516,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2530,7 +2555,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="J46" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2544,7 +2569,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2560,15 +2585,15 @@
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="I48" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update rp outline assignment and schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="960" windowWidth="25600" windowHeight="13560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="164">
   <si>
     <t>date</t>
   </si>
@@ -82,9 +77,6 @@
     <t>Create personal codebook for add health</t>
   </si>
   <si>
-    <t>[Week 2 overview](wk02.html)</t>
-  </si>
-  <si>
     <t>Conducting a literature review to refine and support research questions</t>
   </si>
   <si>
@@ -117,9 +109,6 @@
   </si>
   <si>
     <t>install tidyverse, desr packages</t>
-  </si>
-  <si>
-    <t>[Week 3 overview](wk03.html)</t>
   </si>
   <si>
     <t>Creating bivariate graphics in R</t>
@@ -204,30 +193,6 @@
     <t>Watch OI [[Video]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=FUaXoKdCre4) (6 min)</t>
   </si>
   <si>
-    <t>[Week 5 overview](wk05.html)</t>
-  </si>
-  <si>
-    <t>[Week 6 overview](wk06.html)</t>
-  </si>
-  <si>
-    <t>[Week 7 overview](wk07.html)</t>
-  </si>
-  <si>
-    <t>[Week 8 overview](wk08.html)</t>
-  </si>
-  <si>
-    <t>[Week 9 overview](wk09.html)</t>
-  </si>
-  <si>
-    <t>[Week 10 overview](wk10.html)</t>
-  </si>
-  <si>
-    <t>[Week 11 overview](wk11.html)</t>
-  </si>
-  <si>
-    <t>[Week 13 overview](wk13.html)</t>
-  </si>
-  <si>
     <t>Presentations</t>
   </si>
   <si>
@@ -302,9 +267,6 @@
   </si>
   <si>
     <t>Analysis &amp; Poster work</t>
-  </si>
-  <si>
-    <t>Build your poster</t>
   </si>
   <si>
     <t>Multiple Regression
@@ -473,18 +435,6 @@
 * DC Correlation and Regression</t>
   </si>
   <si>
-    <t>Poster Prep III (Due 11/17)
-* Peer Review PPIII (Due 11/29)</t>
-  </si>
-  <si>
-    <t>Poster Prep II (Due 11/3)
-* Peer Review PPII (Due 11/9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 1 overview](wk01.html)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Download the AddHealth data into your projects folder. 
 * Read the research questions/personal codebook assignment instructions. </t>
   </si>
@@ -498,13 +448,6 @@
   <si>
     <t>PS 2.4, 2.5 (Due 9/10)
 * Data Camp: Intro to ggplot (Due 9/10)</t>
-  </si>
-  <si>
-    <t>[Week 4 overview](wk04.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 12 overview](wk12.html)
-</t>
   </si>
   <si>
     <t xml:space="preserve">Watch PDS video 1 (6 min) 
@@ -571,11 +514,6 @@
     <t>Edward (10am), Kathy (12)</t>
   </si>
   <si>
-    <t>Research Plan Outline (Due 10/1)
-* Poster Prep I (Due 10/15)
-* Peer Review Poster Prep 1 (Due 10/20)</t>
-  </si>
-  <si>
     <t>Open work time</t>
   </si>
   <si>
@@ -593,12 +531,78 @@
     <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
 * Peer Review of this assignment (Due 9/24)
 </t>
+  </si>
+  <si>
+    <t>Research Plan Outline (Due 10/8)
+* Poster Prep I (Due 10/15)
+* Peer Review Poster Prep 1 (Due 10/20)</t>
+  </si>
+  <si>
+    <t>Analysis and Poster work</t>
+  </si>
+  <si>
+    <t>Poster Draft (Due 11/28)
+* Peer Review Poster Draft (Due 12/1)</t>
+  </si>
+  <si>
+    <t>Poster Prep II (Due 11/12)
+* Peer Review PPII (Due 11/16)</t>
+  </si>
+  <si>
+    <t>[Finals](Finals.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 1 ](wk01.html)
+</t>
+  </si>
+  <si>
+    <t>[Week 2 ](wk02.html)</t>
+  </si>
+  <si>
+    <t>[Week 3 ](wk03.html)</t>
+  </si>
+  <si>
+    <t>[Week 4 ](wk04.html)</t>
+  </si>
+  <si>
+    <t>[Week 5 ](wk05.html)</t>
+  </si>
+  <si>
+    <t>[Week 6 ](wk06.html)</t>
+  </si>
+  <si>
+    <t>[Week 7 ](wk07.html)</t>
+  </si>
+  <si>
+    <t>[Week 8 ](wk08.html)</t>
+  </si>
+  <si>
+    <t>[Week 9 ](wk09.html)</t>
+  </si>
+  <si>
+    <t>[Week 10 ](wk10.html)</t>
+  </si>
+  <si>
+    <t>[Week 11 ](wk11.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 12 ](wk12.html)
+</t>
+  </si>
+  <si>
+    <t>[Week 13 ](wk13.html)</t>
+  </si>
+  <si>
+    <t>[Week 14 ](wk14.html)</t>
+  </si>
+  <si>
+    <t>[Week 15 ](wk15.html)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -772,7 +776,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -826,6 +830,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -993,7 +1005,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1027,6 +1039,10 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1060,9 +1076,13 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1398,28 +1418,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="1"/>
-    <col min="3" max="3" width="4.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="4" customWidth="1"/>
-    <col min="5" max="6" width="26" style="10" customWidth="1"/>
-    <col min="7" max="7" width="34.125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="35.25" style="4" customWidth="1"/>
-    <col min="9" max="9" width="31.25" style="4" customWidth="1"/>
-    <col min="10" max="10" width="64.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19" thickBot="1">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -1436,13 +1457,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>14</v>
@@ -1451,7 +1472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="120">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1470,19 +1491,19 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75">
       <c r="B3" s="47">
         <f>B2+2</f>
         <v>41508</v>
@@ -1492,25 +1513,25 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45">
       <c r="A4" s="5"/>
       <c r="B4" s="48">
         <f>B3+2</f>
@@ -1521,22 +1542,22 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="90">
       <c r="A5" s="1">
         <f>A2+1</f>
         <v>2</v>
@@ -1553,23 +1574,23 @@
         <v>16</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60">
       <c r="B6" s="47">
         <f t="shared" si="1"/>
         <v>41515</v>
@@ -1579,23 +1600,23 @@
         <v>Wed</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="14"/>
       <c r="H6" s="4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="105">
       <c r="A7" s="5"/>
       <c r="B7" s="48">
         <f t="shared" si="1"/>
@@ -1606,27 +1627,27 @@
         <v>Fri</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>20</v>
-      </c>
       <c r="F7" s="16" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="40" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <f>A5+1</f>
         <v>3</v>
@@ -1640,18 +1661,18 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="4" t="s">
-        <v>30</v>
+        <v>151</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
     </row>
-    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30">
       <c r="B9" s="47">
         <f t="shared" si="1"/>
         <v>41522</v>
@@ -1664,20 +1685,20 @@
         <v>9</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="14"/>
       <c r="H9" s="4" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="180">
       <c r="A10" s="5"/>
       <c r="B10" s="48">
         <f t="shared" si="1"/>
@@ -1694,20 +1715,20 @@
         <v>10</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="J10" s="40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="105">
       <c r="A11" s="1">
         <f>A8+1</f>
         <v>4</v>
@@ -1721,26 +1742,26 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="75">
       <c r="B12" s="47">
         <f>B9+7</f>
         <v>41529</v>
@@ -1750,23 +1771,23 @@
         <v>Wed</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30">
       <c r="A13" s="5"/>
       <c r="B13" s="48">
         <f>B10+7</f>
@@ -1777,20 +1798,20 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="J13" s="46"/>
     </row>
-    <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="30">
       <c r="A14" s="1">
         <f>A11+1</f>
         <v>5</v>
@@ -1811,19 +1832,19 @@
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="4" t="s">
-        <v>57</v>
+        <v>153</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="60">
       <c r="B15" s="47">
         <f t="shared" si="1"/>
         <v>41536</v>
@@ -1833,22 +1854,22 @@
         <v>Wed</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="35"/>
       <c r="F15" s="35" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45">
       <c r="A16" s="5"/>
       <c r="B16" s="48">
         <f t="shared" si="1"/>
@@ -1859,20 +1880,20 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="38" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="J16" s="37"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="45">
       <c r="A17" s="1">
         <f>A14+1</f>
         <v>6</v>
@@ -1886,24 +1907,24 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="4" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="B18" s="2">
         <f t="shared" si="1"/>
         <v>41543</v>
@@ -1913,18 +1934,18 @@
         <v>Wed</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="135">
       <c r="A19" s="5"/>
       <c r="B19" s="6">
         <f t="shared" si="1"/>
@@ -1935,22 +1956,22 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="75">
       <c r="A20" s="1">
         <f>A17+1</f>
         <v>7</v>
@@ -1964,26 +1985,26 @@
         <v>Mon</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="4" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60">
       <c r="B21" s="2">
         <f t="shared" si="1"/>
         <v>41550</v>
@@ -1993,20 +2014,20 @@
         <v>Wed</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="14"/>
       <c r="H21" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="75">
       <c r="A22" s="5"/>
       <c r="B22" s="6">
         <f t="shared" si="1"/>
@@ -2017,22 +2038,22 @@
         <v>Fri</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30">
       <c r="A23" s="1">
         <f>A20+1</f>
         <v>8</v>
@@ -2046,18 +2067,18 @@
         <v>Mon</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="4" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="J23" s="30"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="B24" s="2">
         <f t="shared" si="1"/>
         <v>41557</v>
@@ -2069,7 +2090,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="5"/>
       <c r="B25" s="6">
         <f t="shared" si="1"/>
@@ -2080,20 +2101,20 @@
         <v>Fri</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30">
       <c r="A26" s="1">
         <f>A23+1</f>
         <v>9</v>
@@ -2107,24 +2128,24 @@
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="4" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="75">
       <c r="B27" s="2">
         <f t="shared" si="1"/>
         <v>41564</v>
@@ -2136,10 +2157,10 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="H27" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <f t="shared" si="1"/>
@@ -2150,20 +2171,20 @@
         <v>Fri</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="31" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="1">
         <f>A26+1</f>
         <v>10</v>
@@ -2177,24 +2198,24 @@
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="4" t="s">
-        <v>62</v>
+        <v>158</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30">
       <c r="B30" s="2">
         <f t="shared" si="1"/>
         <v>41571</v>
@@ -2204,15 +2225,15 @@
         <v>Wed</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="J30" s="39" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="5"/>
       <c r="B31" s="6">
         <f t="shared" si="1"/>
@@ -2223,7 +2244,7 @@
         <v>Fri</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -2232,7 +2253,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="60">
       <c r="A32" s="1">
         <f>A29+1</f>
         <v>11</v>
@@ -2246,24 +2267,24 @@
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="4" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="B33" s="2">
         <f t="shared" si="1"/>
         <v>41578</v>
@@ -2275,7 +2296,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="30">
       <c r="A34" s="5"/>
       <c r="B34" s="6">
         <f t="shared" si="1"/>
@@ -2286,7 +2307,7 @@
         <v>Fri</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
@@ -2294,10 +2315,10 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="1">
         <f>A32+1</f>
         <v>12</v>
@@ -2311,24 +2332,24 @@
         <v>Mon</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="4" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30">
       <c r="B36" s="2">
         <f t="shared" si="1"/>
         <v>41585</v>
@@ -2338,14 +2359,14 @@
         <v>Wed</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="5"/>
       <c r="B37" s="41">
         <f t="shared" si="1"/>
@@ -2356,7 +2377,7 @@
         <v>Fri</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="E37" s="44"/>
       <c r="F37" s="44"/>
@@ -2365,7 +2386,7 @@
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <f>A35+1</f>
         <v>13</v>
@@ -2379,18 +2400,18 @@
         <v>Mon</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="4" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="B39" s="2">
         <f t="shared" si="1"/>
         <v>41592</v>
@@ -2398,14 +2419,11 @@
       <c r="C39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
     </row>
-    <row r="40" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="5"/>
       <c r="B40" s="6">
         <f t="shared" si="1"/>
@@ -2415,17 +2433,17 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D40" s="29"/>
+      <c r="D40" s="29" t="s">
+        <v>75</v>
+      </c>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
-      <c r="J40" s="31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="31"/>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="18"/>
       <c r="B41" s="19">
         <f t="shared" si="1"/>
@@ -2442,7 +2460,7 @@
       <c r="I41" s="21"/>
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="75">
       <c r="A42" s="1">
         <v>14</v>
       </c>
@@ -2455,15 +2473,21 @@
         <v>Mon</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
+      <c r="G42" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="H42" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="J42" s="30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="B43" s="2">
         <f>B42+2</f>
         <v>41606</v>
@@ -2473,11 +2497,11 @@
         <v>Wed</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F43" s="14"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="5"/>
       <c r="B44" s="6">
         <f>B43+2</f>
@@ -2494,10 +2518,10 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <f>A42+1</f>
         <v>15</v>
@@ -2511,14 +2535,17 @@
         <v>Mon</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F45" s="14"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30">
       <c r="B46" s="2">
         <f>B43+7</f>
         <v>41613</v>
@@ -2528,15 +2555,15 @@
         <v>Wed</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="J46" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="5"/>
       <c r="B47" s="6">
         <f>B44+7</f>
@@ -2547,7 +2574,7 @@
         <v>Fri</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -2556,26 +2583,34 @@
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="30">
       <c r="A48" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
       <c r="D48" s="27" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
+      <c r="G48" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="I48" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="58" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add wk7 and error assessment. change schedule grid to weekly instead of daily.
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="960" windowWidth="25600" windowHeight="13560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
   <si>
     <t>date</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>topic</t>
-  </si>
-  <si>
-    <t>R for 1 sample inference - mean, prop</t>
   </si>
   <si>
     <t>Week</t>
@@ -99,9 +96,6 @@
     <t>comments</t>
   </si>
   <si>
-    <t>Chi-square</t>
-  </si>
-  <si>
     <t>data viz lab</t>
   </si>
   <si>
@@ -121,34 +115,16 @@
   </si>
   <si>
     <t>Distributions Ch  3</t>
-  </si>
-  <si>
-    <t>Foundations for Inference</t>
   </si>
   <si>
     <t>Probability
 * Assessing Normality</t>
   </si>
   <si>
-    <t>LLN CLT</t>
-  </si>
-  <si>
-    <t>Confidence intervals</t>
-  </si>
-  <si>
-    <t>confidence intervals (4.5, 4.6)</t>
-  </si>
-  <si>
-    <t>Using R for hypothesis testing</t>
-  </si>
-  <si>
     <t>presentations</t>
   </si>
   <si>
     <t>project work time</t>
-  </si>
-  <si>
-    <t>Hypothesis testing (4.8)</t>
   </si>
   <si>
     <t>Using codebooks
@@ -172,35 +148,16 @@
     <t>Indicator variables and contrasts</t>
   </si>
   <si>
-    <t>Watch OI [[Video]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=NVbPE1_Cbx8) on HT and DE (8 min)</t>
-  </si>
-  <si>
     <t>Watch OI video on the [[Normal Distribution]](https://www.youtube.com/watch?list=PLkIselvEzpM6V9h55s0l9Kzivih9BUWeW&amp;v=S_p5D-YXLS4) (20 min) and [[Assessing Normality]](https://www.youtube.com/watch?v=smJBsZ4YQZw&amp;index=2&amp;list=PLkIselvEzpM6V9h55s0l9Kzivih9BUWeW) (10 min)</t>
   </si>
   <si>
-    <t>Watch PDS video 11 (30 min)</t>
-  </si>
-  <si>
-    <t>Watch PDS video 12 (28 min)</t>
-  </si>
-  <si>
     <t>Watch PDS video 14 (21 min)</t>
   </si>
   <si>
     <t>Watch PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
   </si>
   <si>
-    <t>Watch OI [[Video]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=FUaXoKdCre4) (6 min)</t>
-  </si>
-  <si>
     <t>Presentations</t>
-  </si>
-  <si>
-    <t>Watch OI Video on [[conditions for ANOVA]](https://www.coursera.org/learn/inferential-statistics-intro/lecture/hSgp3/conditions-for-anova) (3 min)</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 10 (30 min)
-* Watch OI Video on the [[CLT]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=lsCc_pS3O28) (5 min)</t>
   </si>
   <si>
     <t>Regression Assigment (Due 11/17)</t>
@@ -254,10 +211,6 @@
     <t>Kristel week 5</t>
   </si>
   <si>
-    <t>The T distribution
-* Hypothesis testing</t>
-  </si>
-  <si>
     <t>Watch PDS Video 17 (1 hr)
 * Read PDS Chapter 17</t>
   </si>
@@ -273,9 +226,6 @@
 * Confounding</t>
   </si>
   <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
     <t>Finish remaining assignments</t>
   </si>
   <si>
@@ -312,12 +262,6 @@
     <t xml:space="preserve">Exam 1 </t>
   </si>
   <si>
-    <t>Exam 2</t>
-  </si>
-  <si>
-    <t>Exam on Ch 3-5</t>
-  </si>
-  <si>
     <t>Exam on Ch 2</t>
   </si>
   <si>
@@ -328,6 +272,280 @@
   </si>
   <si>
     <t>PS 3.1, 3.2 (Due 10/1)</t>
+  </si>
+  <si>
+    <t>PDS video 4 - post personal codebook, talks about lit review
+use kristel ch4 notes</t>
+  </si>
+  <si>
+    <t>could take an entire class period</t>
+  </si>
+  <si>
+    <t>Read Nature paper (Due 8/23)
+* DC: Intro to R - Basic Building Blocks (Due 8/27)
+* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
+* Metacognition Inventory  (Due 8/27)
+* Read Learning - Your first job paper (Due 8/27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch the introduction video 
+* Acquire course materials
+* Sign up for data camp, Google Group. 
+* Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS 2.2 (Due 9/3) 
+* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
+* Complete both corresponding BBL quizzes (Due 9/3)
+</t>
+  </si>
+  <si>
+    <t>RAT on data types 
+* Medical Records Assignment</t>
+  </si>
+  <si>
+    <t>RAT: CN 4.1-4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correlation Assignment (Due 10/29)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderation Assignment Due (11/5)
+</t>
+  </si>
+  <si>
+    <t>RAT: Multiple Regression</t>
+  </si>
+  <si>
+    <t>RAT: Moderation</t>
+  </si>
+  <si>
+    <t>RAT: Correlation</t>
+  </si>
+  <si>
+    <t>RAT: ANOVA</t>
+  </si>
+  <si>
+    <t>Build your own exam questions (Due 12/6)</t>
+  </si>
+  <si>
+    <t>Post assessment in R 
+* Post Metacognition Assessment</t>
+  </si>
+  <si>
+    <t>RAT: Logistic Regression</t>
+  </si>
+  <si>
+    <t>PS 7.1, 7.3 (Due 10/29)
+* DC Correlation and Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download the AddHealth data into your projects folder. 
+* Read the research questions/personal codebook assignment instructions. </t>
+  </si>
+  <si>
+    <t>Import the Add Health data into R
+* Read and create a codebook for AddHealth</t>
+  </si>
+  <si>
+    <t>Citation assignment (Due 9/10)</t>
+  </si>
+  <si>
+    <t>PS 2.4, 2.5 (Due 9/10)
+* Data Camp: Intro to ggplot (Due 9/10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch PDS video 1 (6 min) 
+* Download the Add Health codebook </t>
+  </si>
+  <si>
+    <t>Watch PDS Video 2 (24 min) 
+* Read Course Notes (CN) Section 2.1 and Open Intro Textbook (OI) Section 1.2</t>
+  </si>
+  <si>
+    <t>PDS Video 4 (8 min)
+* Read: How to read a journal article
+* Read lecture notes on literature reviews</t>
+  </si>
+  <si>
+    <t>Read CN Section 2.2</t>
+  </si>
+  <si>
+    <t>Watch PDS Video 6 (30min)
+* Read CN Section 2.3</t>
+  </si>
+  <si>
+    <t>Discuss examples in CN 2.3</t>
+  </si>
+  <si>
+    <t>PS 2.7 (Due 9/10)
+* DM Prep questions (9/10)</t>
+  </si>
+  <si>
+    <t>No Class (Holiday)</t>
+  </si>
+  <si>
+    <t>RAT on data management
+* data management with the depression data</t>
+  </si>
+  <si>
+    <t>data management
+video focuses on recoding, skip patterns and missing data</t>
+  </si>
+  <si>
+    <t>RAT on CN 2.2
+* Discussion examples in CN 2.2</t>
+  </si>
+  <si>
+    <t>Data management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watch PDS Video 7 (30min)
+* Install the `ggplot2`  packages
+* Download the `dm_depress.Rmd` into your `math315/code` folder </t>
+  </si>
+  <si>
+    <t>Watch PDS Video 8 (30min)
+* Start a new RMD file - replicate all univariate plots in tutorial</t>
+  </si>
+  <si>
+    <t>Read about writing empirical research</t>
+  </si>
+  <si>
+    <t>data viz lab
+Edward (10am), Kathy (12)</t>
+  </si>
+  <si>
+    <t>Edward (10am), Kathy (12)</t>
+  </si>
+  <si>
+    <t>Open work time</t>
+  </si>
+  <si>
+    <t>Open work time on DM and graphing</t>
+  </si>
+  <si>
+    <t>Introduce Research plan outline
+* Prep for Exam 1</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment (Due 9/26)
+* Peer Review Biv. Graph (Due 10/1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
+* Peer Review of this assignment (Due 9/24)
+</t>
+  </si>
+  <si>
+    <t>Research Plan Outline (Due 10/8)
+* Poster Prep I (Due 10/15)
+* Peer Review Poster Prep 1 (Due 10/20)</t>
+  </si>
+  <si>
+    <t>Analysis and Poster work</t>
+  </si>
+  <si>
+    <t>Poster Draft (Due 11/28)
+* Peer Review Poster Draft (Due 12/1)</t>
+  </si>
+  <si>
+    <t>Poster Prep II (Due 11/12)
+* Peer Review PPII (Due 11/16)</t>
+  </si>
+  <si>
+    <t>[Finals](Finals.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 1 ](wk01.html)
+</t>
+  </si>
+  <si>
+    <t>[Week 2 ](wk02.html)</t>
+  </si>
+  <si>
+    <t>[Week 3 ](wk03.html)</t>
+  </si>
+  <si>
+    <t>[Week 4 ](wk04.html)</t>
+  </si>
+  <si>
+    <t>[Week 5 ](wk05.html)</t>
+  </si>
+  <si>
+    <t>[Week 6 ](wk06.html)</t>
+  </si>
+  <si>
+    <t>[Week 7 ](wk07.html)</t>
+  </si>
+  <si>
+    <t>[Week 8 ](wk08.html)</t>
+  </si>
+  <si>
+    <t>[Week 9 ](wk09.html)</t>
+  </si>
+  <si>
+    <t>[Week 10 ](wk10.html)</t>
+  </si>
+  <si>
+    <t>[Week 11 ](wk11.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 12 ](wk12.html)
+</t>
+  </si>
+  <si>
+    <t>[Week 13 ](wk13.html)</t>
+  </si>
+  <si>
+    <t>[Week 14 ](wk14.html)</t>
+  </si>
+  <si>
+    <t>[Week 15 ](wk15.html)</t>
+  </si>
+  <si>
+    <t>Foundations for Inference
+* Confidence Intervals
+* T Distribution
+* Hypothesis Testing</t>
+  </si>
+  <si>
+    <t>LLN CLT
+confidence intervals (4.5, 4.6)
+Hypothesis testing (4.8)</t>
+  </si>
+  <si>
+    <t>[PDS Video 10](http://passiondrivenstatistics.com/2015/07/15/chapter-10/) (30 min)
+* OI Video on the [[CLT]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=lsCc_pS3O28) (5 min)
+* OI Video on [[Confidence Intervals]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=FUaXoKdCre4) (6 min)
+* OI Video on [[Hypothesis testing]](https://www.youtube.com/watch?list=PLkIselvEzpM7Pjo94m1e7J5jkIZkbQAl4&amp;v=NVbPE1_Cbx8) (8 min)</t>
+  </si>
+  <si>
+    <t>Data Camp: Foundations for Inference: Sampling Distributions (Due 10/3)
+* PS 4.1, 4.2 (Due 10/3)
+* Data Camp: Foundations for Inference: Confidence Intervals (Due 10/5)
+* PS 4.4 (Due 10/5)
+* PS 4.7, 4.8 (Due 10/8)</t>
+  </si>
+  <si>
+    <t>Using R for hypothesis testing
+* Exam 2 on Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam on Ch 3-5 on Friday. </t>
+  </si>
+  <si>
+    <t>R for 1 sample inference - mean, prop. Ch 5</t>
+  </si>
+  <si>
+    <t>Bivariate Analysis</t>
+  </si>
+  <si>
+    <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
+* OpenIntro Video on [[conditions for ANOVA]](https://www.coursera.org/learn/inferential-statistics-intro/lecture/hSgp3/conditions-for-anova) (3 min)
+* [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)</t>
   </si>
   <si>
     <r>
@@ -346,257 +564,13 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-* PS 6.6  (Due 10/22)</t>
+* PS 6.6  (Due 10/22)
+* Chi-Squared Assignment (Due 10/27)</t>
     </r>
-  </si>
-  <si>
-    <t>PDS video 4 - post personal codebook, talks about lit review
-use kristel ch4 notes</t>
-  </si>
-  <si>
-    <t>could take an entire class period</t>
-  </si>
-  <si>
-    <t>Read Nature paper (Due 8/23)
-* DC: Intro to R - Basic Building Blocks (Due 8/27)
-* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
-* Metacognition Inventory  (Due 8/27)
-* Read Learning - Your first job paper (Due 8/27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch the introduction video 
-* Acquire course materials
-* Sign up for data camp, Google Group. 
-* Fill out the [OH Survey](https://goo.gl/forms/nPjWFAosETEflXP32)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS 2.2 (Due 9/3) 
-* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
-* Complete both corresponding BBL quizzes (Due 9/3)
-</t>
-  </si>
-  <si>
-    <t>RAT on data types 
-* Medical Records Assignment</t>
-  </si>
-  <si>
-    <t>RAT: CN 4.1-4.4</t>
-  </si>
-  <si>
-    <t>PS 4.7, 4.8 (10/8)</t>
-  </si>
-  <si>
-    <t>Data Camp: Foundations for Inference: Sampling Distributions (Due 10/3)
-* PS 4.1, 4.2 (Due 10/3)</t>
-  </si>
-  <si>
-    <t>Data Camp: Foundations for Inference: Confidence Intervals (Due 10/5)
-PS 4.4 (Due 10/5)</t>
-  </si>
-  <si>
-    <t>Chi-Squared Assignment (Due 10/27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correlation Assignment (Due 10/29)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderation Assignment Due (11/5)
-</t>
-  </si>
-  <si>
-    <t>RAT: Multiple Regression</t>
-  </si>
-  <si>
-    <t>RAT: Moderation</t>
-  </si>
-  <si>
-    <t>RAT: Correlation</t>
-  </si>
-  <si>
-    <t>RAT: ANOVA</t>
-  </si>
-  <si>
-    <t>Build your own exam questions (Due 12/6)</t>
-  </si>
-  <si>
-    <t>Post assessment in R 
-* Post Metacognition Assessment</t>
-  </si>
-  <si>
-    <t>RAT: Logistic Regression</t>
-  </si>
-  <si>
-    <t>PS 7.1, 7.3 (Due 10/29)
-* DC Correlation and Regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Download the AddHealth data into your projects folder. 
-* Read the research questions/personal codebook assignment instructions. </t>
-  </si>
-  <si>
-    <t>Import the Add Health data into R
-* Read and create a codebook for AddHealth</t>
-  </si>
-  <si>
-    <t>Citation assignment (Due 9/10)</t>
-  </si>
-  <si>
-    <t>PS 2.4, 2.5 (Due 9/10)
-* Data Camp: Intro to ggplot (Due 9/10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch PDS video 1 (6 min) 
-* Download the Add Health codebook </t>
-  </si>
-  <si>
-    <t>Watch PDS Video 2 (24 min) 
-* Read Course Notes (CN) Section 2.1 and Open Intro Textbook (OI) Section 1.2</t>
-  </si>
-  <si>
-    <t>PDS Video 4 (8 min)
-* Read: How to read a journal article
-* Read lecture notes on literature reviews</t>
-  </si>
-  <si>
-    <t>Read CN Section 2.2</t>
-  </si>
-  <si>
-    <t>Watch PDS Video 6 (30min)
-* Read CN Section 2.3</t>
-  </si>
-  <si>
-    <t>Discuss examples in CN 2.3</t>
-  </si>
-  <si>
-    <t>PS 2.7 (Due 9/10)
-* DM Prep questions (9/10)</t>
-  </si>
-  <si>
-    <t>No Class (Holiday)</t>
-  </si>
-  <si>
-    <t>RAT on data management
-* data management with the depression data</t>
-  </si>
-  <si>
-    <t>data management
-video focuses on recoding, skip patterns and missing data</t>
-  </si>
-  <si>
-    <t>RAT on CN 2.2
-* Discussion examples in CN 2.2</t>
-  </si>
-  <si>
-    <t>Data management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watch PDS Video 7 (30min)
-* Install the `ggplot2`  packages
-* Download the `dm_depress.Rmd` into your `math315/code` folder </t>
-  </si>
-  <si>
-    <t>Watch PDS Video 8 (30min)
-* Start a new RMD file - replicate all univariate plots in tutorial</t>
-  </si>
-  <si>
-    <t>Read about writing empirical research</t>
-  </si>
-  <si>
-    <t>data viz lab
-Edward (10am), Kathy (12)</t>
-  </si>
-  <si>
-    <t>Edward (10am), Kathy (12)</t>
-  </si>
-  <si>
-    <t>Open work time</t>
-  </si>
-  <si>
-    <t>Open work time on DM and graphing</t>
-  </si>
-  <si>
-    <t>Introduce Research plan outline
-* Prep for Exam 1</t>
-  </si>
-  <si>
-    <t>Bivariate graphing assignment (Due 9/26)
-* Peer Review Biv. Graph (Due 10/1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Univariate graphing assignment (Due 9/19)
-* Peer Review of this assignment (Due 9/24)
-</t>
-  </si>
-  <si>
-    <t>Research Plan Outline (Due 10/8)
-* Poster Prep I (Due 10/15)
-* Peer Review Poster Prep 1 (Due 10/20)</t>
-  </si>
-  <si>
-    <t>Analysis and Poster work</t>
-  </si>
-  <si>
-    <t>Poster Draft (Due 11/28)
-* Peer Review Poster Draft (Due 12/1)</t>
-  </si>
-  <si>
-    <t>Poster Prep II (Due 11/12)
-* Peer Review PPII (Due 11/16)</t>
-  </si>
-  <si>
-    <t>[Finals](Finals.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 1 ](wk01.html)
-</t>
-  </si>
-  <si>
-    <t>[Week 2 ](wk02.html)</t>
-  </si>
-  <si>
-    <t>[Week 3 ](wk03.html)</t>
-  </si>
-  <si>
-    <t>[Week 4 ](wk04.html)</t>
-  </si>
-  <si>
-    <t>[Week 5 ](wk05.html)</t>
-  </si>
-  <si>
-    <t>[Week 6 ](wk06.html)</t>
-  </si>
-  <si>
-    <t>[Week 7 ](wk07.html)</t>
-  </si>
-  <si>
-    <t>[Week 8 ](wk08.html)</t>
-  </si>
-  <si>
-    <t>[Week 9 ](wk09.html)</t>
-  </si>
-  <si>
-    <t>[Week 10 ](wk10.html)</t>
-  </si>
-  <si>
-    <t>[Week 11 ](wk11.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 12 ](wk12.html)
-</t>
-  </si>
-  <si>
-    <t>[Week 13 ](wk13.html)</t>
-  </si>
-  <si>
-    <t>[Week 14 ](wk14.html)</t>
-  </si>
-  <si>
-    <t>[Week 15 ](wk15.html)</t>
   </si>
 </sst>
 </file>
@@ -609,6 +583,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -688,7 +663,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -728,12 +703,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,7 +824,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,9 +874,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -938,9 +904,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1001,7 +964,25 @@
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1419,11 +1400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1442,7 +1423,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="19" thickBot="1">
       <c r="A1" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -1457,54 +1438,54 @@
         <v>2</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="120">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="45">
         <v>41506</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" ref="C2:C40" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
+        <f t="shared" ref="C2:C34" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="4" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75">
-      <c r="B3" s="47">
+      <c r="B3" s="45">
         <f>B2+2</f>
         <v>41508</v>
       </c>
@@ -1513,27 +1494,27 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45">
       <c r="A4" s="5"/>
-      <c r="B4" s="48">
+      <c r="B4" s="46">
         <f>B3+2</f>
         <v>41510</v>
       </c>
@@ -1542,19 +1523,19 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90">
@@ -1562,8 +1543,8 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="47">
-        <f t="shared" ref="B5:B41" si="1">B2+7</f>
+      <c r="B5" s="45">
+        <f t="shared" ref="B5:B35" si="1">B2+7</f>
         <v>41513</v>
       </c>
       <c r="C5" s="3" t="str">
@@ -1571,27 +1552,27 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="4" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60">
-      <c r="B6" s="47">
+      <c r="B6" s="45">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
@@ -1600,25 +1581,25 @@
         <v>Wed</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="14"/>
       <c r="H6" s="4" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>70</v>
+        <v>96</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="105">
       <c r="A7" s="5"/>
-      <c r="B7" s="48">
+      <c r="B7" s="46">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
@@ -1627,32 +1608,32 @@
         <v>Fri</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>19</v>
-      </c>
       <c r="F7" s="16" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="K7" s="32"/>
+        <v>20</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1">
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="45">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
@@ -1660,20 +1641,20 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
+      <c r="D8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+        <v>128</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:11" ht="30">
-      <c r="B9" s="47">
+      <c r="B9" s="45">
         <f t="shared" si="1"/>
         <v>41522</v>
       </c>
@@ -1681,26 +1662,26 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>20</v>
+      <c r="D9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="F9" s="14"/>
       <c r="H9" s="4" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="180">
       <c r="A10" s="5"/>
-      <c r="B10" s="48">
+      <c r="B10" s="46">
         <f t="shared" si="1"/>
         <v>41524</v>
       </c>
@@ -1709,23 +1690,23 @@
         <v>Fri</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>128</v>
+        <v>104</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="105">
@@ -1733,7 +1714,7 @@
         <f>A8+1</f>
         <v>4</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="45">
         <f t="shared" si="1"/>
         <v>41527</v>
       </c>
@@ -1742,27 +1723,27 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J11" s="45" t="s">
-        <v>60</v>
+        <v>107</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="75">
-      <c r="B12" s="47">
+      <c r="B12" s="45">
         <f>B9+7</f>
         <v>41529</v>
       </c>
@@ -1771,25 +1752,25 @@
         <v>Wed</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>143</v>
+        <v>28</v>
+      </c>
+      <c r="J12" s="37" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30">
       <c r="A13" s="5"/>
-      <c r="B13" s="48">
+      <c r="B13" s="46">
         <f>B10+7</f>
         <v>41531</v>
       </c>
@@ -1798,25 +1779,25 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J13" s="46"/>
+        <v>117</v>
+      </c>
+      <c r="J13" s="44"/>
     </row>
     <row r="14" spans="1:11" ht="30">
       <c r="A14" s="1">
         <f>A11+1</f>
         <v>5</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="45">
         <f>B11+7</f>
         <v>41534</v>
       </c>
@@ -1825,27 +1806,27 @@
         <v>Mon</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="14">
         <v>2.4</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="4" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="15" spans="1:11" ht="60">
-      <c r="B15" s="47">
+      <c r="B15" s="45">
         <f t="shared" si="1"/>
         <v>41536</v>
       </c>
@@ -1853,25 +1834,25 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>142</v>
+      <c r="J15" s="34" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="45">
       <c r="A16" s="5"/>
-      <c r="B16" s="48">
+      <c r="B16" s="46">
         <f t="shared" si="1"/>
         <v>41538</v>
       </c>
@@ -1879,19 +1860,19 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D16" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" s="37"/>
+      <c r="D16" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10" ht="45">
       <c r="A17" s="1">
@@ -1906,22 +1887,22 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>80</v>
+      <c r="D17" s="31" t="s">
+        <v>64</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="4" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1933,16 +1914,16 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D18" s="49" t="s">
-        <v>89</v>
+      <c r="D18" s="52" t="s">
+        <v>73</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="I18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="39" t="s">
-        <v>85</v>
+        <v>74</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="135">
@@ -1956,652 +1937,522 @@
         <v>Fri</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="75">
-      <c r="A20" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="225">
+      <c r="A20" s="47">
         <f>A17+1</f>
         <v>7</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="48">
         <f t="shared" si="1"/>
         <v>41548</v>
       </c>
-      <c r="C20" s="3" t="str">
+      <c r="C20" s="49" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="60">
-      <c r="B21" s="2">
-        <f t="shared" si="1"/>
-        <v>41550</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="H21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="75">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6">
-        <f t="shared" si="1"/>
-        <v>41552</v>
-      </c>
-      <c r="C22" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8" t="s">
-        <v>104</v>
+      <c r="D20" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="I20" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="J20" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45">
+      <c r="A21" s="47">
+        <f>A20+1</f>
+        <v>8</v>
+      </c>
+      <c r="B21" s="48">
+        <f>B20+7</f>
+        <v>41555</v>
+      </c>
+      <c r="C21" s="49" t="str">
+        <f t="shared" si="0"/>
+        <v>Mon</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" s="53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="165">
+      <c r="A22" s="47">
+        <f>A21+1</f>
+        <v>9</v>
+      </c>
+      <c r="B22" s="48">
+        <f>B21+7</f>
+        <v>41562</v>
+      </c>
+      <c r="C22" s="49" t="str">
+        <f t="shared" si="0"/>
+        <v>Mon</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="50" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30">
       <c r="A23" s="1">
-        <f>A20+1</f>
-        <v>8</v>
+        <f>A22+1</f>
+        <v>10</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="1"/>
-        <v>41555</v>
+        <f>B22+7</f>
+        <v>41569</v>
       </c>
       <c r="C23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>6</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="J23" s="30"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="B24" s="2">
-        <f t="shared" si="1"/>
-        <v>41557</v>
-      </c>
-      <c r="C24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
+        <v>135</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
+      <c r="J24" s="37" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="5"/>
-      <c r="B25" s="6">
-        <f t="shared" si="1"/>
-        <v>41559</v>
-      </c>
-      <c r="C25" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30">
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="60">
       <c r="A26" s="1">
         <f>A23+1</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="1"/>
-        <v>41562</v>
+        <v>41576</v>
       </c>
       <c r="C26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="4" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="75">
+        <v>88</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="B27" s="2">
         <f t="shared" si="1"/>
-        <v>41564</v>
+        <v>7</v>
       </c>
       <c r="C27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Wed</v>
+        <v>Fri</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
-      <c r="H27" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:10" ht="30">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <f t="shared" si="1"/>
-        <v>41566</v>
+        <v>7</v>
       </c>
       <c r="C28" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="31" t="s">
-        <v>107</v>
+      <c r="J28" s="29" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30">
       <c r="A29" s="1">
         <f>A26+1</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="1"/>
-        <v>41569</v>
+        <v>41583</v>
       </c>
       <c r="C29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="4" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J29" s="30" t="s">
-        <v>108</v>
+        <v>87</v>
+      </c>
+      <c r="J29" s="28" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30">
       <c r="B30" s="2">
         <f t="shared" si="1"/>
-        <v>41571</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Wed</v>
+        <v>Fri</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="14"/>
+        <v>39</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="F30" s="14"/>
-      <c r="J30" s="39" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="5"/>
-      <c r="B31" s="6">
+      <c r="B31" s="39">
         <f t="shared" si="1"/>
-        <v>41573</v>
-      </c>
-      <c r="C31" s="7" t="str">
+        <v>14</v>
+      </c>
+      <c r="C31" s="40" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" ht="60">
+      <c r="D31" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <f>A29+1</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B32" s="2">
         <f t="shared" si="1"/>
-        <v>41576</v>
+        <v>41590</v>
       </c>
       <c r="C32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>53</v>
+        <v>138</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J32" s="30" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="B33" s="2">
         <f t="shared" si="1"/>
-        <v>41578</v>
+        <v>21</v>
       </c>
       <c r="C33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Wed</v>
+        <v>Fri</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
     </row>
-    <row r="34" spans="1:10" ht="30">
+    <row r="34" spans="1:10">
       <c r="A34" s="5"/>
       <c r="B34" s="6">
         <f t="shared" si="1"/>
-        <v>41580</v>
+        <v>21</v>
       </c>
       <c r="C34" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>75</v>
+      <c r="D34" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="30">
-      <c r="A35" s="1">
-        <f>A32+1</f>
-        <v>12</v>
-      </c>
-      <c r="B35" s="2">
-        <f t="shared" si="1"/>
-        <v>41583</v>
-      </c>
-      <c r="C35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Mon</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J35" s="30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="30">
-      <c r="B36" s="2">
-        <f t="shared" si="1"/>
-        <v>41585</v>
-      </c>
-      <c r="C36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="5"/>
-      <c r="B37" s="41">
-        <f t="shared" si="1"/>
-        <v>41587</v>
-      </c>
-      <c r="C37" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D37" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="1">
-        <f>A35+1</f>
-        <v>13</v>
-      </c>
-      <c r="B38" s="2">
-        <f t="shared" si="1"/>
-        <v>41590</v>
-      </c>
-      <c r="C38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Mon</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="B39" s="2">
-        <f t="shared" si="1"/>
-        <v>41592</v>
-      </c>
-      <c r="C39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6">
-        <f t="shared" si="1"/>
-        <v>41594</v>
-      </c>
-      <c r="C40" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="31"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19">
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18">
         <f t="shared" si="1"/>
         <v>41597</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="21" t="s">
+      <c r="C35" s="19"/>
+      <c r="D35" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-    </row>
-    <row r="42" spans="1:10" ht="75">
-      <c r="A42" s="1">
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="1:10" ht="75">
+      <c r="A36" s="1">
         <v>14</v>
       </c>
-      <c r="B42" s="2">
-        <f>B41+7</f>
+      <c r="B36" s="2">
+        <f>B35+7</f>
         <v>41604</v>
       </c>
-      <c r="C42" s="3" t="str">
-        <f t="shared" ref="C42:C47" si="2">TEXT(WEEKDAY(B42,1)+1, "ddd")</f>
+      <c r="C36" s="3" t="str">
+        <f t="shared" ref="C36:C41" si="2">TEXT(WEEKDAY(B36,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>145</v>
+      <c r="D36" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="B37" s="2">
+        <f>B36+2</f>
+        <v>41606</v>
+      </c>
+      <c r="C37" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6">
+        <f>B37+2</f>
+        <v>41608</v>
+      </c>
+      <c r="C38" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
+        <f>A36+1</f>
+        <v>15</v>
+      </c>
+      <c r="B39" s="2">
+        <f>B36+7</f>
+        <v>41611</v>
+      </c>
+      <c r="C39" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Mon</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="14"/>
+      <c r="G39" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30">
+      <c r="B40" s="2">
+        <f>B37+7</f>
+        <v>41613</v>
+      </c>
+      <c r="C40" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>Wed</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="J40" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6">
+        <f>B38+7</f>
+        <v>41615</v>
+      </c>
+      <c r="C41" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>Fri</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" ht="30">
+      <c r="A42" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="26" t="s">
+        <v>75</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="G42" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J42" s="30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="B43" s="2">
-        <f>B42+2</f>
-        <v>41606</v>
-      </c>
-      <c r="C43" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Wed</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="14"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6">
-        <f>B43+2</f>
-        <v>41608</v>
-      </c>
-      <c r="C44" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Fri</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="1">
-        <f>A42+1</f>
-        <v>15</v>
-      </c>
-      <c r="B45" s="2">
-        <f>B42+7</f>
-        <v>41611</v>
-      </c>
-      <c r="C45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Mon</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="30">
-      <c r="B46" s="2">
-        <f>B43+7</f>
-        <v>41613</v>
-      </c>
-      <c r="C46" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Wed</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="J46" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6">
-        <f>B44+7</f>
-        <v>41615</v>
-      </c>
-      <c r="C47" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>Fri</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="1:10" ht="30">
-      <c r="A48" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>115</v>
+        <v>125</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change to weekly schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="141">
   <si>
     <t>date</t>
   </si>
@@ -118,13 +118,6 @@
   </si>
   <si>
     <t>Data visualization lab - bivariate portion</t>
-  </si>
-  <si>
-    <t>Distributions Ch  3</t>
-  </si>
-  <si>
-    <t>Probability
-* Assessing Normality</t>
   </si>
   <si>
     <t>presentations</t>
@@ -148,9 +141,6 @@
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Watch OI video on the [[Normal Distribution]](https://www.youtube.com/watch?list=PLkIselvEzpM6V9h55s0l9Kzivih9BUWeW&amp;v=S_p5D-YXLS4) (20 min) and [[Assessing Normality]](https://www.youtube.com/watch?v=smJBsZ4YQZw&amp;index=2&amp;list=PLkIselvEzpM6V9h55s0l9Kzivih9BUWeW) (10 min)</t>
-  </si>
-  <si>
     <t>Watch PDS video 14 (21 min)</t>
   </si>
   <si>
@@ -219,34 +209,16 @@
     <t>Finish all remaining graphics assignments</t>
   </si>
   <si>
-    <t>Research Plan Introduction</t>
-  </si>
-  <si>
     <t>Moderation</t>
   </si>
   <si>
-    <t>Error Analysis Due 10/27</t>
-  </si>
-  <si>
-    <t>Error Analysis Due 10/6</t>
-  </si>
-  <si>
     <t>Watch PDS Video 9 (30min)</t>
   </si>
   <si>
-    <t xml:space="preserve">Exam 1 </t>
-  </si>
-  <si>
-    <t>Exam on Ch 2</t>
-  </si>
-  <si>
     <t>Final Exam</t>
   </si>
   <si>
     <t>Exam on Weeks 9-12</t>
-  </si>
-  <si>
-    <t>PS 3.1, 3.2 (Due 10/1)</t>
   </si>
   <si>
     <t>PDS video 4 - post personal codebook, talks about lit review
@@ -371,9 +343,6 @@
 * Start a new RMD file - replicate all univariate plots in tutorial</t>
   </si>
   <si>
-    <t>Read about writing empirical research</t>
-  </si>
-  <si>
     <t>data viz lab
 Edward (10am), Kathy (12)</t>
   </si>
@@ -385,10 +354,6 @@
   </si>
   <si>
     <t>Open work time on DM and graphing</t>
-  </si>
-  <si>
-    <t>Introduce Research plan outline
-* Prep for Exam 1</t>
   </si>
   <si>
     <t>Bivariate graphing assignment (Due 9/26)
@@ -486,11 +451,6 @@
     <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
 * OpenIntro Video on [[conditions for ANOVA]](https://www.coursera.org/learn/inferential-statistics-intro/lecture/hSgp3/conditions-for-anova) (3 min)
 * [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)</t>
-  </si>
-  <si>
-    <t>Research Plan Outline (Due 10/8)
-* Poster Prep Stage I (Due 10/15)
-* Peer Review Poster Prep Stage 1 (Due 10/20)</t>
   </si>
   <si>
     <r>
@@ -556,12 +516,75 @@
   <si>
     <t>Using R for hypothesis testing</t>
   </si>
+  <si>
+    <t>Introduction to the class structure and logistics, Reproducible research, Data Analysis Life cycle, Add Health Data</t>
+  </si>
+  <si>
+    <t>Read Nature paper (Due 8/23)
+* DC: Intro to R - Basic Building Blocks (Due 8/27)
+* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
+* Metacognition Inventory  (Due 8/27)
+* Read Learning - Your first job paper (Due 8/27)
+* R Markdown test file (Due 8/23)
+* HW 1 (Due 8/27)</t>
+  </si>
+  <si>
+    <t>Data architecture
+* codebooks
+* creating research questions
+* Importing data into R
+ * Conducting a lit review</t>
+  </si>
+  <si>
+    <t>PS 2.2 (Due 9/3) 
+* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
+* Complete both corresponding BBL quizzes (Due 9/3)
+* Personal Codebook / Research question assignment (Due 9/5)
+* Citation assignment (Due 9/10)</t>
+  </si>
+  <si>
+    <t>Describing Univariate data</t>
+  </si>
+  <si>
+    <t>Data management
+* Data Visualization</t>
+  </si>
+  <si>
+    <t>[Notes on doing data management](https://norcalbiostat.netlify.com/lec/doing-dm/)
+* [Data Viz Tutorial](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data management assignment [addhealth_dm.Rmd](https://norcalbiostat.github.io/MATH315/hw/dm_addhealth.html) (Due 9/17)
+* [Univariate graphing assignment](https://norcalbiostat.github.io/MATH315/hw/univ_graphing.html) (Due 9/19)
+* [Peer Review](https://docs.google.com/forms/d/e/1FAIpQLSfIaJNSVKErpQm4RUjdCc9UhFwq6pLqCBqFOQDPvgxS_d2XKg/closedform) of this assignment (Due 9/24)
+</t>
+  </si>
+  <si>
+    <t>PS 2.8, 2.10 (Due 9/24)
+[Bivariate graphing assignment](https://norcalbiostat.github.io/MATH315/hw/biv_graphing.html) (Due 9/26)
+* [Peer Review Biv. Graph](https://norcalbiostat.github.io/MATH315/project.html) (Due 10/1)</t>
+  </si>
+  <si>
+    <t>Research Plan Introduction
+* Exam 1 (Wed)
+* Probability</t>
+  </si>
+  <si>
+    <t>[Research Plan Outline](https://norcalbiostat.github.io/MATH315/hw/research_plan_outline.html) (Due 10/8)
+* [Poster Prep Stage I](https://norcalbiostat.github.io/MATH315/project.html) (Due 10/15)
+* Peer Review Poster Prep Stage 1 (Due 10/20)
+* [Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/6
+* PS 3.1, 3.2 (Due 10/1)</t>
+  </si>
+  <si>
+    <t>[Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/27</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -654,8 +677,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -698,8 +774,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -736,6 +818,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -816,7 +909,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -831,9 +924,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -858,59 +948,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -955,6 +997,121 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1034,8 +1191,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1371,12 +1528,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1384,17 +1541,17 @@
     <col min="1" max="1" width="6.5" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="47" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="47" customWidth="1"/>
-    <col min="7" max="7" width="20.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.75" style="8" customWidth="1"/>
-    <col min="9" max="9" width="31.125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="53.75" style="8" customWidth="1"/>
+    <col min="4" max="4" width="26" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="30" customWidth="1"/>
+    <col min="7" max="7" width="20.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.75" style="7" customWidth="1"/>
+    <col min="9" max="9" width="31.125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="53.75" style="7" customWidth="1"/>
     <col min="11" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1414,10 +1571,10 @@
         <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>13</v>
@@ -1426,810 +1583,474 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="58">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="59">
         <v>41506</v>
       </c>
-      <c r="C2" s="7" t="str">
-        <f t="shared" ref="C2:C26" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
+      <c r="C2" s="60" t="str">
+        <f t="shared" ref="C2:C14" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
-        <f>B2+2</f>
-        <v>41508</v>
-      </c>
-      <c r="C3" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11">
-        <f>B3+2</f>
-        <v>41510</v>
-      </c>
-      <c r="C4" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="F2" s="62"/>
+      <c r="G2" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="6">
-        <f t="shared" ref="B5:B20" si="1">B2+7</f>
+      <c r="B3" s="64">
+        <f>B2+7</f>
         <v>41513</v>
       </c>
-      <c r="C5" s="7" t="str">
+      <c r="C3" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <f t="shared" si="1"/>
-        <v>41515</v>
-      </c>
-      <c r="C6" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="H6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11">
-        <f t="shared" si="1"/>
-        <v>41517</v>
-      </c>
-      <c r="C7" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <f>A5+1</f>
+      <c r="D3" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="6">
-        <f t="shared" si="1"/>
+      <c r="B4" s="64">
+        <f>B3+7</f>
         <v>41520</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C4" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <f t="shared" si="1"/>
-        <v>41522</v>
-      </c>
-      <c r="C9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="H9" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="189" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11">
-        <f t="shared" si="1"/>
-        <v>41524</v>
-      </c>
-      <c r="C10" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <f>A8+1</f>
+      <c r="D4" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="67"/>
+    </row>
+    <row r="5" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B11" s="6">
-        <f t="shared" si="1"/>
+      <c r="B5" s="10">
+        <f>B4+7</f>
         <v>41527</v>
       </c>
-      <c r="C11" s="7" t="str">
+      <c r="C5" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <f>B9+7</f>
-        <v>41529</v>
-      </c>
-      <c r="C12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11">
-        <f>B10+7</f>
-        <v>41531</v>
-      </c>
-      <c r="C13" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <f>A11+1</f>
+      <c r="D5" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="66" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="66" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="B14" s="6">
-        <f>B11+7</f>
+      <c r="B6" s="64">
+        <f>B5+7</f>
         <v>41534</v>
       </c>
-      <c r="C14" s="7" t="str">
+      <c r="C6" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E6" s="20">
         <v>2.4</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
-        <f t="shared" si="1"/>
-        <v>41536</v>
-      </c>
-      <c r="C15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11">
-        <f t="shared" si="1"/>
-        <v>41538</v>
-      </c>
-      <c r="C16" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <f>A14+1</f>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <f>A6+1</f>
         <v>6</v>
       </c>
-      <c r="B17" s="28">
-        <f t="shared" si="1"/>
+      <c r="B7" s="14">
+        <f>B6+7</f>
         <v>41541</v>
       </c>
-      <c r="C17" s="7" t="str">
+      <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="28">
-        <f t="shared" si="1"/>
-        <v>41543</v>
-      </c>
-      <c r="C18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Wed</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="I18" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="32">
-        <f t="shared" si="1"/>
-        <v>41545</v>
-      </c>
-      <c r="C19" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Fri</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="189" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
-        <f>A17+1</f>
+      <c r="D7" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="57"/>
+      <c r="J7" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <f>A7+1</f>
         <v>7</v>
       </c>
-      <c r="B20" s="34">
-        <f t="shared" si="1"/>
+      <c r="B8" s="17">
+        <f>B7+7</f>
         <v>41548</v>
       </c>
-      <c r="C20" s="35" t="str">
+      <c r="C8" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D20" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="36" t="s">
+      <c r="D8" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="H20" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="I20" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
-        <f t="shared" ref="A21:A26" si="2">A20+1</f>
+      <c r="I8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <f t="shared" ref="A9:A14" si="1">A8+1</f>
         <v>8</v>
       </c>
-      <c r="B21" s="34">
-        <f t="shared" ref="B21:B29" si="3">B20+7</f>
+      <c r="B9" s="17">
+        <f t="shared" ref="B9:B17" si="2">B8+7</f>
         <v>41555</v>
       </c>
-      <c r="C21" s="35" t="str">
+      <c r="C9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D9" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="J21" s="38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="33">
+    </row>
+    <row r="10" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="17">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="B22" s="34">
-        <f t="shared" si="3"/>
         <v>41562</v>
       </c>
-      <c r="C22" s="35" t="str">
+      <c r="C10" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D22" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="I22" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A23" s="33">
+      <c r="D10" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="17">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="B23" s="34">
-        <f t="shared" si="3"/>
         <v>41569</v>
       </c>
-      <c r="C23" s="35" t="str">
+      <c r="C11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D23" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="H23" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="33">
+      <c r="D11" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="17">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="B24" s="34">
-        <f t="shared" si="3"/>
         <v>41576</v>
       </c>
-      <c r="C24" s="35" t="str">
+      <c r="C12" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D24" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="H24" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="J24" s="39" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A25" s="33">
+      <c r="D12" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="17">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="B25" s="34">
-        <f t="shared" si="3"/>
         <v>41583</v>
       </c>
-      <c r="C25" s="35" t="str">
+      <c r="C13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D25" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="H25" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="D13" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="14">
         <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="B26" s="28">
-        <f t="shared" si="3"/>
         <v>41590</v>
       </c>
-      <c r="C26" s="7" t="str">
+      <c r="C14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41">
+      <c r="D14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24">
+        <f t="shared" si="2"/>
+        <v>41597</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="17">
+        <f t="shared" si="2"/>
+        <v>41604</v>
+      </c>
+      <c r="C16" s="18" t="str">
+        <f t="shared" ref="C16:C17" si="3">TEXT(WEEKDAY(B16,1)+1, "ddd")</f>
+        <v>Mon</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="19"/>
+      <c r="J16" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <f>A16+1</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="17">
+        <f t="shared" si="2"/>
+        <v>41611</v>
+      </c>
+      <c r="C17" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>41597</v>
-      </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-    </row>
-    <row r="28" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A28" s="33">
-        <v>14</v>
-      </c>
-      <c r="B28" s="34">
-        <f t="shared" si="3"/>
-        <v>41604</v>
-      </c>
-      <c r="C28" s="35" t="str">
-        <f t="shared" ref="C28:C29" si="4">TEXT(WEEKDAY(B28,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D28" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="H28" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="I28" s="36"/>
-      <c r="J28" s="39" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="33">
-        <f>A28+1</f>
-        <v>15</v>
-      </c>
-      <c r="B29" s="34">
-        <f t="shared" si="3"/>
-        <v>41611</v>
-      </c>
-      <c r="C29" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v>Mon</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="D17" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B18" s="14">
         <v>41618</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="I30" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>79</v>
+      <c r="C18" s="6"/>
+      <c r="D18" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="I18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2244,475 +2065,478 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="22.375" style="34"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="189" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="36">
         <v>41506</v>
       </c>
-      <c r="C2" s="7" t="str">
+      <c r="C2" s="37" t="str">
         <f t="shared" ref="C2:C16" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>69</v>
+      <c r="F2" s="39"/>
+      <c r="G2" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6">
+      <c r="A3" s="35"/>
+      <c r="B3" s="36">
         <f>B2+2</f>
         <v>41508</v>
       </c>
-      <c r="C3" s="7" t="str">
+      <c r="C3" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>44</v>
+      <c r="I3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41">
         <f>B3+2</f>
         <v>41510</v>
       </c>
-      <c r="C4" s="12" t="str">
+      <c r="C4" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>45</v>
+      <c r="D4" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="35">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="36">
         <f t="shared" ref="B5:B16" si="1">B2+7</f>
         <v>41513</v>
       </c>
-      <c r="C5" s="7" t="str">
+      <c r="C5" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>71</v>
+      <c r="F5" s="39"/>
+      <c r="G5" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6">
+      <c r="A6" s="35"/>
+      <c r="B6" s="36">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
-      <c r="C6" s="7" t="str">
+      <c r="C6" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>52</v>
+      <c r="F6" s="39"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
-      <c r="C7" s="12" t="str">
+      <c r="C7" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I7" s="13" t="s">
+      <c r="F7" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="15" t="s">
-        <v>83</v>
+      <c r="J7" s="45" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="35">
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="36">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
-      <c r="C8" s="7" t="str">
+      <c r="C8" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="D8" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6">
+      <c r="A9" s="35"/>
+      <c r="B9" s="36">
         <f t="shared" si="1"/>
         <v>41522</v>
       </c>
-      <c r="C9" s="7" t="str">
+      <c r="C9" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>84</v>
+      <c r="F9" s="39"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11">
+      <c r="A10" s="40"/>
+      <c r="B10" s="41">
         <f t="shared" si="1"/>
         <v>41524</v>
       </c>
-      <c r="C10" s="12" t="str">
+      <c r="C10" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>91</v>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="45" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="35">
         <f>A8+1</f>
         <v>4</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="36">
         <f t="shared" si="1"/>
         <v>41527</v>
       </c>
-      <c r="C11" s="7" t="str">
+      <c r="C11" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>42</v>
+      <c r="D11" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6">
+      <c r="A12" s="35"/>
+      <c r="B12" s="36">
         <f>B9+7</f>
         <v>41529</v>
       </c>
-      <c r="C12" s="7" t="str">
+      <c r="C12" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
+      <c r="E12" s="39"/>
+      <c r="F12" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" s="8" t="s">
+      <c r="G12" s="38"/>
+      <c r="H12" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>106</v>
+      <c r="J12" s="46" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11">
+      <c r="A13" s="40"/>
+      <c r="B13" s="41">
         <f>B10+7</f>
         <v>41531</v>
       </c>
-      <c r="C13" s="12" t="str">
+      <c r="C13" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="J13" s="13"/>
+      <c r="D13" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="44"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="35">
         <f>A11+1</f>
         <v>5</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="36">
         <f>B11+7</f>
         <v>41534</v>
       </c>
-      <c r="C14" s="7" t="str">
+      <c r="C14" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="39">
         <v>2.4</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>41</v>
+      <c r="F14" s="39"/>
+      <c r="G14" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36">
         <f t="shared" si="1"/>
         <v>41536</v>
       </c>
-      <c r="C15" s="7" t="str">
+      <c r="C15" s="37" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23" t="s">
+      <c r="E15" s="53"/>
+      <c r="F15" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="25" t="s">
-        <v>105</v>
+      <c r="J15" s="54" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41">
         <f t="shared" si="1"/>
         <v>41538</v>
       </c>
-      <c r="C16" s="12" t="str">
+      <c r="C16" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="26"/>
+      <c r="D16" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add wk8, sample exam 2
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -439,9 +439,6 @@
 * PS 4.7, 4.8 (Due 10/8)</t>
   </si>
   <si>
-    <t xml:space="preserve">Exam on Ch 3-5 on Friday. </t>
-  </si>
-  <si>
     <t>R for 1 sample inference - mean, prop. Ch 5</t>
   </si>
   <si>
@@ -514,9 +511,6 @@
 </t>
   </si>
   <si>
-    <t>Using R for hypothesis testing</t>
-  </si>
-  <si>
     <t>Introduction to the class structure and logistics, Reproducible research, Data Analysis Life cycle, Add Health Data</t>
   </si>
   <si>
@@ -578,6 +572,13 @@
   </si>
   <si>
     <t>[Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam on Ch 4-5 on Friday. </t>
+  </si>
+  <si>
+    <t>Inference using R
+* Exam 2</t>
   </si>
 </sst>
 </file>
@@ -909,7 +910,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -924,6 +925,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,55 +952,40 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1009,109 +998,109 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1533,523 +1522,522 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="20.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.75" style="7" customWidth="1"/>
-    <col min="9" max="9" width="31.125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="53.75" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="4"/>
+    <col min="1" max="1" width="6.5" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.375" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="53" customWidth="1"/>
+    <col min="5" max="5" width="19.875" style="65" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="20.125" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.75" style="53" customWidth="1"/>
+    <col min="9" max="9" width="31.125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="53.75" style="53" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="58">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="32">
         <v>41506</v>
       </c>
-      <c r="C2" s="60" t="str">
+      <c r="C2" s="33" t="str">
         <f t="shared" ref="C2:C14" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="62" t="s">
+      <c r="D2" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61" t="s">
-        <v>130</v>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
-        <f>A2+1</f>
+      <c r="A3" s="36">
+        <f t="shared" ref="A3:A8" si="1">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="64">
-        <f>B2+7</f>
+      <c r="B3" s="37">
+        <f t="shared" ref="B3:B8" si="2">B2+7</f>
         <v>41513</v>
       </c>
-      <c r="C3" s="18" t="str">
+      <c r="C3" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D3" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="19" t="s">
+      <c r="D3" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65" t="s">
-        <v>132</v>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <f>A3+1</f>
+      <c r="A4" s="36">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B4" s="64">
-        <f>B3+7</f>
+      <c r="B4" s="37">
+        <f t="shared" si="2"/>
         <v>41520</v>
       </c>
-      <c r="C4" s="18" t="str">
+      <c r="C4" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D4" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="67" t="s">
+      <c r="D4" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <f>A4+1</f>
+      <c r="A5" s="43">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" s="10">
-        <f>B4+7</f>
+      <c r="B5" s="44">
+        <f t="shared" si="2"/>
         <v>41527</v>
       </c>
-      <c r="C5" s="11" t="str">
+      <c r="C5" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="66" t="s">
-        <v>135</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="66" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <f>A5+1</f>
+      <c r="A6" s="36">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" s="64">
-        <f>B5+7</f>
+      <c r="B6" s="37">
+        <f t="shared" si="2"/>
         <v>41534</v>
       </c>
-      <c r="C6" s="18" t="str">
+      <c r="C6" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="40">
         <v>2.4</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65" t="s">
-        <v>137</v>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <f>A6+1</f>
+      <c r="A7" s="48">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B7" s="14">
-        <f>B6+7</f>
+      <c r="B7" s="49">
+        <f t="shared" si="2"/>
         <v>41541</v>
       </c>
-      <c r="C7" s="6" t="str">
+      <c r="C7" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D7" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="7" t="s">
+      <c r="D7" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="15" t="s">
-        <v>139</v>
+      <c r="J7" s="54" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <f>A7+1</f>
+      <c r="A8" s="36">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B8" s="17">
-        <f>B7+7</f>
+      <c r="B8" s="55">
+        <f t="shared" si="2"/>
         <v>41548</v>
       </c>
-      <c r="C8" s="18" t="str">
+      <c r="C8" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="40"/>
+      <c r="G8" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="39" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <f t="shared" ref="A9:A14" si="1">A8+1</f>
+      <c r="A9" s="36">
+        <f t="shared" ref="A9:A14" si="3">A8+1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="17">
-        <f t="shared" ref="B9:B17" si="2">B8+7</f>
+      <c r="B9" s="55">
+        <f t="shared" ref="B9:B17" si="4">B8+7</f>
         <v>41555</v>
       </c>
-      <c r="C9" s="18" t="str">
+      <c r="C9" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19" t="s">
+      <c r="D9" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>140</v>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <f t="shared" si="1"/>
+      <c r="A10" s="36">
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B10" s="17">
-        <f t="shared" si="2"/>
+      <c r="B10" s="55">
+        <f t="shared" si="4"/>
         <v>41562</v>
       </c>
-      <c r="C10" s="18" t="str">
+      <c r="C10" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="H10" s="19" t="s">
+      <c r="I10" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
-        <f t="shared" si="1"/>
+      <c r="A11" s="36">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B11" s="17">
-        <f t="shared" si="2"/>
+      <c r="B11" s="55">
+        <f t="shared" si="4"/>
         <v>41569</v>
       </c>
-      <c r="C11" s="18" t="str">
+      <c r="C11" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <f t="shared" si="1"/>
+      <c r="A12" s="36">
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B12" s="17">
-        <f t="shared" si="2"/>
+      <c r="B12" s="55">
+        <f t="shared" si="4"/>
         <v>41576</v>
       </c>
-      <c r="C12" s="18" t="str">
+      <c r="C12" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19" t="s">
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="I12" s="19" t="s">
+      <c r="H12" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="22" t="s">
-        <v>121</v>
+      <c r="J12" s="57" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <f t="shared" si="1"/>
+      <c r="A13" s="36">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B13" s="17">
-        <f t="shared" si="2"/>
+      <c r="B13" s="55">
+        <f t="shared" si="4"/>
         <v>41583</v>
       </c>
-      <c r="C13" s="18" t="str">
+      <c r="C13" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19" t="s">
+      <c r="D13" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="57" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <f t="shared" si="1"/>
+      <c r="A14" s="48">
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B14" s="14">
-        <f t="shared" si="2"/>
+      <c r="B14" s="49">
+        <f t="shared" si="4"/>
         <v>41590</v>
       </c>
-      <c r="C14" s="6" t="str">
+      <c r="C14" s="50" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7" t="s">
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="53" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24">
-        <f t="shared" si="2"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59">
+        <f t="shared" si="4"/>
         <v>41597</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26" t="s">
+      <c r="C15" s="60"/>
+      <c r="D15" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
     </row>
     <row r="16" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="36">
         <v>14</v>
       </c>
-      <c r="B16" s="17">
-        <f t="shared" si="2"/>
+      <c r="B16" s="55">
+        <f t="shared" si="4"/>
         <v>41604</v>
       </c>
-      <c r="C16" s="18" t="str">
-        <f t="shared" ref="C16:C17" si="3">TEXT(WEEKDAY(B16,1)+1, "ddd")</f>
+      <c r="C16" s="38" t="str">
+        <f t="shared" ref="C16:C17" si="5">TEXT(WEEKDAY(B16,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="19" t="s">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="22" t="s">
-        <v>127</v>
+      <c r="I16" s="39"/>
+      <c r="J16" s="57" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="36">
         <f>A16+1</f>
         <v>15</v>
       </c>
-      <c r="B17" s="17">
-        <f t="shared" si="2"/>
+      <c r="B17" s="55">
+        <f t="shared" si="4"/>
         <v>41611</v>
       </c>
-      <c r="C17" s="18" t="str">
-        <f t="shared" si="3"/>
+      <c r="C17" s="38" t="str">
+        <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="20" t="s">
+      <c r="D17" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="19" t="s">
+      <c r="F17" s="40"/>
+      <c r="G17" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19" t="s">
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="49">
         <v>41618</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="29" t="s">
+      <c r="C18" s="50"/>
+      <c r="D18" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="I18" s="7" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="I18" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="53" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2074,469 +2062,469 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="22.375" style="34"/>
+    <col min="1" max="16384" width="22.375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="189" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="6">
         <v>41506</v>
       </c>
-      <c r="C2" s="37" t="str">
+      <c r="C2" s="7" t="str">
         <f t="shared" ref="C2:C16" si="0">TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="38" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6">
         <f>B2+2</f>
         <v>41508</v>
       </c>
-      <c r="C3" s="37" t="str">
+      <c r="C3" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11">
         <f>B3+2</f>
         <v>41510</v>
       </c>
-      <c r="C4" s="42" t="str">
+      <c r="C4" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
+      <c r="A5" s="5">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="6">
         <f t="shared" ref="B5:B16" si="1">B2+7</f>
         <v>41513</v>
       </c>
-      <c r="C5" s="37" t="str">
+      <c r="C5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="38" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6">
         <f t="shared" si="1"/>
         <v>41515</v>
       </c>
-      <c r="C6" s="37" t="str">
+      <c r="C6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11">
         <f t="shared" si="1"/>
         <v>41517</v>
       </c>
-      <c r="C7" s="42" t="str">
+      <c r="C7" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
+      <c r="A8" s="5">
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="6">
         <f t="shared" si="1"/>
         <v>41520</v>
       </c>
-      <c r="C8" s="37" t="str">
+      <c r="C8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="38" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6">
         <f t="shared" si="1"/>
         <v>41522</v>
       </c>
-      <c r="C9" s="37" t="str">
+      <c r="C9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="41">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11">
         <f t="shared" si="1"/>
         <v>41524</v>
       </c>
-      <c r="C10" s="42" t="str">
+      <c r="C10" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43" t="s">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="J10" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+      <c r="A11" s="5">
         <f>A8+1</f>
         <v>4</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="6">
         <f t="shared" si="1"/>
         <v>41527</v>
       </c>
-      <c r="C11" s="37" t="str">
+      <c r="C11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="J11" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6">
         <f>B9+7</f>
         <v>41529</v>
       </c>
-      <c r="C12" s="37" t="str">
+      <c r="C12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="46" t="s">
+      <c r="J12" s="16" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="41">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11">
         <f>B10+7</f>
         <v>41531</v>
       </c>
-      <c r="C13" s="42" t="str">
+      <c r="C13" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="J13" s="43"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
+      <c r="A14" s="5">
         <f>A11+1</f>
         <v>5</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="6">
         <f>B11+7</f>
         <v>41534</v>
       </c>
-      <c r="C14" s="37" t="str">
+      <c r="C14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="9">
         <v>2.4</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6">
         <f t="shared" si="1"/>
         <v>41536</v>
       </c>
-      <c r="C15" s="37" t="str">
+      <c r="C15" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53" t="s">
+      <c r="E15" s="23"/>
+      <c r="F15" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52" t="s">
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="54" t="s">
+      <c r="J15" s="24" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="41">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11">
         <f t="shared" si="1"/>
         <v>41538</v>
       </c>
-      <c r="C16" s="42" t="str">
+      <c r="C16" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56" t="s">
+      <c r="E16" s="26"/>
+      <c r="F16" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55" t="s">
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="55"/>
+      <c r="J16" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update schedule with links
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -261,9 +261,6 @@
     <t>RAT: Correlation</t>
   </si>
   <si>
-    <t>RAT: ANOVA</t>
-  </si>
-  <si>
     <t>Build your own exam questions (Due 12/6)</t>
   </si>
   <si>
@@ -442,14 +439,122 @@
     <t>R for 1 sample inference - mean, prop. Ch 5</t>
   </si>
   <si>
-    <t>Bivariate Analysis</t>
-  </si>
-  <si>
     <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
 * OpenIntro Video on [[conditions for ANOVA]](https://www.coursera.org/learn/inferential-statistics-intro/lecture/hSgp3/conditions-for-anova) (3 min)
 * [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)</t>
   </si>
   <si>
+    <t>Moderation Assignment Due (11/5)
+* Poster Prep Stage II (Due 11/12)
+* Peer Review Stage II (Due 11/16)</t>
+  </si>
+  <si>
+    <t>PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
+  </si>
+  <si>
+    <t>Correlation &amp; Linear Regression</t>
+  </si>
+  <si>
+    <t>Multiple Regression
+* Confounding
+* Indicator Variables
+* _No Class Friday_</t>
+  </si>
+  <si>
+    <t>Presentations
+* Types of Bias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poster Draft (Due 11/28)
+* Peer Review Poster Draft (Due 12/1)
+* Final version of poster (Due 12/3)
+</t>
+  </si>
+  <si>
+    <t>Introduction to the class structure and logistics, Reproducible research, Data Analysis Life cycle, Add Health Data</t>
+  </si>
+  <si>
+    <t>Read Nature paper (Due 8/23)
+* DC: Intro to R - Basic Building Blocks (Due 8/27)
+* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
+* Metacognition Inventory  (Due 8/27)
+* Read Learning - Your first job paper (Due 8/27)
+* R Markdown test file (Due 8/23)
+* HW 1 (Due 8/27)</t>
+  </si>
+  <si>
+    <t>Data architecture
+* codebooks
+* creating research questions
+* Importing data into R
+ * Conducting a lit review</t>
+  </si>
+  <si>
+    <t>PS 2.2 (Due 9/3) 
+* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
+* Complete both corresponding BBL quizzes (Due 9/3)
+* Personal Codebook / Research question assignment (Due 9/5)
+* Citation assignment (Due 9/10)</t>
+  </si>
+  <si>
+    <t>Describing Univariate data</t>
+  </si>
+  <si>
+    <t>Data management
+* Data Visualization</t>
+  </si>
+  <si>
+    <t>[Notes on doing data management](https://norcalbiostat.netlify.com/lec/doing-dm/)
+* [Data Viz Tutorial](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data management assignment [addhealth_dm.Rmd](https://norcalbiostat.github.io/MATH315/hw/dm_addhealth.html) (Due 9/17)
+* [Univariate graphing assignment](https://norcalbiostat.github.io/MATH315/hw/univ_graphing.html) (Due 9/19)
+* [Peer Review](https://docs.google.com/forms/d/e/1FAIpQLSfIaJNSVKErpQm4RUjdCc9UhFwq6pLqCBqFOQDPvgxS_d2XKg/closedform) of this assignment (Due 9/24)
+</t>
+  </si>
+  <si>
+    <t>PS 2.8, 2.10 (Due 9/24)
+[Bivariate graphing assignment](https://norcalbiostat.github.io/MATH315/hw/biv_graphing.html) (Due 9/26)
+* [Peer Review Biv. Graph](https://norcalbiostat.github.io/MATH315/project.html) (Due 10/1)</t>
+  </si>
+  <si>
+    <t>Research Plan Introduction
+* Exam 1 (Wed)
+* Probability</t>
+  </si>
+  <si>
+    <t>[Research Plan Outline](https://norcalbiostat.github.io/MATH315/hw/research_plan_outline.html) (Due 10/8)
+* [Poster Prep Stage I](https://norcalbiostat.github.io/MATH315/project.html) (Due 10/15)
+* Peer Review Poster Prep Stage 1 (Due 10/20)
+* [Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/6
+* PS 3.1, 3.2 (Due 10/1)</t>
+  </si>
+  <si>
+    <t>[Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam on Ch 4-5 on Friday. </t>
+  </si>
+  <si>
+    <t>Inference using R
+* Exam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS 7.1, 7.3 (Due 10/29)
+* DC Correlation and Regression
+</t>
+  </si>
+  <si>
+    <t>Bivariate Inference
+* Two sample tests for means
+* ANOVA
+* Chi-squared tests</t>
+  </si>
+  <si>
+    <r>
+      <t>[Bivariate Inference Assignment](hw/Bivariate_Inference.html)</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -459,7 +564,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ANOVA Assignment (Due 10/22)</t>
+      <t xml:space="preserve"> (Due 10/29)</t>
     </r>
     <r>
       <rPr>
@@ -472,113 +577,12 @@
       </rPr>
       <t xml:space="preserve">
 * PS 6.6  (Due 10/22)
-* Chi-Squared Assignment (Due 10/27)
-* Poster Prep Stage II (Due 10/29)
+* [Poster Prep Stage II](https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 10/29)
 * Peer Review Stage II (Due 11/1)</t>
     </r>
   </si>
   <si>
-    <t>Moderation Assignment Due (11/5)
-* Poster Prep Stage II (Due 11/12)
-* Peer Review Stage II (Due 11/16)</t>
-  </si>
-  <si>
-    <t>PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
-  </si>
-  <si>
-    <t>Correlation &amp; Linear Regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correlation Assignment (Due 10/29)
-* PS 7.1, 7.3 (Due 10/29)
-* DC Correlation and Regression
-</t>
-  </si>
-  <si>
-    <t>Multiple Regression
-* Confounding
-* Indicator Variables
-* _No Class Friday_</t>
-  </si>
-  <si>
-    <t>Presentations
-* Types of Bias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poster Draft (Due 11/28)
-* Peer Review Poster Draft (Due 12/1)
-* Final version of poster (Due 12/3)
-</t>
-  </si>
-  <si>
-    <t>Introduction to the class structure and logistics, Reproducible research, Data Analysis Life cycle, Add Health Data</t>
-  </si>
-  <si>
-    <t>Read Nature paper (Due 8/23)
-* DC: Intro to R - Basic Building Blocks (Due 8/27)
-* Complete corresponding BBL Quiz on DC lesson (Due 8/27)
-* Metacognition Inventory  (Due 8/27)
-* Read Learning - Your first job paper (Due 8/27)
-* R Markdown test file (Due 8/23)
-* HW 1 (Due 8/27)</t>
-  </si>
-  <si>
-    <t>Data architecture
-* codebooks
-* creating research questions
-* Importing data into R
- * Conducting a lit review</t>
-  </si>
-  <si>
-    <t>PS 2.2 (Due 9/3) 
-* Data Camp (2 lessons): Open Intro - Intro to R, and Intro to Data (Due 9/3)
-* Complete both corresponding BBL quizzes (Due 9/3)
-* Personal Codebook / Research question assignment (Due 9/5)
-* Citation assignment (Due 9/10)</t>
-  </si>
-  <si>
-    <t>Describing Univariate data</t>
-  </si>
-  <si>
-    <t>Data management
-* Data Visualization</t>
-  </si>
-  <si>
-    <t>[Notes on doing data management](https://norcalbiostat.netlify.com/lec/doing-dm/)
-* [Data Viz Tutorial](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data management assignment [addhealth_dm.Rmd](https://norcalbiostat.github.io/MATH315/hw/dm_addhealth.html) (Due 9/17)
-* [Univariate graphing assignment](https://norcalbiostat.github.io/MATH315/hw/univ_graphing.html) (Due 9/19)
-* [Peer Review](https://docs.google.com/forms/d/e/1FAIpQLSfIaJNSVKErpQm4RUjdCc9UhFwq6pLqCBqFOQDPvgxS_d2XKg/closedform) of this assignment (Due 9/24)
-</t>
-  </si>
-  <si>
-    <t>PS 2.8, 2.10 (Due 9/24)
-[Bivariate graphing assignment](https://norcalbiostat.github.io/MATH315/hw/biv_graphing.html) (Due 9/26)
-* [Peer Review Biv. Graph](https://norcalbiostat.github.io/MATH315/project.html) (Due 10/1)</t>
-  </si>
-  <si>
-    <t>Research Plan Introduction
-* Exam 1 (Wed)
-* Probability</t>
-  </si>
-  <si>
-    <t>[Research Plan Outline](https://norcalbiostat.github.io/MATH315/hw/research_plan_outline.html) (Due 10/8)
-* [Poster Prep Stage I](https://norcalbiostat.github.io/MATH315/project.html) (Due 10/15)
-* Peer Review Poster Prep Stage 1 (Due 10/20)
-* [Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/6
-* PS 3.1, 3.2 (Due 10/1)</t>
-  </si>
-  <si>
-    <t>[Error Analysis](https://norcalbiostat.github.io/MATH315/wk06.html#wednesday:_exam_1) Due 10/27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exam on Ch 4-5 on Friday. </t>
-  </si>
-  <si>
-    <t>Inference using R
-* Exam 2</t>
+    <t xml:space="preserve">RAT: Two independent sample tests for a difference in mean or proprtions. </t>
   </si>
 </sst>
 </file>
@@ -910,7 +914,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1101,6 +1105,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1522,7 +1532,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1584,19 +1594,19 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
       <c r="G2" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1613,17 +1623,17 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1640,12 +1650,12 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
       <c r="G4" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
@@ -1665,19 +1675,19 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1701,12 +1711,12 @@
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
@@ -1723,15 +1733,15 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
@@ -1748,23 +1758,23 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>112</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>113</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I8" s="39" t="s">
         <v>64</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1781,21 +1791,21 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -1811,25 +1821,25 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D10" s="39" t="s">
-        <v>117</v>
+      <c r="D10" s="66" t="s">
+        <v>138</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H10" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="I10" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="J10" s="66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1843,12 +1853,12 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
       <c r="G11" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H11" s="39" t="s">
         <v>36</v>
@@ -1856,8 +1866,8 @@
       <c r="I11" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="57" t="s">
-        <v>123</v>
+      <c r="J11" s="67" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1879,16 +1889,16 @@
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I12" s="39" t="s">
         <v>66</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -1905,12 +1915,12 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
       <c r="G13" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H13" s="39" t="s">
         <v>51</v>
@@ -1941,10 +1951,10 @@
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1977,19 +1987,19 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
       <c r="G16" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H16" s="39" t="s">
         <v>52</v>
       </c>
       <c r="I16" s="39"/>
       <c r="J16" s="57" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2006,19 +2016,19 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2038,7 +2048,7 @@
         <v>58</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2116,7 +2126,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>61</v>
@@ -2175,7 +2185,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>46</v>
@@ -2205,10 +2215,10 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>63</v>
@@ -2236,10 +2246,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>49</v>
@@ -2266,13 +2276,13 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2289,12 +2299,12 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -2319,13 +2329,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -2349,13 +2359,13 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -2372,20 +2382,20 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>39</v>
@@ -2410,13 +2420,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2430,7 +2440,7 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>50</v>
@@ -2439,7 +2449,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2464,7 +2474,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>56</v>
@@ -2491,7 +2501,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2499,7 +2509,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2517,7 +2527,7 @@
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>

</xml_diff>

<commit_message>
build wk 9 bivariate inference
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -439,11 +442,6 @@
     <t>R for 1 sample inference - mean, prop. Ch 5</t>
   </si>
   <si>
-    <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
-* OpenIntro Video on [[conditions for ANOVA]](https://www.coursera.org/learn/inferential-statistics-intro/lecture/hSgp3/conditions-for-anova) (3 min)
-* [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)</t>
-  </si>
-  <si>
     <t>Moderation Assignment Due (11/5)
 * Poster Prep Stage II (Due 11/12)
 * Peer Review Stage II (Due 11/16)</t>
@@ -552,19 +550,11 @@
 * Chi-squared tests</t>
   </si>
   <si>
+    <t xml:space="preserve">RAT:  CN 6.4 ANOVA (Wed) </t>
+  </si>
+  <si>
     <r>
       <t>[Bivariate Inference Assignment](hw/Bivariate_Inference.html)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Due 10/29)</t>
     </r>
     <r>
       <rPr>
@@ -572,30 +562,37 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve"> (Due 10/29)
 * PS 6.6  (Due 10/22)
 * [Poster Prep Stage II](https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 10/29)
 * Peer Review Stage II (Due 11/1)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">RAT: Two independent sample tests for a difference in mean or proprtions. </t>
+    <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
+* [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)
+* Course Notes  6.2-6.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -619,14 +616,6 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -830,89 +819,89 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1190,8 +1179,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1527,30 +1516,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.375" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="53" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="65" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="65" customWidth="1"/>
-    <col min="7" max="7" width="20.125" style="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.75" style="53" customWidth="1"/>
-    <col min="9" max="9" width="31.125" style="53" customWidth="1"/>
-    <col min="10" max="10" width="53.75" style="53" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="30"/>
+    <col min="5" max="5" width="19.83203125" style="65" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="65" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.6640625" style="53" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" style="53" customWidth="1"/>
+    <col min="10" max="10" width="53.6640625" style="53" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="31">
         <v>1</v>
       </c>
@@ -1594,7 +1583,7 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
@@ -1606,10 +1595,10 @@
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="36">
         <f t="shared" ref="A3:A8" si="1">A2+1</f>
         <v>2</v>
@@ -1623,7 +1612,7 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
@@ -1633,10 +1622,10 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="36">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1650,7 +1639,7 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
@@ -1661,7 +1650,7 @@
       <c r="I4" s="39"/>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A5" s="43">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1675,7 +1664,7 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
@@ -1683,14 +1672,14 @@
         <v>99</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="36">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1716,10 +1705,10 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A7" s="48">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1733,7 +1722,7 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
@@ -1741,10 +1730,10 @@
         <v>101</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A8" s="36">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1777,7 +1766,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
         <f t="shared" ref="A9:A14" si="3">A8+1</f>
         <v>8</v>
@@ -1791,7 +1780,7 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="40" t="s">
         <v>115</v>
@@ -1802,13 +1791,13 @@
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1822,24 +1811,24 @@
         <v>Mon</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="H10" s="39" t="s">
-        <v>116</v>
+      <c r="H10" s="66" t="s">
+        <v>140</v>
       </c>
       <c r="I10" s="66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J10" s="66" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1853,7 +1842,7 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
@@ -1867,10 +1856,10 @@
         <v>67</v>
       </c>
       <c r="J11" s="67" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="36">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1892,16 +1881,16 @@
         <v>106</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I12" s="39" t="s">
         <v>66</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="36">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1915,7 +1904,7 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
@@ -1932,7 +1921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="48">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1957,7 +1946,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="58"/>
       <c r="B15" s="59">
         <f t="shared" si="4"/>
@@ -1974,7 +1963,7 @@
       <c r="I15" s="61"/>
       <c r="J15" s="61"/>
     </row>
-    <row r="16" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -1999,10 +1988,10 @@
       </c>
       <c r="I16" s="39"/>
       <c r="J16" s="57" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="36">
         <f>A16+1</f>
         <v>15</v>
@@ -2016,7 +2005,7 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
@@ -2031,7 +2020,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="63" t="s">
         <v>3</v>
       </c>
@@ -2054,28 +2043,23 @@
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="58" orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="22.375" style="4"/>
+    <col min="1" max="16384" width="22.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2107,7 +2091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="189" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2138,7 +2122,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="6">
         <f>B2+2</f>
@@ -2168,7 +2152,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="11">
         <f>B3+2</f>
@@ -2194,7 +2178,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f>A2+1</f>
         <v>2</v>
@@ -2227,7 +2211,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="6">
         <f t="shared" si="1"/>
@@ -2255,7 +2239,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="11">
         <f t="shared" si="1"/>
@@ -2285,7 +2269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <f>A5+1</f>
         <v>3</v>
@@ -2310,7 +2294,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="6">
         <f t="shared" si="1"/>
@@ -2338,7 +2322,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="11">
         <f t="shared" si="1"/>
@@ -2368,7 +2352,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <f>A8+1</f>
         <v>4</v>
@@ -2401,7 +2385,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="6">
         <f>B9+7</f>
@@ -2429,7 +2413,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="11">
         <f>B10+7</f>
@@ -2453,7 +2437,7 @@
       </c>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <f>A11+1</f>
         <v>5</v>
@@ -2486,7 +2470,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="6">
         <f t="shared" si="1"/>
@@ -2512,7 +2496,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="11">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
add wk9 and 10, bivariate inference
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="146">
   <si>
     <t>date</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>Watch PDS video 14 (21 min)</t>
   </si>
   <si>
     <t>Regression Assigment (Due 11/17)</t>
@@ -381,37 +378,6 @@
     <t>[Week 5 ](wk05.html)</t>
   </si>
   <si>
-    <t>[Week 6 ](wk06.html)</t>
-  </si>
-  <si>
-    <t>[Week 7 ](wk07.html)</t>
-  </si>
-  <si>
-    <t>[Week 8 ](wk08.html)</t>
-  </si>
-  <si>
-    <t>[Week 9 ](wk09.html)</t>
-  </si>
-  <si>
-    <t>[Week 10 ](wk10.html)</t>
-  </si>
-  <si>
-    <t>[Week 11 ](wk11.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 12 ](wk12.html)
-</t>
-  </si>
-  <si>
-    <t>[Week 13 ](wk13.html)</t>
-  </si>
-  <si>
-    <t>[Week 14 ](wk14.html)</t>
-  </si>
-  <si>
-    <t>[Week 15 ](wk15.html)</t>
-  </si>
-  <si>
     <t>Foundations for Inference
 * Confidence Intervals
 * T Distribution
@@ -439,16 +405,7 @@
     <t>R for 1 sample inference - mean, prop. Ch 5</t>
   </si>
   <si>
-    <t>PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
-  </si>
-  <si>
     <t>Correlation &amp; Linear Regression</t>
-  </si>
-  <si>
-    <t>Multiple Regression
-* Confounding
-* Indicator Variables
-* _No Class Friday_</t>
   </si>
   <si>
     <t>Introduction to the class structure and logistics, Reproducible research, Data Analysis Life cycle, Add Health Data</t>
@@ -548,11 +505,6 @@
     </r>
   </si>
   <si>
-    <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
-* [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)
-* Course Notes  6.2-6.4</t>
-  </si>
-  <si>
     <t xml:space="preserve">PS 7.1, 7.3 (Due 10/29)
 * DC Correlation and Regression (Due 10/29)
 </t>
@@ -574,6 +526,85 @@
     <t>Moderation Assignment Due (11/5)
 * Poster Prep Stage III (Due 11/17)
 * Peer Review Stage III (Due 11/27 Before Class)</t>
+  </si>
+  <si>
+    <t>[Week 07: Oct 2](wk07.html)</t>
+  </si>
+  <si>
+    <t>[Week 08: Oct 9](wk08.html)</t>
+  </si>
+  <si>
+    <t>[Week 09: Oct 16](wk09.html)</t>
+  </si>
+  <si>
+    <t>[Week 10: Oct 23](wk10.html)</t>
+  </si>
+  <si>
+    <t>[Week 11: Oct 30](wk11.html)</t>
+  </si>
+  <si>
+    <t>[Week 12: Nov 6](wk12.html)</t>
+  </si>
+  <si>
+    <t>[Week 13: Nov 13](wk13.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 01: Aug 21](wk01.html) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 02: Aug 28](wk02.html)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 03: Sep 4](wk03.html)
+</t>
+  </si>
+  <si>
+    <t>[Week 04: Sep 11](wk04.html)</t>
+  </si>
+  <si>
+    <t>[Week 05: Sep 18](wk05.html)</t>
+  </si>
+  <si>
+    <t>[Week 06: Sep 25](wk06.html)</t>
+  </si>
+  <si>
+    <t>[Week 14: Nov 27](wk14.html)</t>
+  </si>
+  <si>
+    <t>[Week 15: Dec 6](wk15.html)</t>
+  </si>
+  <si>
+    <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
+* [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)
+* Course Notes  6.2-6.4
+* [Categorical Analysis](docs/lec04_cda.html) notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)
+</t>
+  </si>
+  <si>
+    <t>PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)
+* [Regression](docs/lec05_LinReg.html) notes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Multiple Regression
+* Confounding
+* Indicator Variables
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* _No Class Friday_</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -904,7 +935,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1107,6 +1138,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1528,7 +1568,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1605,7 @@
       <c r="F1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="70" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="28" t="s">
@@ -1590,19 +1630,19 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
-      <c r="G2" s="34" t="s">
-        <v>95</v>
+      <c r="G2" s="71" t="s">
+        <v>134</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1619,20 +1659,20 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
-      <c r="G3" s="39" t="s">
-        <v>96</v>
+      <c r="G3" s="72" t="s">
+        <v>135</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1646,12 +1686,12 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
-      <c r="G4" s="41" t="s">
-        <v>97</v>
+      <c r="G4" s="71" t="s">
+        <v>136</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
@@ -1671,19 +1711,19 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
-      <c r="G5" s="46" t="s">
-        <v>98</v>
+      <c r="G5" s="65" t="s">
+        <v>137</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1706,13 +1746,13 @@
         <v>2.4</v>
       </c>
       <c r="F6" s="40"/>
-      <c r="G6" s="39" t="s">
-        <v>99</v>
+      <c r="G6" s="65" t="s">
+        <v>138</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
@@ -1729,15 +1769,15 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="G7" s="53" t="s">
-        <v>100</v>
+      <c r="G7" s="65" t="s">
+        <v>139</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
@@ -1754,23 +1794,23 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F8" s="40"/>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="39" t="s">
-        <v>112</v>
-      </c>
       <c r="I8" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1787,24 +1827,24 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F9" s="40"/>
-      <c r="G9" s="39" t="s">
-        <v>102</v>
+      <c r="G9" s="65" t="s">
+        <v>128</v>
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1818,24 +1858,24 @@
         <v>Mon</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
-      <c r="G10" s="39" t="s">
-        <v>103</v>
+      <c r="G10" s="65" t="s">
+        <v>129</v>
       </c>
       <c r="H10" s="65" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="I10" s="65" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="J10" s="65" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1849,24 +1889,24 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
-      <c r="G11" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>36</v>
+      <c r="G11" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>144</v>
       </c>
       <c r="I11" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="67" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1880,21 +1920,21 @@
         <v>Mon</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
-      <c r="G12" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>115</v>
+      <c r="G12" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>143</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -1910,25 +1950,25 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D13" s="39" t="s">
-        <v>117</v>
+      <c r="D13" s="68" t="s">
+        <v>145</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
-      <c r="G13" s="39" t="s">
-        <v>106</v>
+      <c r="G13" s="65" t="s">
+        <v>132</v>
       </c>
       <c r="H13" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1946,11 +1986,11 @@
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
-      <c r="G14" s="53" t="s">
-        <v>107</v>
+      <c r="G14" s="65" t="s">
+        <v>133</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1983,19 +2023,19 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="68" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="39" t="s">
-        <v>108</v>
+      <c r="G16" s="65" t="s">
+        <v>140</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" s="39"/>
       <c r="J16" s="66" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2012,19 +2052,19 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="68" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
-      <c r="G17" s="39" t="s">
-        <v>109</v>
+      <c r="G17" s="65" t="s">
+        <v>141</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2036,20 +2076,21 @@
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
+      <c r="G18" s="39"/>
       <c r="I18" s="53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" orientation="landscape"/>
+  <pageSetup scale="58" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2117,16 +2158,16 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -2140,23 +2181,23 @@
         <v>Wed</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2170,19 +2211,19 @@
         <v>Fri</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
@@ -2206,16 +2247,16 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -2237,13 +2278,13 @@
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>72</v>
-      </c>
       <c r="J6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2263,17 +2304,17 @@
         <v>18</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2290,12 +2331,12 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -2320,13 +2361,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -2350,13 +2391,13 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -2373,23 +2414,23 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2411,13 +2452,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2431,16 +2472,16 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2465,16 +2506,16 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>34</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2492,7 +2533,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2500,7 +2541,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2514,16 +2555,16 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" s="25"/>
     </row>

</xml_diff>

<commit_message>
add wk10, moderation assignment for wk11
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1577,7 +1577,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1946,7 +1946,7 @@
       <c r="I12" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="66" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       <c r="I13" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="67" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dm add health add moderation assignment to schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -546,11 +546,6 @@
   <si>
     <t>Presentations (MW)
 * What's next? (F)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderation Assignment Due (11/5)
-* Regression/Confounding Assigment (Due 11/17)
-</t>
   </si>
   <si>
     <t>Poster Prep Stage III (Due 11/17)
@@ -622,11 +617,16 @@
   <si>
     <t>RAT: Linear Regression (7-7.2) Wednesday!</t>
   </si>
+  <si>
+    <t xml:space="preserve">[Moderation Assignment](hw/Moderation.html) Due (11/5)
+* Regression/Confounding Assigment (Due 11/17)
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1235,8 +1235,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1572,12 +1572,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1881,7 +1881,7 @@
         <v>112</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1908,13 +1908,13 @@
         <v>118</v>
       </c>
       <c r="H11" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="I11" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="66" t="s">
         <v>140</v>
-      </c>
-      <c r="I11" s="67" t="s">
-        <v>148</v>
-      </c>
-      <c r="J11" s="66" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>60</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1964,7 +1964,7 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="72"/>
       <c r="F13" s="40"/>
@@ -1972,13 +1972,13 @@
         <v>120</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J13" s="67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1995,7 +1995,7 @@
         <v>Mon</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
@@ -2003,10 +2003,10 @@
         <v>121</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J14" s="8"/>
     </row>
@@ -2112,7 +2112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
adjustments, add faq, links to moderation and regression assignments
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="147">
   <si>
     <t>date</t>
   </si>
@@ -187,10 +187,6 @@
   </si>
   <si>
     <t>Kristel week 5</t>
-  </si>
-  <si>
-    <t>Watch Video on [Preparing your final project](https://www.youtube.com/watch?v=NjPWVbXdRuo&amp;list=PLDEF0B9CBD27AD37E&amp;index=49) (13 min)
-* Read PDS Chapter 18</t>
   </si>
   <si>
     <t>Finish remaining assignments</t>
@@ -468,9 +464,6 @@
 </t>
   </si>
   <si>
-    <t>Poster building</t>
-  </si>
-  <si>
     <t>[Week 07: Oct 2](wk07.html)</t>
   </si>
   <si>
@@ -530,43 +523,12 @@
     <t>Friday free work day</t>
   </si>
   <si>
-    <t>Moderation
-* Confounding 
-* Multiple Regression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)
-* [PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
-</t>
-  </si>
-  <si>
     <t>Correlation
 * Linear Regression</t>
   </si>
   <si>
     <t>Presentations (MW)
 * What's next? (F)</t>
-  </si>
-  <si>
-    <t>Poster Prep Stage III (Due 11/17)
-* Peer Review Stage III (Due 11/27 Before Class)</t>
-  </si>
-  <si>
-    <r>
-      <t>[Bivariate Inference Assignment](hw/Bivariate_Inference.html)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Due 10/29)
-* PS 6.6  (Due 10/22)
-</t>
-    </r>
   </si>
   <si>
     <t>PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)
@@ -597,36 +559,103 @@
     </r>
   </si>
   <si>
-    <t>CN 8.2
-* Logistic Regression Notes [[TBD]]</t>
-  </si>
-  <si>
-    <t>CN Ch 8.2
+    <t>RAT: Linear Regression (7-7.2) Wednesday!</t>
+  </si>
+  <si>
+    <t>Poster building (MW)
+* Study Design (F)</t>
+  </si>
+  <si>
+    <t>[Poster Prep Stage III]((https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 11/17)
+* Peer Review Stage III (Due 11/27 Before Class)</t>
+  </si>
+  <si>
+    <t>[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)
+* [PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
+* CN / OI Ch 8</t>
+  </si>
+  <si>
+    <t>Logistic Regression Notes [[TBD]]
+* CN / OI Chapter 8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Watch Video on [Preparing your final project](https://www.youtube.com/watch?v=NjPWVbXdRuo&amp;list=PLDEF0B9CBD27AD37E&amp;index=49) (13 min)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Read PDS Chapter 18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 * Chapter 1: Data Collection</t>
-  </si>
-  <si>
-    <t>Model Building / Model Fit
-* Study Design</t>
-  </si>
-  <si>
-    <t>RAT: Study Design</t>
-  </si>
-  <si>
-    <t>RAT: Logstic Regression</t>
-  </si>
-  <si>
-    <t>RAT: Linear Regression (7-7.2) Wednesday!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Moderation Assignment](hw/Moderation.html) Due (11/5)
-* Regression/Confounding Assigment (Due 11/17)
+    </r>
+  </si>
+  <si>
+    <t>RAT (F): Study Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_Inference.html) (Due 10/29)
+* [[Completed Bivariate Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPWGQxU1FsNm1DcG8?usp=sharing)
+* PS 6.6  (Due 10/22)
 </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Moderation Assignment](hw/Moderation.html) Due (11/5)
+* [[Completed Moderation Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPU3dsamgwOWVHVzg?usp=sharing)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* [Regression/Confounding Assigment](hw/Regression.html) (Due 11/17)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+* [[Completed Regression Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPcFBabzNpNHFOdFU?usp=sharing)</t>
+    </r>
+  </si>
+  <si>
+    <t>RAT: Multiple Regression &amp; Indicator Variables</t>
+  </si>
+  <si>
+    <t>Moderation (M)
+* Confounding (W)
+* Multiple Regression (W)
+* Model building, model fit (F(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1235,8 +1264,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1572,7 +1601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
@@ -1639,19 +1668,19 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
       <c r="G2" s="70" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1668,17 +1697,17 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="71" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1695,12 +1724,12 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
       <c r="G4" s="70" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
@@ -1720,19 +1749,19 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="64" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1756,12 +1785,12 @@
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
@@ -1778,15 +1807,15 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
@@ -1803,23 +1832,23 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>92</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>93</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="64" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H8" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="39" t="s">
         <v>94</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1836,21 +1865,21 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1867,21 +1896,21 @@
         <v>Mon</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="64" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H10" s="64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1898,26 +1927,26 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="67" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="64" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I11" s="67" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1931,26 +1960,26 @@
         <v>Mon</v>
       </c>
       <c r="D12" s="67" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1964,21 +1993,21 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E13" s="72"/>
       <c r="F13" s="40"/>
       <c r="G13" s="64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>146</v>
-      </c>
-      <c r="J13" s="67" t="s">
-        <v>137</v>
+        <v>145</v>
+      </c>
+      <c r="J13" s="65" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1994,20 +2023,14 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>144</v>
-      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>145</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2027,7 +2050,7 @@
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
     </row>
-    <row r="16" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -2040,19 +2063,21 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
       <c r="G16" s="64" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="39"/>
+        <v>126</v>
+      </c>
+      <c r="H16" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="67" t="s">
+        <v>142</v>
+      </c>
       <c r="J16" s="65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2069,19 +2094,19 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="67" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2093,16 +2118,16 @@
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
       <c r="G18" s="39"/>
       <c r="I18" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2112,7 +2137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2175,16 +2200,16 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>45</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -2234,7 +2259,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>43</v>
@@ -2264,16 +2289,16 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -2295,10 +2320,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>46</v>
@@ -2321,17 +2346,17 @@
         <v>18</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2348,12 +2373,12 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -2378,13 +2403,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -2408,13 +2433,13 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -2431,20 +2456,20 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>36</v>
@@ -2469,13 +2494,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2489,7 +2514,7 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>47</v>
@@ -2498,7 +2523,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2523,10 +2548,10 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>34</v>
@@ -2550,7 +2575,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2558,7 +2583,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2572,16 +2597,16 @@
         <v>Fri</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J16" s="25"/>
     </row>

</xml_diff>

<commit_message>
update wk 11, add wk12, update schedule
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -235,9 +235,6 @@
     <t>RAT: CN 4.1-4.4</t>
   </si>
   <si>
-    <t>RAT: Moderation</t>
-  </si>
-  <si>
     <t>Build your own exam questions (Due 12/6)</t>
   </si>
   <si>
@@ -542,8 +539,34 @@
 * Peer Review Stage II (Due 11/1)</t>
   </si>
   <si>
+    <t>RAT: Linear Regression (7-7.2) Wednesday!</t>
+  </si>
+  <si>
+    <t>[Poster Prep Stage III]((https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 11/17)
+* Peer Review Stage III (Due 11/27 Before Class)</t>
+  </si>
+  <si>
+    <t>Logistic Regression Notes [[TBD]]
+* CN / OI Chapter 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_Inference.html) (Due 10/29)
+* [[Completed Bivariate Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPWGQxU1FsNm1DcG8?usp=sharing)
+* PS 6.6  (Due 10/22)
+</t>
+  </si>
+  <si>
+    <t>RAT: Multiple Regression &amp; Indicator Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderation (M)
+* Study Design (W)
+* Multiple Regression (F)
+</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Indicator Variables
+      <t xml:space="preserve">Categorical Predictors
 * Logistic Regression
 </t>
     </r>
@@ -557,26 +580,6 @@
       </rPr>
       <t>* _No Class Friday_</t>
     </r>
-  </si>
-  <si>
-    <t>RAT: Linear Regression (7-7.2) Wednesday!</t>
-  </si>
-  <si>
-    <t>Poster building (MW)
-* Study Design (F)</t>
-  </si>
-  <si>
-    <t>[Poster Prep Stage III]((https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 11/17)
-* Peer Review Stage III (Due 11/27 Before Class)</t>
-  </si>
-  <si>
-    <t>[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)
-* [PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
-* CN / OI Ch 8</t>
-  </si>
-  <si>
-    <t>Logistic Regression Notes [[TBD]]
-* CN / OI Chapter 8</t>
   </si>
   <si>
     <r>
@@ -603,22 +606,26 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-* Chapter 1: Data Collection</t>
+</t>
     </r>
   </si>
   <si>
-    <t>RAT (F): Study Design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_Inference.html) (Due 10/29)
-* [[Completed Bivariate Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPWGQxU1FsNm1DcG8?usp=sharing)
-* PS 6.6  (Due 10/22)
-</t>
+    <t>[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)
+* CN Chapter 1: Data Collection
+* [PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
+* CN / OI Ch 8</t>
+  </si>
+  <si>
+    <t>RAT: Study Design (W)</t>
+  </si>
+  <si>
+    <t>* Model Building (M)
+* Flex lecture time (W)
+* Open work time (F)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">[Moderation Assignment](hw/Moderation.html) Due (11/5)
-* [[Completed Moderation Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPU3dsamgwOWVHVzg?usp=sharing)
+      <t xml:space="preserve">[Moderation Assignment](hw/Moderation.html) (Due 11/5)
 </t>
     </r>
     <r>
@@ -629,7 +636,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* [Regression/Confounding Assigment](hw/Regression.html) (Due 11/17)</t>
+      <t>* [Regression Assigment](hw/Regression.html) (Due 11/17)</t>
     </r>
     <r>
       <rPr>
@@ -639,23 +646,17 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-* [[Completed Regression Assignments]](https://drive.google.com/drive/folders/0B83Z8_sNw3KPcFBabzNpNHFOdFU?usp=sharing)</t>
+</t>
     </r>
   </si>
   <si>
-    <t>RAT: Multiple Regression &amp; Indicator Variables</t>
-  </si>
-  <si>
-    <t>Moderation (M)
-* Confounding (W)
-* Multiple Regression (W)
-* Model building, model fit (F(</t>
+    <t>Poster building</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1264,8 +1265,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1601,12 +1602,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1668,19 +1669,19 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
       <c r="G2" s="70" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1697,17 +1698,17 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1724,12 +1725,12 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
       <c r="G4" s="70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
@@ -1749,19 +1750,19 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1785,12 +1786,12 @@
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
@@ -1807,15 +1808,15 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
@@ -1832,23 +1833,23 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>91</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>92</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I8" s="39" t="s">
         <v>58</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1865,21 +1866,21 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1896,21 +1897,21 @@
         <v>Mon</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H10" s="64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I10" s="64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J10" s="64" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1927,26 +1928,26 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="I11" s="67" t="s">
-        <v>136</v>
-      </c>
-      <c r="J11" s="66" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1960,23 +1961,23 @@
         <v>Mon</v>
       </c>
       <c r="D12" s="67" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="40"/>
       <c r="G12" s="64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>59</v>
+        <v>142</v>
+      </c>
+      <c r="I12" s="67" t="s">
+        <v>143</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -1993,24 +1994,24 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E13" s="72"/>
       <c r="F13" s="40"/>
       <c r="G13" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I13" s="67" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2023,11 +2024,13 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -2063,21 +2066,19 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
       <c r="G16" s="64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H16" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="67" t="s">
-        <v>142</v>
-      </c>
+      <c r="I16" s="67"/>
       <c r="J16" s="65" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2094,19 +2095,19 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2127,7 +2128,7 @@
         <v>52</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2137,7 +2138,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2200,7 +2201,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>55</v>
@@ -2259,7 +2260,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>43</v>
@@ -2289,10 +2290,10 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>57</v>
@@ -2320,10 +2321,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>46</v>
@@ -2350,13 +2351,13 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2373,12 +2374,12 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -2403,13 +2404,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -2433,13 +2434,13 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -2456,20 +2457,20 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>36</v>
@@ -2494,13 +2495,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2514,7 +2515,7 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>47</v>
@@ -2523,7 +2524,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2548,7 +2549,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>50</v>
@@ -2575,7 +2576,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2583,7 +2584,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2601,7 +2602,7 @@
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>

</xml_diff>

<commit_message>
add temp reg assignment
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH315\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH315/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -598,7 +598,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -618,6 +617,13 @@
     <t>* Model Building (M)
 * Flex lecture time (W)
 * Open work time (F)</t>
+  </si>
+  <si>
+    <t>Poster building</t>
+  </si>
+  <si>
+    <t>[Poster Prep Stage III](https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 11/17)
+* Peer Review Stage III (Due 11/27 Before Class)</t>
   </si>
   <si>
     <r>
@@ -632,7 +638,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* [Regression Assigment](hw/Regression.html) (Due 11/17)</t>
+      <t>* [Regression Assigment](hw/Regression_Assignment.html) (Due 11/17)</t>
     </r>
     <r>
       <rPr>
@@ -645,18 +651,11 @@
 </t>
     </r>
   </si>
-  <si>
-    <t>Poster building</t>
-  </si>
-  <si>
-    <t>[Poster Prep Stage III](https://norcalbiostat.github.io/MATH315/project.html#poster_preparation) (Due 11/17)
-* Peer Review Stage III (Due 11/27 Before Class)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1610,22 +1609,22 @@
       <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.375" style="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" style="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="53" customWidth="1"/>
-    <col min="5" max="5" width="19.875" style="63" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="63" customWidth="1"/>
-    <col min="7" max="7" width="20.125" style="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.625" style="53" customWidth="1"/>
-    <col min="9" max="9" width="31.125" style="53" customWidth="1"/>
-    <col min="10" max="10" width="53.625" style="53" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="30"/>
+    <col min="5" max="5" width="19.83203125" style="63" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="63" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.6640625" style="53" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" style="53" customWidth="1"/>
+    <col min="10" max="10" width="53.6640625" style="53" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>6</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="31">
         <v>1</v>
       </c>
@@ -1684,7 +1683,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="36">
         <f t="shared" ref="A3:A8" si="1">A2+1</f>
         <v>2</v>
@@ -1711,7 +1710,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="36">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1736,7 +1735,7 @@
       <c r="I4" s="39"/>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A5" s="43">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1765,7 +1764,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="36">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1794,7 +1793,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A7" s="48">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1819,7 +1818,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A8" s="36">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1852,7 +1851,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
         <f t="shared" ref="A9:A14" si="3">A8+1</f>
         <v>8</v>
@@ -1883,7 +1882,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1914,7 +1913,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1947,7 +1946,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" s="36">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1977,10 +1976,10 @@
         <v>142</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="36">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -2008,10 +2007,10 @@
         <v>137</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="48">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2036,7 +2035,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="56"/>
       <c r="B15" s="57">
         <f t="shared" si="4"/>
@@ -2053,7 +2052,7 @@
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
     </row>
-    <row r="16" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="40"/>
@@ -2081,7 +2080,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="36">
         <f>A16+1</f>
         <v>15</v>
@@ -2110,7 +2109,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="61" t="s">
         <v>3</v>
       </c>
@@ -2145,12 +2144,12 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="22.375" style="4"/>
+    <col min="1" max="16384" width="22.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="189" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2213,7 +2212,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="6">
         <f>B2+2</f>
@@ -2243,7 +2242,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="11">
         <f>B3+2</f>
@@ -2269,7 +2268,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f>A2+1</f>
         <v>2</v>
@@ -2302,7 +2301,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="6">
         <f t="shared" si="1"/>
@@ -2330,7 +2329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="11">
         <f t="shared" si="1"/>
@@ -2360,7 +2359,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <f>A5+1</f>
         <v>3</v>
@@ -2385,7 +2384,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="6">
         <f t="shared" si="1"/>
@@ -2413,7 +2412,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="11">
         <f t="shared" si="1"/>
@@ -2443,7 +2442,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <f>A8+1</f>
         <v>4</v>
@@ -2476,7 +2475,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="6">
         <f>B9+7</f>
@@ -2504,7 +2503,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="11">
         <f>B10+7</f>
@@ -2528,7 +2527,7 @@
       </c>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <f>A11+1</f>
         <v>5</v>
@@ -2561,7 +2560,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="6">
         <f t="shared" si="1"/>
@@ -2587,7 +2586,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="11">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
add var select notes
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="150">
   <si>
     <t>date</t>
   </si>
@@ -623,6 +623,11 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>Open Intro Section 8.2, 8.4
+* Logistic Regression [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)
+* Variable Selection [[HTML]](docs/lec09_VarSelect.html) [[PDF]](docs/lec09_VarSelect.pdf)</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1584,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1979,7 +1984,7 @@
       <c r="I13" s="66"/>
       <c r="J13" s="65"/>
     </row>
-    <row r="14" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -2000,7 +2005,9 @@
       <c r="G14" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="I14" s="66" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
update project page with buttons
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -493,12 +493,6 @@
     <t>[Week 06: Sep 25](wk06.html)</t>
   </si>
   <si>
-    <t>[Week 14: Nov 27](wk14.html)</t>
-  </si>
-  <si>
-    <t>[Week 15: Dec 6](wk15.html)</t>
-  </si>
-  <si>
     <t>[PDS video 11](http://passiondrivenstatistics.com/2016/05/11/r-chapter-11/) (30 min)
 * [PDS video 12](http://passiondrivenstatistics.com/2016/06/29/r-chapter-12/) (28 min)
 * Course Notes  6.2-6.4
@@ -603,31 +597,26 @@
     <t>Common Final Exam (Both classes same time)</t>
   </si>
   <si>
-    <t xml:space="preserve">Poster Draft (Due 11/29)
-* Peer Review Poster Draft (Due 12/1)
-* Final version of poster (Due 12/4, or 12/6)
-</t>
-  </si>
-  <si>
-    <r>
-      <t>Watch Video on [Preparing your final project](https://www.youtube.com/watch?v=NjPWVbXdRuo&amp;list=PLDEF0B9CBD27AD37E&amp;index=49) (13 min)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>Open Intro Section 8.2, 8.4
 * Logistic Regression [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)
 * Variable Selection [[HTML]](docs/lec09_VarSelect.html) [[PDF]](docs/lec09_VarSelect.pdf)</t>
+  </si>
+  <si>
+    <t>[Week 14: Nov 27](index.html)</t>
+  </si>
+  <si>
+    <t>[Week 15: Dec 6](index.html)</t>
+  </si>
+  <si>
+    <t>[Poster Guidelines](https://norcalbiostat.netlify.com/lec/poster_guidelines/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poster Draft (Due 11/29)
+* Peer Review Poster Draft (Due 12/1)
+* Final version of poster (Due 12/3)
+* Final poster scoring (Due 12/8)
+* Team evaluation (Due 12/8)
+</t>
   </si>
 </sst>
 </file>
@@ -823,7 +812,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -871,6 +860,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1138,9 +1136,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1163,6 +1158,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1584,7 +1582,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1621,7 +1619,7 @@
       <c r="F1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="67" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="28" t="s">
@@ -1652,7 +1650,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
-      <c r="G2" s="69" t="s">
+      <c r="G2" s="68" t="s">
         <v>117</v>
       </c>
       <c r="H2" s="34"/>
@@ -1679,7 +1677,7 @@
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="69" t="s">
         <v>118</v>
       </c>
       <c r="H3" s="39"/>
@@ -1706,7 +1704,7 @@
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
-      <c r="G4" s="69" t="s">
+      <c r="G4" s="68" t="s">
         <v>119</v>
       </c>
       <c r="H4" s="39"/>
@@ -1882,13 +1880,13 @@
         <v>112</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I10" s="63" t="s">
         <v>109</v>
       </c>
       <c r="J10" s="63" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1904,22 +1902,22 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D11" s="66" t="s">
-        <v>128</v>
-      </c>
-      <c r="E11" s="71" t="s">
-        <v>127</v>
+      <c r="D11" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="70" t="s">
+        <v>125</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="H11" s="66" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11" s="66"/>
-      <c r="J11" s="65" t="s">
-        <v>131</v>
+      <c r="H11" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="65"/>
+      <c r="J11" s="64" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1935,26 +1933,26 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D12" s="66" t="s">
-        <v>133</v>
-      </c>
-      <c r="E12" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="F12" s="71" t="s">
-        <v>143</v>
+      <c r="D12" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>141</v>
       </c>
       <c r="G12" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="66" t="s">
-        <v>134</v>
-      </c>
-      <c r="I12" s="66" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="65" t="s">
-        <v>141</v>
+      <c r="H12" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="J12" s="64" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1970,19 +1968,19 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D13" s="66" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="71"/>
+      <c r="D13" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="70"/>
       <c r="F13" s="40"/>
       <c r="G13" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="I13" s="66"/>
-      <c r="J13" s="65"/>
+      <c r="H13" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" s="65"/>
+      <c r="J13" s="64"/>
     </row>
     <row r="14" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="48">
@@ -1998,7 +1996,7 @@
         <v>Mon</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
@@ -2006,13 +2004,13 @@
         <v>116</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I14" s="66" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="I14" s="65" t="s">
+        <v>140</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2032,7 +2030,7 @@
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
     </row>
-    <row r="16" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -2044,22 +2042,22 @@
         <f t="shared" ref="C16:C17" si="5">TEXT(WEEKDAY(B16,1)+1, "ddd")</f>
         <v>Mon</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="70" t="s">
         <v>136</v>
-      </c>
-      <c r="E16" s="71" t="s">
-        <v>138</v>
       </c>
       <c r="F16" s="40"/>
       <c r="G16" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="66" t="s">
+        <v>146</v>
+      </c>
+      <c r="H16" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="I16" s="66"/>
+      <c r="I16" s="65"/>
       <c r="J16" s="64" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2075,19 +2073,19 @@
         <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
-      <c r="D17" s="66" t="s">
-        <v>129</v>
+      <c r="D17" s="65" t="s">
+        <v>127</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="63" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
-      <c r="J17" s="67" t="s">
+      <c r="J17" s="66" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2099,14 +2097,14 @@
         <v>41621</v>
       </c>
       <c r="C18" s="50"/>
-      <c r="D18" s="72" t="s">
-        <v>146</v>
+      <c r="D18" s="71" t="s">
+        <v>144</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
-      <c r="G18" s="39"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
add poster drafts for review
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="151">
   <si>
     <t>date</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>RAT: CN 4.1-4.4</t>
-  </si>
-  <si>
-    <t>Build your own exam questions (Due 12/6)</t>
   </si>
   <si>
     <t>Post assessment in R 
@@ -507,10 +504,6 @@
   <si>
     <t>Correlation
 * Linear Regression</t>
-  </si>
-  <si>
-    <t>Presentations (MW)
-* What's next? (F)</t>
   </si>
   <si>
     <t>PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)
@@ -617,6 +610,17 @@
 * Final poster scoring (Due 12/8)
 * Team evaluation (Due 12/8)
 </t>
+  </si>
+  <si>
+    <t>Presentations (MW)
+* Exam review (F)</t>
+  </si>
+  <si>
+    <t>Print posters before class on Monday. 
+* Review Practice Exam</t>
+  </si>
+  <si>
+    <t>Build your own exam questions (Due 12/6)</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
@@ -1644,19 +1648,19 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
       <c r="G2" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1673,17 +1677,17 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="69" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1700,12 +1704,12 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
       <c r="G4" s="68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
@@ -1725,19 +1729,19 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1761,12 +1765,12 @@
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
@@ -1783,15 +1787,15 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
@@ -1808,23 +1812,23 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>89</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>90</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8" s="39" t="s">
         <v>57</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1841,21 +1845,21 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1872,21 +1876,21 @@
         <v>Mon</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I10" s="63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J10" s="63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1903,21 +1907,21 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H11" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I11" s="65"/>
       <c r="J11" s="64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1934,25 +1938,25 @@
         <v>Mon</v>
       </c>
       <c r="D12" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="65" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="70" t="s">
-        <v>124</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>141</v>
-      </c>
-      <c r="G12" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="65" t="s">
-        <v>133</v>
-      </c>
       <c r="J12" s="64" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1969,15 +1973,15 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" s="70"/>
       <c r="F13" s="40"/>
       <c r="G13" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="65" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I13" s="65"/>
       <c r="J13" s="64"/>
@@ -1996,21 +2000,21 @@
         <v>Mon</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I14" s="65" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2043,21 +2047,21 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="70" t="s">
         <v>134</v>
-      </c>
-      <c r="E16" s="70" t="s">
-        <v>136</v>
       </c>
       <c r="F16" s="40"/>
       <c r="G16" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="H16" s="65" t="s">
         <v>146</v>
-      </c>
-      <c r="H16" s="65" t="s">
-        <v>148</v>
       </c>
       <c r="I16" s="65"/>
       <c r="J16" s="64" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2074,19 +2078,21 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="H17" s="39"/>
+        <v>145</v>
+      </c>
+      <c r="H17" s="65" t="s">
+        <v>149</v>
+      </c>
       <c r="I17" s="39"/>
       <c r="J17" s="66" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2098,19 +2104,19 @@
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
       <c r="G18" s="72"/>
       <c r="H18" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>51</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2189,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>54</v>
@@ -2242,7 +2248,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>43</v>
@@ -2272,10 +2278,10 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>56</v>
@@ -2303,10 +2309,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>46</v>
@@ -2333,13 +2339,13 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2356,12 +2362,12 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -2386,13 +2392,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -2416,13 +2422,13 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -2439,20 +2445,20 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>36</v>
@@ -2477,13 +2483,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2497,7 +2503,7 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>47</v>
@@ -2506,7 +2512,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2531,7 +2537,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>50</v>
@@ -2558,7 +2564,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2566,7 +2572,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2584,7 +2590,7 @@
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>

</xml_diff>

<commit_message>
finish roll your own. update schedule and index. add citations for addhealth and R
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -604,23 +604,23 @@
     <t>[Poster Guidelines](https://norcalbiostat.netlify.com/lec/poster_guidelines/)</t>
   </si>
   <si>
+    <t>Presentations (MW)
+* Exam review (F)</t>
+  </si>
+  <si>
+    <t>Print posters before class on Monday. 
+* Review Practice Exam</t>
+  </si>
+  <si>
+    <t>[Build your own exam questions](hw/roll_your_own.html) (Due 12/6)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poster Draft (Due 11/29)
 * Peer Review Poster Draft (Due 12/1)
-* Final version of poster (Due 12/3)
-* Final poster scoring (Due 12/8)
-* Team evaluation (Due 12/8)
+* [Final version of poster](https://www.dropbox.com/request/NtC88NHRbo5oIyRcSxoD) (Due 12/3)
+* [Final poster scoring](https://goo.gl/forms/QORgO0jjqNzp3T5i2) (Due 12/8)
+* [Team evaluation](https://goo.gl/forms/o7XsKk4C491jBuXk1) (Due 12/8)
 </t>
-  </si>
-  <si>
-    <t>Presentations (MW)
-* Exam review (F)</t>
-  </si>
-  <si>
-    <t>Print posters before class on Monday. 
-* Review Practice Exam</t>
-  </si>
-  <si>
-    <t>Build your own exam questions (Due 12/6)</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1146,25 +1145,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1586,7 +1585,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J17:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1622,7 @@
       <c r="F1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="66" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="28" t="s">
@@ -1654,7 +1653,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="67" t="s">
         <v>116</v>
       </c>
       <c r="H2" s="34"/>
@@ -1681,7 +1680,7 @@
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="68" t="s">
         <v>117</v>
       </c>
       <c r="H3" s="39"/>
@@ -1708,7 +1707,7 @@
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="67" t="s">
         <v>118</v>
       </c>
       <c r="H4" s="39"/>
@@ -1909,7 +1908,7 @@
       <c r="D11" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="69" t="s">
         <v>124</v>
       </c>
       <c r="F11" s="40"/>
@@ -1940,10 +1939,10 @@
       <c r="D12" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="69" t="s">
         <v>139</v>
       </c>
       <c r="G12" s="63" t="s">
@@ -1975,7 +1974,7 @@
       <c r="D13" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="70"/>
+      <c r="E13" s="69"/>
       <c r="F13" s="40"/>
       <c r="G13" s="63" t="s">
         <v>114</v>
@@ -2034,7 +2033,7 @@
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
     </row>
-    <row r="16" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>14</v>
       </c>
@@ -2049,7 +2048,7 @@
       <c r="D16" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="69" t="s">
         <v>134</v>
       </c>
       <c r="F16" s="40"/>
@@ -2061,7 +2060,7 @@
       </c>
       <c r="I16" s="65"/>
       <c r="J16" s="64" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2078,7 +2077,7 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
@@ -2088,11 +2087,11 @@
         <v>145</v>
       </c>
       <c r="H17" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="I17" s="39"/>
+      <c r="J17" s="72" t="s">
         <v>149</v>
-      </c>
-      <c r="I17" s="39"/>
-      <c r="J17" s="66" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2103,12 +2102,12 @@
         <v>41621</v>
       </c>
       <c r="C18" s="50"/>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="70" t="s">
         <v>142</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
-      <c r="G18" s="72"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="8" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
added links for assessments
</commit_message>
<xml_diff>
--- a/schedule_315.xlsx
+++ b/schedule_315.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="3" r:id="rId1"/>
     <sheet name="daily historical" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -230,10 +230,6 @@
   </si>
   <si>
     <t>RAT: CN 4.1-4.4</t>
-  </si>
-  <si>
-    <t>Post assessment in R 
-* Post Metacognition Assessment</t>
   </si>
   <si>
     <t xml:space="preserve">Download the AddHealth data into your projects folder. 
@@ -622,11 +618,15 @@
 * [Team evaluation](https://goo.gl/forms/o7XsKk4C491jBuXk1) (Due 12/8)
 </t>
   </si>
+  <si>
+    <t>[Post assessment in R](https://goo.gl/forms/NBn1ESRVQzIjo0Zl1)
+* [Post Metacognition Assessment](https://goo.gl/forms/Wj8QRRasC7u6Guir2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1243,8 +1243,8 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1580,12 +1580,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J17:J18"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J21:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1647,19 +1647,19 @@
         <v>Mon</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="35"/>
       <c r="G2" s="67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1676,17 +1676,17 @@
         <v>Mon</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1703,12 +1703,12 @@
         <v>Mon</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="42"/>
       <c r="G4" s="67" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
@@ -1728,19 +1728,19 @@
         <v>Mon</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47"/>
       <c r="G5" s="63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I5" s="46"/>
       <c r="J5" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1764,12 +1764,12 @@
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
       <c r="J6" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
@@ -1786,15 +1786,15 @@
         <v>Mon</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="189" x14ac:dyDescent="0.25">
@@ -1811,23 +1811,23 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>88</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>89</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="39" t="s">
         <v>57</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1844,21 +1844,21 @@
         <v>Mon</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J9" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1875,21 +1875,21 @@
         <v>Mon</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40"/>
       <c r="G10" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I10" s="63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J10" s="63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
@@ -1906,21 +1906,21 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E11" s="69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I11" s="65"/>
       <c r="J11" s="64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -1937,25 +1937,25 @@
         <v>Mon</v>
       </c>
       <c r="D12" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="69" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="G12" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="65" t="s">
+      <c r="I12" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="I12" s="65" t="s">
-        <v>131</v>
-      </c>
       <c r="J12" s="64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1972,15 +1972,15 @@
         <v>Mon</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="69"/>
       <c r="F13" s="40"/>
       <c r="G13" s="63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H13" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I13" s="65"/>
       <c r="J13" s="64"/>
@@ -1999,21 +1999,21 @@
         <v>Mon</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="52"/>
       <c r="F14" s="52"/>
       <c r="G14" s="63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I14" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2046,21 +2046,21 @@
         <v>Mon</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" s="69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F16" s="40"/>
       <c r="G16" s="63" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I16" s="65"/>
       <c r="J16" s="64" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2077,24 +2077,24 @@
         <v>Mon</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H17" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I17" s="39"/>
       <c r="J17" s="72" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
         <v>3</v>
       </c>
@@ -2103,19 +2103,19 @@
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" s="52"/>
       <c r="F18" s="52"/>
       <c r="G18" s="71"/>
       <c r="H18" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="J18" s="53" t="s">
-        <v>58</v>
+      <c r="J18" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>54</v>
@@ -2247,7 +2247,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>43</v>
@@ -2277,10 +2277,10 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>56</v>
@@ -2308,10 +2308,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>46</v>
@@ -2338,13 +2338,13 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2361,12 +2361,12 @@
         <v>Mon</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
@@ -2391,13 +2391,13 @@
       <c r="F9" s="9"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
@@ -2421,13 +2421,13 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.25">
@@ -2444,20 +2444,20 @@
         <v>Mon</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>36</v>
@@ -2482,13 +2482,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
         <v>Fri</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>47</v>
@@ -2511,7 +2511,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>50</v>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
@@ -2571,7 +2571,7 @@
         <v>29</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>

</xml_diff>